<commit_message>
feat: some experiments failded!
</commit_message>
<xml_diff>
--- a/experiments/EnKF-DM/EnKF_DM.xlsx
+++ b/experiments/EnKF-DM/EnKF_DM.xlsx
@@ -506,7 +506,7 @@
         </is>
       </c>
       <c r="H2" t="n">
-        <v>70.75546097755432</v>
+        <v>77.78589487075806</v>
       </c>
     </row>
     <row r="3">
@@ -540,7 +540,7 @@
         </is>
       </c>
       <c r="H3" t="n">
-        <v>70.74167704582214</v>
+        <v>74.38535714149475</v>
       </c>
     </row>
     <row r="4">
@@ -574,7 +574,7 @@
         </is>
       </c>
       <c r="H4" t="n">
-        <v>70.17102479934692</v>
+        <v>71.93408989906311</v>
       </c>
     </row>
     <row r="5">
@@ -585,7 +585,7 @@
         <v>20</v>
       </c>
       <c r="C5" t="n">
-        <v>7.000000000000001</v>
+        <v>7</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
@@ -608,7 +608,7 @@
         </is>
       </c>
       <c r="H5" t="n">
-        <v>74.254399061203</v>
+        <v>75.30217671394348</v>
       </c>
     </row>
     <row r="6">
@@ -619,7 +619,7 @@
         <v>20</v>
       </c>
       <c r="C6" t="n">
-        <v>7.000000000000001</v>
+        <v>7</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
@@ -642,7 +642,7 @@
         </is>
       </c>
       <c r="H6" t="n">
-        <v>74.38867139816284</v>
+        <v>75.37547779083252</v>
       </c>
     </row>
     <row r="7">
@@ -653,7 +653,7 @@
         <v>20</v>
       </c>
       <c r="C7" t="n">
-        <v>7.000000000000001</v>
+        <v>7</v>
       </c>
       <c r="D7" t="inlineStr">
         <is>
@@ -676,7 +676,7 @@
         </is>
       </c>
       <c r="H7" t="n">
-        <v>74.6134831905365</v>
+        <v>74.52739834785461</v>
       </c>
     </row>
     <row r="8">
@@ -710,7 +710,7 @@
         </is>
       </c>
       <c r="H8" t="n">
-        <v>85.54149055480957</v>
+        <v>85.59782409667969</v>
       </c>
     </row>
     <row r="9">
@@ -744,7 +744,7 @@
         </is>
       </c>
       <c r="H9" t="n">
-        <v>85.36442947387695</v>
+        <v>84.92439103126526</v>
       </c>
     </row>
     <row r="10">
@@ -778,7 +778,7 @@
         </is>
       </c>
       <c r="H10" t="n">
-        <v>85.242671251297</v>
+        <v>84.96928477287292</v>
       </c>
     </row>
     <row r="11">
@@ -812,7 +812,7 @@
         </is>
       </c>
       <c r="H11" t="n">
-        <v>342.7151923179626</v>
+        <v>277.5933349132538</v>
       </c>
     </row>
     <row r="12">
@@ -846,7 +846,7 @@
         </is>
       </c>
       <c r="H12" t="n">
-        <v>338.5596952438354</v>
+        <v>340.7719860076904</v>
       </c>
     </row>
     <row r="13">
@@ -880,7 +880,7 @@
         </is>
       </c>
       <c r="H13" t="n">
-        <v>336.663430929184</v>
+        <v>323.6778903007507</v>
       </c>
     </row>
     <row r="14">
@@ -914,7 +914,7 @@
         </is>
       </c>
       <c r="H14" t="n">
-        <v>70.53723955154419</v>
+        <v>70.30623340606689</v>
       </c>
     </row>
     <row r="15">
@@ -948,7 +948,7 @@
         </is>
       </c>
       <c r="H15" t="n">
-        <v>70.34985494613647</v>
+        <v>69.56742978096008</v>
       </c>
     </row>
     <row r="16">
@@ -982,7 +982,7 @@
         </is>
       </c>
       <c r="H16" t="n">
-        <v>70.36283254623413</v>
+        <v>69.43870735168457</v>
       </c>
     </row>
     <row r="17">
@@ -993,7 +993,7 @@
         <v>40</v>
       </c>
       <c r="C17" t="n">
-        <v>7.000000000000001</v>
+        <v>7</v>
       </c>
       <c r="D17" t="inlineStr">
         <is>
@@ -1016,7 +1016,7 @@
         </is>
       </c>
       <c r="H17" t="n">
-        <v>74.55875134468079</v>
+        <v>73.55969309806824</v>
       </c>
     </row>
     <row r="18">
@@ -1027,7 +1027,7 @@
         <v>40</v>
       </c>
       <c r="C18" t="n">
-        <v>7.000000000000001</v>
+        <v>7</v>
       </c>
       <c r="D18" t="inlineStr">
         <is>
@@ -1050,7 +1050,7 @@
         </is>
       </c>
       <c r="H18" t="n">
-        <v>74.85596895217896</v>
+        <v>73.5262131690979</v>
       </c>
     </row>
     <row r="19">
@@ -1061,7 +1061,7 @@
         <v>40</v>
       </c>
       <c r="C19" t="n">
-        <v>7.000000000000001</v>
+        <v>7</v>
       </c>
       <c r="D19" t="inlineStr">
         <is>
@@ -1084,7 +1084,7 @@
         </is>
       </c>
       <c r="H19" t="n">
-        <v>74.6719765663147</v>
+        <v>73.7636022567749</v>
       </c>
     </row>
     <row r="20">
@@ -1118,7 +1118,7 @@
         </is>
       </c>
       <c r="H20" t="n">
-        <v>87.21559858322144</v>
+        <v>85.75948619842529</v>
       </c>
     </row>
     <row r="21">
@@ -1152,7 +1152,7 @@
         </is>
       </c>
       <c r="H21" t="n">
-        <v>87.17182087898254</v>
+        <v>86.539879322052</v>
       </c>
     </row>
     <row r="22">
@@ -1186,7 +1186,7 @@
         </is>
       </c>
       <c r="H22" t="n">
-        <v>88.62365412712097</v>
+        <v>85.40753579139709</v>
       </c>
     </row>
     <row r="23">
@@ -1220,7 +1220,7 @@
         </is>
       </c>
       <c r="H23" t="n">
-        <v>336.3985924720764</v>
+        <v>323.9832694530487</v>
       </c>
     </row>
     <row r="24">
@@ -1245,16 +1245,16 @@
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>[[19.021624, 1.7472506, 1.6688626, 1.6790348, 1.8209208, 2.0521138, 2.054815, 2.121197, 2.1072383, 2.2947822, 2.2321472, 2.2020862, 2.203415, 2.342676, 2.2746873, 2.1141517, 2.1437209, 2.200093, 2.0943432, 2.1294081, 2.1982484, 2.2858732, 2.2473252, 2.3265853, 2.3782306, 2.4171698, 2.4565198, 2.4303195, 2.5046697, 2.4850793, 2.2438388, 2.3138103, 2.3832576, 2.5628574, 2.3710432, 2.3893197, 2.3391805, 2.327397, 2.2596638, 2.250886, 2.2748454, 2.3521206, 2.3668537, 2.3700805, 2.3499148, 2.3175216, 2.19469, 2.2315097, 2.153515, 2.2928116, 2.2493265, 2.2492402, 2.256126, 2.2592123, 2.1748374, 2.2384064, 2.1362283, 2.2334552, 2.1477578, 2.1999106], [41.160154581771344, 2.2780125259242587, 2.1610585651149505, 2.1968287326070084, 2.340628006937008, 2.6530549524269045, 2.688579431263903, 2.733204356693886, 2.6847907316182034, 2.98218939673899, 2.9415941317713727, 2.9172215251848725, 2.906163860398083, 3.0780257000857194, 2.9454326250992438, 2.7831548961007715, 2.7649099858895987, 2.829150103678323, 2.7400951608436004, 2.78815486041123, 2.88691019086744, 3.017844534659792, 2.932624341795303, 3.061667192847038, 3.1064453125, 3.2189176941677418, 3.2183788789291734, 3.2254834899432496, 3.2700148285229176, 3.2353290127591015, 2.9247851235781415, 3.0280047476465453, 3.130082079752665, 3.385610925040619, 3.1612115519618937, 3.134712993619697, 3.0501001748065555, 3.044512336403995, 2.9506724027717826, 2.9548233235014085, 3.0015086513218585, 3.139293483288676, 3.096037972328284, 3.1566965523754886, 3.0625096535043963, 3.0054083393432327, 2.8618846781680096, 2.9180574824924834, 2.7404727628175976, 2.9431541082725357, 2.885711287641249, 2.936553965068291, 2.8630779032819262, 2.9035766775793967, 2.8054028292171673, 2.8883489772624644, 2.75672679418869, 2.905007209440599, 2.8174084534957555, 2.8946508467827816], [441145320000000.0, 52017083000000.0, 40760355000000.0, 48267750000000.0, 41424490000000.0, 42451270000000.0, 61486240000000.0, 6260.68, 54481916000000.0, 58039424000000.0, 6366.137, 57946445000000.0, 47629325000000.0, 56094470000000.0, 49927720000000.0, 64990325000000.0, 8361.617, 50599584000000.0, 5152.938, 56292810000000.0, 6371.2886, 45006200000000.0, 6633.4023, 7128.0786, 51563690000000.0, 41842820000000.0, 6144.8223, 6787.595, 5968.099, 55253735000000.0, 64847620000000.0, 63564930000000.0, 72822250000000.0, 7395.583, 52759890000000.0, 65773670000000.0, 72028690000000.0, 49346247000000.0, 65391846000000.0, 75884560000000.0, 7169.6333, 66582957000000.0, 7739.726, 60339387000000.0, 76294890000000.0, 5271.6904, 49897995000000.0, 61713144000000.0, 57031550000000.0, 6769.0747, 68719380000000.0, 79270260000000.0, 56241448000000.0, 57616740000000.0, 57487240000000.0, 67438075000000.0, 55158640000000.0, 57344390000000.0, 52678070000000.0, 51055505000000.0]]</t>
+          <t>[[19.02176, 1.7472546, 1.6686623, 1.6804498, 1.8234748, 2.0567968, 2.0541499, 2.1025896, 2.082619, 2.2651103, 2.215875, 2.1893785, 2.1784718, 2.3399267, 2.2709596, 2.0905743, 2.1226783, 2.1735947, 2.0658956, 2.1080647, 2.177268, 2.255952, 2.2219763, 2.3233242, 2.376677, 2.4080663, 2.4382944, 2.4178338, 2.4693623, 2.44362, 2.1842036, 2.2880027, 2.3688931, 2.548528, 2.368388, 2.3757915, 2.3159866, 2.3102343, 2.2411745, 2.248682, 2.2434347, 2.3183036, 2.3094804, 2.3381104, 2.3277817, 2.308232, 2.1712632, 2.1929915, 2.1154976, 2.2651815, 2.2163498, 2.2139623, 2.229633, 2.2395742, 2.1395252, 2.2082717, 2.1252108, 2.2369177, 2.143524, 2.202378], [41.160378494524316, 2.2780490522453714, 2.1608564404381103, 2.1999625376199368, 2.3445409838770885, 2.6565401704157368, 2.6857989050772964, 2.7101663597536376, 2.659005385285455, 2.9385146965475895, 2.9190096753944457, 2.9003500168137877, 2.865493814675041, 3.0788923362450458, 2.9522896044233584, 2.7545940000317626, 2.733574886425921, 2.8023241547026254, 2.7018578707107688, 2.7577194760116597, 2.8502182391749047, 2.9647498235286704, 2.893514972147711, 3.0724040665327332, 3.1197311234158733, 3.214239867958204, 3.196521483682237, 3.212415517445723, 3.217763657041282, 3.1807477153568087, 2.8529255156957585, 3.0072897716939515, 3.1164390793661267, 3.375849016564811, 3.1516625331271246, 3.1110726327635887, 3.017814513394728, 3.017135795098871, 2.9218511733445296, 2.951111283554445, 2.95474247308888, 3.092274015121352, 3.0128945753085734, 3.120861364696261, 3.0299426533525318, 2.9963060525131855, 2.8367273160888633, 2.862162914168446, 2.68315118641385, 2.896680931989737, 2.8402225289001346, 2.8914600712596683, 2.8362508973699825, 2.877943605221691, 2.7622623151479964, 2.842642264450477, 2.73451032031231, 2.895556393194903, 2.7892238025342784, 2.890857089236371], [441150850000000.0, 52021562000000.0, 40812310000000.0, 48144637000000.0, 41482656000000.0, 42036028000000.0, 61592870000000.0, 6137.408, 53151310000000.0, 57708267000000.0, 6511.1577, 59019603000000.0, 47464195000000.0, 55951520000000.0, 50571120000000.0, 63425527000000.0, 8403.246, 52235355000000.0, 5028.979, 54609130000000.0, 6309.0854, 44809553000000.0, 6543.846, 7122.4155, 50262930000000.0, 42360877000000.0, 5959.397, 6778.546, 5918.5645, 56257610000000.0, 65908542000000.0, 63196006000000.0, 71972650000000.0, 7504.006, 52294377000000.0, 67073334000000.0, 72488610000000.0, 48526596000000.0, 65680326000000.0, 75816120000000.0, 7015.835, 64904644000000.0, 7730.006, 61673017000000.0, 76134380000000.0, 5345.244, 50544520000000.0, 59899830000000.0, 54860440000000.0, 6857.1704, 70424540000000.0, 80371970000000.0, 53843006000000.0, 58826800000000.0, 57945630000000.0, 66538940000000.0, 54770807000000.0, 58336750000000.0, 54317250000000.0, 52513194000000.0]]</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>[[0.5746889179880883, 0.4093414806236034, 0.6746598295478284, 1.111367769135079, 1.3202222714604115, 1.485152677677311, 1.5377773696905177, 1.5732058029362739, 1.5960050552962717, 1.6356759408975727, 1.6676483258788333, 1.645690681202403, 1.6899033656116504, 1.6659161869792418, 1.7149840598025181, 1.557789622451348, 1.653117117898323, 1.6320885125319866, 1.6042307844753627, 1.5943568455600639, 1.7099610877880418, 1.6638761176657784, 1.7018304276144107, 1.7292271116886975, 1.8644399638538391, 1.7743912788019622, 1.8720356425240399, 1.7864240175974575, 1.9271318282804355, 1.7982840856427764, 1.7385979489148733, 1.7246279120751864, 1.8196267609858592, 1.8451035747135742, 1.760685956816855, 1.7656870566211988, 1.7679155203620653, 1.700016920458462, 1.7161162723007726, 1.6673735477572382, 1.7572667905999868, 1.71495115691516, 1.7886998607388818, 1.7464965232862537, 1.790051091629203, 1.7086070520537713, 1.7004542509540364, 1.676395632274662, 1.6727734808979748, 1.6695118859823985, 1.733694808162006, 1.7169705957255823, 1.7824812285658322, 1.6928345094879587, 1.6887727564327142, 1.686603032582686, 1.6675679434126975, 1.665538523008742, 1.6686260215465503, 1.6608645882867201], [1.1616134150194324, 0.7057049082626717, 0.9587663092501608, 1.4630407883834746, 1.7007152367280212, 1.9258137728148188, 1.980579855036033, 2.004836021123198, 2.026396981292455, 2.097103224062101, 2.17839557598828, 2.1568830443417295, 2.1812950810785154, 2.1530162685825553, 2.1900705560908493, 2.0393760169915245, 2.1273961875292424, 2.090520624771634, 2.0804071448614967, 2.081158844242852, 2.215258227199857, 2.1863174475024296, 2.2009116882702355, 2.276831496076033, 2.4357783686385, 2.3814476959141913, 2.4632557778285924, 2.3746428525319505, 2.5110650795796645, 2.329528370419528, 2.2568825571570597, 2.2430048280894046, 2.364638878669504, 2.434017160128259, 2.322693720556796, 2.324374060527786, 2.292921849436863, 2.2181707970994546, 2.2278969780445332, 2.1568816405720623, 2.2961395923114676, 2.2603819436781523, 2.307095832573329, 2.298573938004298, 2.296389512203678, 2.2020386665757603, 2.2100569536280688, 2.166707489215235, 2.116627691858602, 2.1344155018020543, 2.2140687893292608, 2.2201370419747977, 2.24929627792784, 2.1751853893302617, 2.1692997892975487, 2.1549902792641853, 2.148820110401961, 2.155125066281213, 2.1637163223224407, 2.143971548851504], [14904819238068.84, 12020254966188.525, 17325928349849.896, 32019902224676.117, 29192209881720.117, 33235290465096.22, 44932891807761.33, 5014.474406990886, 43455580938917.945, 46016414398721.47, 5219.613223928844, 43473399544259.33, 40522027436476.65, 40891816693938.875, 38171585269601.52, 51273930620454.13, 6338.7564681704525, 39761520613227.6, 3982.458082485737, 39676239889236.62, 5019.731019637449, 35950344421608.805, 5041.208392446936, 5197.338403733854, 42767927445245.93, 33914438787115.914, 4642.020566991956, 5549.208518824561, 4962.634195190842, 38999307988070.805, 49086345062904.55, 51771387123418.25, 57291875110858.555, 5379.266267658753, 42054016346484.445, 49727722645499.97, 53877823236545.23, 35541362210883.47, 51816342501962.76, 58891172018294.21, 5523.438247485153, 52262025118373.89, 6195.039997986388, 47046394786861.414, 57608221538626.086, 4027.809571848401, 40566998231287.305, 44882872372730.5, 45980475705976.74, 5079.3270132457465, 54536573542401.79, 61157792922273.52, 44384380680868.516, 44436401263338.8, 45525367433970.4, 51888471288897.68, 43172586854771.87, 40991205733706.86, 45436390995142.04, 39394331573549.836]]</t>
+          <t>[[0.5746170611944467, 0.40939703499509006, 0.675497757727855, 1.1119396429706532, 1.3282352989118968, 1.4799903067765074, 1.5191278639484578, 1.5504595877822203, 1.5734746347959336, 1.6058494425660255, 1.647290541777229, 1.6115886151037921, 1.6677676950253522, 1.6515336684885025, 1.6948505999910233, 1.528346003794593, 1.6266257133924584, 1.5984005955826697, 1.5823611182045907, 1.573170328787402, 1.6610749380732517, 1.6186285244995544, 1.6705939387346234, 1.722047166599254, 1.8437839906526, 1.7617982333578746, 1.8520747310144186, 1.758277403279238, 1.8717077696465612, 1.7221617803553397, 1.6663455324336647, 1.698578705874035, 1.8041863345851115, 1.8224256306278095, 1.7527971654051822, 1.7392073394596297, 1.7358440622451736, 1.6533960054719734, 1.6873683693932753, 1.6343444496326487, 1.7162131848620694, 1.6521720284856847, 1.7237246019008499, 1.708067502641387, 1.7648801213112537, 1.6771704540220052, 1.6527771253884662, 1.6411412884778789, 1.6384832942542817, 1.6365396448548557, 1.6822151587512535, 1.6785270372695835, 1.7417600662606991, 1.6546185199435968, 1.6545177921840597, 1.6665622121379364, 1.6526848422866198, 1.6545021357538112, 1.6631216460136733, 1.664363825984572], [1.1613842608169893, 0.7056146733050147, 0.9603057023157424, 1.4674806864278975, 1.7063878543577073, 1.9178732052090566, 1.9511987751961577, 1.976132826774635, 2.001127869777952, 2.06141460439858, 2.1510461849352733, 2.1129973286635617, 2.159424134773678, 2.1419154737036967, 2.1749987592386546, 2.0057167552918, 2.0929811523787136, 2.0533697081782214, 2.0609937572081334, 2.0469630368790486, 2.150417046121192, 2.1208481313920826, 2.1678143164195336, 2.2695065839504442, 2.424654433544134, 2.37440018973234, 2.4444179683004768, 2.331865209124119, 2.426549337089467, 2.2184145901740275, 2.1658431010397936, 2.2126347982430405, 2.349857985816374, 2.4180119755630356, 2.303154665620541, 2.2804014244938666, 2.254650652806506, 2.1635662902637183, 2.182344748900742, 2.1109735200966178, 2.236264423097769, 2.1700167033037787, 2.224482164026887, 2.2436959527111036, 2.2750184458383513, 2.157115558672533, 2.1424638466200716, 2.1141233516528293, 2.0664342067161776, 2.0843440523789836, 2.149080557196955, 2.1852947699374674, 2.2078141550262136, 2.1251127150159, 2.1205801280275542, 2.1175751784799868, 2.1300123890693166, 2.1282051692754607, 2.1459321988375586, 2.153959097240614], [14916063885322.502, 12038632948413.543, 17477946726665.479, 32599814267491.97, 30250001868570.375, 32569636546112.688, 44761132805367.94, 4955.607129356308, 42322344874870.016, 45208703787489.67, 5249.569476248824, 43791719665144.72, 38181755357511.414, 41196647081156.4, 38921744834570.484, 48818795567398.93, 6372.950327182027, 39811794825145.37, 4079.275945363819, 37679390833411.09, 4911.192864036088, 34504498060006.64, 4798.805712589678, 5004.8584679373, 41915652777296.15, 34155912052608.152, 4692.2090780491635, 5666.353871557639, 4773.208593843263, 40334922911345.23, 48847178818259.38, 51460394287639.21, 56220386094557.664, 5686.550591772182, 40649039212162.98, 51830760705149.42, 54292211506353.26, 35741073746235.1, 52562677936592.78, 56891166853900.77, 5512.952478134675, 50531356659351.46, 6177.108548049303, 47023960882130.13, 57666072386285.54, 4278.689564863864, 39933232569794.7, 42765286518523.41, 43798956641491.24, 5204.50113078694, 54732142480994.6, 60234654379363.375, 42592629413267.695, 45136927940412.08, 46959735072361.45, 50734372098861.69, 42801511994559.43, 42898819438343.625, 46796549586279.16, 41562349760968.195]]</t>
         </is>
       </c>
       <c r="H24" t="n">
-        <v>336.59290599823</v>
+        <v>320.8354687690735</v>
       </c>
     </row>
     <row r="25">
@@ -1288,7 +1288,7 @@
         </is>
       </c>
       <c r="H25" t="n">
-        <v>342.6138072013855</v>
+        <v>323.3363773822784</v>
       </c>
     </row>
     <row r="26">
@@ -1322,7 +1322,7 @@
         </is>
       </c>
       <c r="H26" t="n">
-        <v>71.11842179298401</v>
+        <v>70.63749957084656</v>
       </c>
     </row>
     <row r="27">
@@ -1356,7 +1356,7 @@
         </is>
       </c>
       <c r="H27" t="n">
-        <v>72.65575385093689</v>
+        <v>69.9848210811615</v>
       </c>
     </row>
     <row r="28">
@@ -1390,7 +1390,7 @@
         </is>
       </c>
       <c r="H28" t="n">
-        <v>70.56700134277344</v>
+        <v>70.05865335464478</v>
       </c>
     </row>
     <row r="29">
@@ -1401,7 +1401,7 @@
         <v>60</v>
       </c>
       <c r="C29" t="n">
-        <v>7.000000000000001</v>
+        <v>7</v>
       </c>
       <c r="D29" t="inlineStr">
         <is>
@@ -1424,7 +1424,7 @@
         </is>
       </c>
       <c r="H29" t="n">
-        <v>73.99883222579956</v>
+        <v>74.42346000671387</v>
       </c>
     </row>
     <row r="30">
@@ -1435,7 +1435,7 @@
         <v>60</v>
       </c>
       <c r="C30" t="n">
-        <v>7.000000000000001</v>
+        <v>7</v>
       </c>
       <c r="D30" t="inlineStr">
         <is>
@@ -1458,7 +1458,7 @@
         </is>
       </c>
       <c r="H30" t="n">
-        <v>73.61430740356445</v>
+        <v>74.37551927566528</v>
       </c>
     </row>
     <row r="31">
@@ -1469,7 +1469,7 @@
         <v>60</v>
       </c>
       <c r="C31" t="n">
-        <v>7.000000000000001</v>
+        <v>7</v>
       </c>
       <c r="D31" t="inlineStr">
         <is>
@@ -1492,7 +1492,7 @@
         </is>
       </c>
       <c r="H31" t="n">
-        <v>73.83419299125671</v>
+        <v>74.45973873138428</v>
       </c>
     </row>
     <row r="32">
@@ -1526,7 +1526,7 @@
         </is>
       </c>
       <c r="H32" t="n">
-        <v>86.1461296081543</v>
+        <v>86.39232158660889</v>
       </c>
     </row>
     <row r="33">
@@ -1560,7 +1560,7 @@
         </is>
       </c>
       <c r="H33" t="n">
-        <v>86.28099322319031</v>
+        <v>86.65736937522888</v>
       </c>
     </row>
     <row r="34">
@@ -1594,7 +1594,7 @@
         </is>
       </c>
       <c r="H34" t="n">
-        <v>86.20981001853943</v>
+        <v>86.61663103103638</v>
       </c>
     </row>
     <row r="35">
@@ -1628,7 +1628,7 @@
         </is>
       </c>
       <c r="H35" t="n">
-        <v>324.1020879745483</v>
+        <v>322.390789270401</v>
       </c>
     </row>
     <row r="36">
@@ -1662,7 +1662,7 @@
         </is>
       </c>
       <c r="H36" t="n">
-        <v>328.0311641693115</v>
+        <v>322.4779179096222</v>
       </c>
     </row>
     <row r="37">
@@ -1696,7 +1696,7 @@
         </is>
       </c>
       <c r="H37" t="n">
-        <v>328.280775308609</v>
+        <v>325.5778000354767</v>
       </c>
     </row>
     <row r="38">
@@ -1730,7 +1730,7 @@
         </is>
       </c>
       <c r="H38" t="n">
-        <v>70.43763780593872</v>
+        <v>70.85962176322937</v>
       </c>
     </row>
     <row r="39">
@@ -1764,7 +1764,7 @@
         </is>
       </c>
       <c r="H39" t="n">
-        <v>70.5172905921936</v>
+        <v>70.68206572532654</v>
       </c>
     </row>
     <row r="40">
@@ -1798,7 +1798,7 @@
         </is>
       </c>
       <c r="H40" t="n">
-        <v>69.65368914604187</v>
+        <v>70.77211713790894</v>
       </c>
     </row>
     <row r="41">
@@ -1809,7 +1809,7 @@
         <v>80</v>
       </c>
       <c r="C41" t="n">
-        <v>7.000000000000001</v>
+        <v>7</v>
       </c>
       <c r="D41" t="inlineStr">
         <is>
@@ -1832,7 +1832,7 @@
         </is>
       </c>
       <c r="H41" t="n">
-        <v>74.26700520515442</v>
+        <v>74.82894897460938</v>
       </c>
     </row>
     <row r="42">
@@ -1843,7 +1843,7 @@
         <v>80</v>
       </c>
       <c r="C42" t="n">
-        <v>7.000000000000001</v>
+        <v>7</v>
       </c>
       <c r="D42" t="inlineStr">
         <is>
@@ -1866,7 +1866,7 @@
         </is>
       </c>
       <c r="H42" t="n">
-        <v>74.07641315460205</v>
+        <v>74.74545335769653</v>
       </c>
     </row>
     <row r="43">
@@ -1877,7 +1877,7 @@
         <v>80</v>
       </c>
       <c r="C43" t="n">
-        <v>7.000000000000001</v>
+        <v>7</v>
       </c>
       <c r="D43" t="inlineStr">
         <is>
@@ -1900,7 +1900,7 @@
         </is>
       </c>
       <c r="H43" t="n">
-        <v>74.37517905235291</v>
+        <v>74.86355686187744</v>
       </c>
     </row>
     <row r="44">
@@ -1934,7 +1934,7 @@
         </is>
       </c>
       <c r="H44" t="n">
-        <v>86.62823486328125</v>
+        <v>86.6973729133606</v>
       </c>
     </row>
     <row r="45">
@@ -1968,7 +1968,7 @@
         </is>
       </c>
       <c r="H45" t="n">
-        <v>87.60683989524841</v>
+        <v>86.83557367324829</v>
       </c>
     </row>
     <row r="46">
@@ -2002,7 +2002,7 @@
         </is>
       </c>
       <c r="H46" t="n">
-        <v>86.74522924423218</v>
+        <v>87.40689468383789</v>
       </c>
     </row>
     <row r="47">
@@ -2036,7 +2036,7 @@
         </is>
       </c>
       <c r="H47" t="n">
-        <v>326.8348772525787</v>
+        <v>324.3329286575317</v>
       </c>
     </row>
     <row r="48">
@@ -2070,7 +2070,7 @@
         </is>
       </c>
       <c r="H48" t="n">
-        <v>326.8818576335907</v>
+        <v>325.1775486469269</v>
       </c>
     </row>
     <row r="49">
@@ -2104,7 +2104,7 @@
         </is>
       </c>
       <c r="H49" t="n">
-        <v>325.6274273395538</v>
+        <v>325.307831287384</v>
       </c>
     </row>
     <row r="50">
@@ -2138,7 +2138,7 @@
         </is>
       </c>
       <c r="H50" t="n">
-        <v>69.82395505905151</v>
+        <v>70.45864129066467</v>
       </c>
     </row>
     <row r="51">
@@ -2172,7 +2172,7 @@
         </is>
       </c>
       <c r="H51" t="n">
-        <v>70.42151308059692</v>
+        <v>70.82089686393738</v>
       </c>
     </row>
     <row r="52">
@@ -2206,7 +2206,7 @@
         </is>
       </c>
       <c r="H52" t="n">
-        <v>70.21504950523376</v>
+        <v>70.28847098350525</v>
       </c>
     </row>
     <row r="53">
@@ -2217,7 +2217,7 @@
         <v>100</v>
       </c>
       <c r="C53" t="n">
-        <v>7.000000000000001</v>
+        <v>7</v>
       </c>
       <c r="D53" t="inlineStr">
         <is>
@@ -2240,7 +2240,7 @@
         </is>
       </c>
       <c r="H53" t="n">
-        <v>74.24421191215515</v>
+        <v>74.95986318588257</v>
       </c>
     </row>
     <row r="54">
@@ -2251,7 +2251,7 @@
         <v>100</v>
       </c>
       <c r="C54" t="n">
-        <v>7.000000000000001</v>
+        <v>7</v>
       </c>
       <c r="D54" t="inlineStr">
         <is>
@@ -2274,7 +2274,7 @@
         </is>
       </c>
       <c r="H54" t="n">
-        <v>74.02620816230774</v>
+        <v>74.89960408210754</v>
       </c>
     </row>
     <row r="55">
@@ -2285,7 +2285,7 @@
         <v>100</v>
       </c>
       <c r="C55" t="n">
-        <v>7.000000000000001</v>
+        <v>7</v>
       </c>
       <c r="D55" t="inlineStr">
         <is>
@@ -2308,7 +2308,7 @@
         </is>
       </c>
       <c r="H55" t="n">
-        <v>74.10019207000732</v>
+        <v>74.77932119369507</v>
       </c>
     </row>
     <row r="56">
@@ -2342,7 +2342,7 @@
         </is>
       </c>
       <c r="H56" t="n">
-        <v>90.00622415542603</v>
+        <v>86.73352861404419</v>
       </c>
     </row>
     <row r="57">
@@ -2376,7 +2376,7 @@
         </is>
       </c>
       <c r="H57" t="n">
-        <v>98.45256376266479</v>
+        <v>87.44598460197449</v>
       </c>
     </row>
     <row r="58">
@@ -2410,7 +2410,7 @@
         </is>
       </c>
       <c r="H58" t="n">
-        <v>88.22850680351257</v>
+        <v>86.96142029762268</v>
       </c>
     </row>
     <row r="59">
@@ -2444,7 +2444,7 @@
         </is>
       </c>
       <c r="H59" t="n">
-        <v>327.8595552444458</v>
+        <v>324.3675866127014</v>
       </c>
     </row>
     <row r="60">
@@ -2478,7 +2478,7 @@
         </is>
       </c>
       <c r="H60" t="n">
-        <v>327.3955166339874</v>
+        <v>325.2948715686798</v>
       </c>
     </row>
     <row r="61">
@@ -2503,16 +2503,16 @@
       </c>
       <c r="F61" t="inlineStr">
         <is>
-          <t>[[4.5329, 1.629069, 1.5980245, 1.7719696, 1.9128791, 2.0950766, 2.1013708, 2.224636, 2.1874566, 2.3154078, 2.1270778, 2.0976756, 2.0675163, 2.2326815, 2.3350818, 2.2944613, 2.1632218, 2.140396, 2.0798836, 2.2221222, 2.0735862, 2.2134638, 2.1693118, 2.2378035, 2.2970107, 2.3814275, 2.4074605, 2.4473157, 2.3940332, 2.5086439, 2.4902732, 2.3724163, 2.3359494, 2.311555, 2.26369, 2.413797, 2.3025343, 2.3469276, 2.3938441, 2.31991, 2.1598372, 2.2929592, 2.2175002, 2.1938481, 2.1598237, 2.19496, 2.2072766, 2.1903408, 2.1947067, 2.2525072, 2.3219862, 2.2610734, 2.284334, 2.324153, 2.190139, 2.2085333, 2.1996434, 2.2273061, 2.1913385, 2.239844], [6.106633890944122, 2.1068657538144064, 2.066221751754418, 2.293213917299388, 2.465416698093703, 2.735995177788974, 2.775829132895344, 2.9575913980892894, 2.8290071744912124, 2.9913654044653635, 2.7252361930187368, 2.6946828797840605, 2.675507424258883, 2.912119035813536, 3.0396574168669175, 2.9500218794706368, 2.783850407872935, 2.808845943752716, 2.7188116483166347, 2.9029438533051057, 2.6596433618428663, 2.866756063738157, 2.821809746377487, 2.874315429123288, 2.9953055209067103, 3.1472411047861066, 3.1254620019814796, 3.206196870419408, 3.0938051777552626, 3.2237205273869955, 3.192415523740715, 3.0563089501560063, 2.9898997991096325, 2.9354406402309237, 2.9326724702373412, 3.150950146231394, 2.9651998072390646, 3.0046033509244974, 3.0488479877536037, 2.978631849679119, 2.753268640172269, 2.9870717910910405, 2.8492797075198797, 2.8790559768561454, 2.811717454338146, 2.7938858340564767, 2.8142222747263874, 2.813741960755518, 2.794802020026864, 2.8625740541432463, 2.962936330604954, 2.952272806882407, 2.962409063947483, 3.0258073218118944, 2.8757654912465536, 2.9009975427711177, 2.8579231286679145, 2.882281329420546, 2.8590087656084884, 2.902670676300312], [87905985000000.0, 44005150000000.0, 44930005000000.0, 38902623000000.0, 42120677000000.0, 37371836000000.0, 5686.91, 6788.6475, 45726495000000.0, 6785.88, 53080075000000.0, 45797974000000.0, 67610610000000.0, 60248360000000.0, 36188174000000.0, 64759700000000.0, 5433.4424, 42541320000000.0, 49615747000000.0, 58388400000000.0, 47906650000000.0, 57303466000000.0, 51573678000000.0, 6202.8726, 6547.6665, 72166770000000.0, 33915415000000.0, 39931180000000.0, 55537954000000.0, 49452530000000.0, 57759820000000.0, 51158492000000.0, 53986653000000.0, 68327040000000.0, 61091830000000.0, 47344300000000.0, 46337186000000.0, 55280755000000.0, 53006326000000.0, 59808800000000.0, 5453.1265, 57494810000000.0, 35691203000000.0, 6955.913, 44678934000000.0, 49299910000000.0, 39436625000000.0, 40376195000000.0, 50719692000000.0, 47190570000000.0, 4843.4497, 36343418000000.0, 49111538000000.0, 37026812000000.0, 50230184000000.0, 48162060000000.0, 46101697000000.0, 52013266000000.0, 5136.2017, 66569913000000.0]]</t>
+          <t>[[4.5329, 1.629069, 1.5980245, 1.7719674, 1.9010519, 2.0852118, 2.0772655, 2.211173, 2.1492293, 2.2866426, 2.1150393, 2.0904655, 2.0305457, 2.2090943, 2.3251975, 2.283997, 2.1381538, 2.126093, 2.0636365, 2.216777, 2.0201018, 2.1909013, 2.1635175, 2.242099, 2.2644753, 2.3502774, 2.3754697, 2.4342024, 2.370375, 2.4994175, 2.4720194, 2.3606415, 2.3124454, 2.2939067, 2.2492883, 2.4145393, 2.281288, 2.3243656, 2.3804996, 2.3098438, 2.1229067, 2.2648213, 2.2111878, 2.1936803, 2.146972, 2.1880064, 2.1951554, 2.1703534, 2.1629324, 2.2306619, 2.3100631, 2.2541835, 2.2602806, 2.3076024, 2.1736844, 2.1981983, 2.172207, 2.2007706, 2.1743674, 2.2250013], [6.106633890944122, 2.1068657538144064, 2.066221751754418, 2.2932153728369737, 2.4506823776676847, 2.7246148003418207, 2.739701842632413, 2.9339111806561227, 2.7764079774912056, 2.951876744858006, 2.707112717056292, 2.68334373408922, 2.6316064624853723, 2.8836303212532077, 3.022826140345465, 2.9424703226075652, 2.7475300013368096, 2.7871430788628744, 2.6837807580458355, 2.8943279570774485, 2.589798548607475, 2.840747967399119, 2.8191331421154326, 2.8820121501849147, 2.944872431169856, 3.1060650714805518, 3.091069611292814, 3.1860557725027423, 3.056393510378401, 3.2084178830850574, 3.171288647504515, 3.043752625638546, 2.9684183035813234, 2.920165025672461, 2.916125674256698, 3.151767228927961, 2.9311989916041776, 2.9656440951312444, 3.02859270481646, 2.9662559875093484, 2.7105649312835327, 2.952446592204807, 2.848082543216336, 2.876835610242082, 2.793482337094235, 2.786410655151506, 2.799143803344036, 2.7930980732461292, 2.7546744066642352, 2.8314961105392715, 2.9398167990352135, 2.9376334302101217, 2.933636823762088, 3.0016300223608, 2.8530196138036006, 2.8897844071803886, 2.8260304824902134, 2.8512357341672034, 2.84528753614289, 2.886308571215823], [87905985000000.0, 44005150000000.0, 44930005000000.0, 38901890000000.0, 42029858000000.0, 36965860000000.0, 5661.9473, 6695.325, 44156640000000.0, 6779.52, 53702073000000.0, 45558438000000.0, 65770294000000.0, 58334800000000.0, 36169404000000.0, 64502930000000.0, 5309.4087, 42432348000000.0, 49558350000000.0, 58535363000000.0, 46657564000000.0, 56484250000000.0, 51662257000000.0, 6146.9897, 6576.3354, 70353984000000.0, 33741544000000.0, 39540770000000.0, 54875665000000.0, 49242542000000.0, 57889545000000.0, 50254120000000.0, 53469025000000.0, 69859975000000.0, 60355036000000.0, 47915796000000.0, 46057744000000.0, 54943185000000.0, 53006260000000.0, 59757835000000.0, 5641.3647, 56817550000000.0, 34992894000000.0, 7018.112, 43702274000000.0, 50949825000000.0, 40725677000000.0, 41247510000000.0, 50957065000000.0, 45954196000000.0, 4746.4253, 36694934000000.0, 48122626000000.0, 36083020000000.0, 47346910000000.0, 47847890000000.0, 44503290000000.0, 51545120000000.0, 5026.524, 66652977000000.0]]</t>
         </is>
       </c>
       <c r="G61" t="inlineStr">
         <is>
-          <t>[[0.36545564370229555, 0.492274193873011, 0.9772335232822069, 1.2889557713476065, 1.4625099402297406, 1.5371380195783928, 1.5795835857653215, 1.6523458257921846, 1.6730871190058463, 1.6747356344526847, 1.5873462579237296, 1.5713638115184205, 1.5947410375691562, 1.6355551941243063, 1.7828498463413704, 1.7137844840732384, 1.6825966310268428, 1.59769266216977, 1.5931700991414801, 1.6799753279885437, 1.592037621933286, 1.6149121079537476, 1.652981576185553, 1.7213610510977673, 1.8226833640412865, 1.7654436343538893, 1.8410270180768629, 1.8516665760131807, 1.8536697622150349, 1.8381029821305641, 1.886603818277256, 1.8259982714448608, 1.8091151653034374, 1.7400813840418012, 1.7317706667893267, 1.8260321306808316, 1.7942040933124155, 1.750712239663118, 1.83633790668995, 1.7550667600639407, 1.6858618419373188, 1.6952664383702898, 1.7025289348702795, 1.6846633214540145, 1.7034378430843182, 1.652142633869099, 1.7059531915617352, 1.6871388890267518, 1.7533111508757004, 1.7225361538907578, 1.8041861562905608, 1.7432256979578753, 1.775366160203873, 1.7609979519916172, 1.7071186752550973, 1.6951282096861306, 1.7208389167377336, 1.6686924023242937, 1.6665334748698162, 1.6730868100755172], [0.744658374879008, 0.7627257789421134, 1.2897362366050575, 1.6654695348227837, 1.8709220582185913, 1.98264126105368, 2.048622027008297, 2.1268095903757236, 2.1440932764681886, 2.143032711281382, 2.0251333986003632, 2.0066960972006336, 2.0352533066588205, 2.125843398555283, 2.315473031598312, 2.1971599662984884, 2.1715846942271817, 2.09519403225706, 2.0542185247586797, 2.1766322195249668, 2.0350460197730733, 2.0986656953512917, 2.151235723374196, 2.2211860219102992, 2.3990190124564417, 2.332947317891089, 2.397142883527333, 2.420566646408548, 2.397858599920702, 2.368509698537882, 2.4096849009467345, 2.3617743668212836, 2.3134333084317573, 2.2180346559281565, 2.236212627769175, 2.374960532337695, 2.289524532996502, 2.2157208016367984, 2.3493311283207827, 2.2311971180716785, 2.1535027407250604, 2.1829833711666327, 2.171111347906698, 2.2054774670047546, 2.1955939325390266, 2.09649844725187, 2.1793128238006925, 2.1670405363502914, 2.2248775580024565, 2.185494011176966, 2.296985096174724, 2.267799692644097, 2.2921587635354377, 2.278094613897878, 2.2341478387229174, 2.211204697979898, 2.2250249882633484, 2.1494917162786087, 2.1712021838350974, 2.1498350182001866], [7681795883177.022, 16327548450989.656, 27874955717395.617, 27630600082277.207, 32457663612205.523, 28153997274490.38, 4510.993130240259, 5463.646118265561, 34226202009575.848, 4897.594829422183, 37321899253838.83, 34198691606757.992, 53252822601002.99, 45298305249083.82, 28405655612561.605, 51234784980779.85, 4470.899526782039, 33749714723872.63, 40464711664353.945, 44526646832823.21, 36335620915686.81, 41996989959693.836, 40139900140008.87, 4954.31295508242, 5206.259988508137, 49291125949809.336, 26784373008196.902, 27973791170556.73, 44217378428675.81, 35243214130819.36, 46520506706298.79, 40682177625640.2, 45154549978184.02, 53071940133804.34, 46508148037291.39, 38384041160750.13, 37518870001659.07, 45215890863214.016, 41783369468325.98, 44494440499378.69, 4411.933361571146, 44046372548181.41, 27396753840495.098, 5552.47282734815, 36414654412693.54, 38856129638883.49, 31987631906254.6, 32707438313848.2, 41870138162480.24, 34381491401138.44, 3994.7582004806636, 27593142183302.258, 39492822568085.125, 28899652788678.473, 40175615970963.39, 37635937459579.51, 37516788127862.72, 39579049294146.75, 3847.022126604569, 51446107348336.79]]</t>
+          <t>[[0.36545564370229555, 0.492274193873011, 0.9772335232822069, 1.2643347428142881, 1.4422258923383546, 1.5186903753048617, 1.5653057925912823, 1.5946496162003536, 1.633105966495094, 1.6521898074864227, 1.575814649924206, 1.5207562931922443, 1.5613703412275168, 1.6264738713956823, 1.7713341655166597, 1.6709500790863359, 1.6494045288923913, 1.5744714308436896, 1.5854248290843749, 1.6112747937398024, 1.5411847838203072, 1.6008837129927216, 1.6544319413505202, 1.6690964754757478, 1.786408019078253, 1.7221606299629195, 1.8111872011061791, 1.815255586702612, 1.8250295105869279, 1.8238418123566287, 1.8681394855149163, 1.778662631358601, 1.7841900599450362, 1.724503445421477, 1.7312571839000304, 1.799206650427577, 1.761721984689062, 1.7227424958837585, 1.8233597901866927, 1.7053648463500417, 1.6421165483767728, 1.6866345698936933, 1.6967853726544682, 1.6584447767251775, 1.6774375390426701, 1.6385969208745044, 1.6878414516444602, 1.6442496529932191, 1.7145454803605378, 1.7024672547871398, 1.7994718490425672, 1.7076296797116808, 1.7363072001096145, 1.7349835175568855, 1.6915675244748822, 1.6480524692596783, 1.6818238839366493, 1.6451143356171682, 1.6407975074923928, 1.6352866563497184], [0.744658374879008, 0.7627257789421134, 1.2897362366050575, 1.6348958627720693, 1.8472563703363514, 1.9601188168503134, 2.0333258613245824, 2.054521794741175, 2.0925141307900823, 2.1087099632404334, 2.0098410290016373, 1.9442324982095789, 1.9973529843986364, 2.1135323089276516, 2.2984002345442804, 2.149456219470227, 2.1324396983412868, 2.0556505661397333, 2.039667757616228, 2.085766132861766, 1.9758371303676248, 2.0840272509624747, 2.1637321260397697, 2.1583951150043883, 2.344029389594686, 2.2726620455879076, 2.3608461979195146, 2.3744152366353988, 2.3552228265217723, 2.349601809276664, 2.3902856547575277, 2.308860867257134, 2.2904737257308248, 2.20402980634205, 2.2344124272089365, 2.336904020004119, 2.24297469237933, 2.1758382224811474, 2.3279929739744842, 2.171483281114559, 2.101577935418944, 2.1764357142712933, 2.168135041993254, 2.1660904644439865, 2.16732248037242, 2.0825172585872376, 2.1603139866834993, 2.116740090190517, 2.1742666630622653, 2.156958083525187, 2.2882597705221617, 2.2209729197615284, 2.2401145231366524, 2.2429645932091056, 2.209775947105219, 2.155678038831754, 2.171591524135687, 2.121200503960416, 2.138099379389116, 2.10263350982091], [7681795883177.022, 16327548450989.656, 27874955717395.617, 27270908025487.69, 32402410380370.89, 27317884825070.332, 4463.493204212393, 5126.733591356293, 32970617598097.83, 4900.120337792754, 38208233841542.28, 32513825112993.297, 52011254326088.79, 43282142112437.086, 28925783093426.387, 50296196702618.625, 4293.4704268877385, 33802404845341.527, 40293450573930.08, 42718211711215.87, 35647847772606.234, 41576477504315.2, 40521432803388.81, 4734.212161287911, 5190.230211598686, 48194002358914.61, 27033189009953.84, 27799681076079.184, 42605554704105.61, 35198441603619.34, 45447202934696.76, 39652915231093.07, 44136626904197.39, 54282618180923.85, 47055643227380.516, 37945905224653.94, 36751580567320.6, 44347916112394.72, 41905052694958.9, 43792126232994.914, 4569.461890690242, 44924154275177.86, 26125093784583.836, 5566.732278716495, 35439616251848.41, 39500991262589.28, 33725889438719.332, 33011911563866.38, 42036750910454.52, 33546258570924.96, 3907.749260053315, 28432672282533.527, 37485339541882.44, 28507106048925.7, 38797528055263.2, 36558637038995.01, 36473235352187.79, 39048414923717.8, 3776.789897682635, 50730477328421.31]]</t>
         </is>
       </c>
       <c r="H61" t="n">
-        <v>330.9424521923065</v>
+        <v>323.5603556632996</v>
       </c>
     </row>
     <row r="62">
@@ -2546,7 +2546,7 @@
         </is>
       </c>
       <c r="H62" t="n">
-        <v>70.2675576210022</v>
+        <v>70.28494024276733</v>
       </c>
     </row>
     <row r="63">
@@ -2580,7 +2580,7 @@
         </is>
       </c>
       <c r="H63" t="n">
-        <v>69.89214444160461</v>
+        <v>69.70389795303345</v>
       </c>
     </row>
     <row r="64">
@@ -2614,7 +2614,7 @@
         </is>
       </c>
       <c r="H64" t="n">
-        <v>69.66054201126099</v>
+        <v>70.29813241958618</v>
       </c>
     </row>
     <row r="65">
@@ -2625,7 +2625,7 @@
         <v>20</v>
       </c>
       <c r="C65" t="n">
-        <v>7.000000000000001</v>
+        <v>7</v>
       </c>
       <c r="D65" t="inlineStr">
         <is>
@@ -2639,16 +2639,16 @@
       </c>
       <c r="F65" t="inlineStr">
         <is>
-          <t>[[5.072774, 1.9171237, 1.40701, 1.5621375, 1.5400696, 1.5958776, 1.5516644, 1.7498499, 1.6910747, 1.7366577, 1.6504236, 1.7822266, 1.6007158, 1.720482, 1.6947293, 1.7268856, 1.6712643, 1.6331738, 1.5772142, 1.5809778, 1.5294951, 1.5841902, 1.5957531, 1.7296977, 1.7116584, 1.7502664, 1.7722313, 1.9293497, 1.9345949, 2.018456, 2.0887556, 2.1050887, 2.0718045, 1.9955047, 1.9294177, 1.9498854, 1.7354919, 1.6314833, 1.650086, 1.7277932, 1.6404128, 1.6929569, 1.647561, 1.728691, 1.632743, 1.8098719, 1.7273577, 1.7803931, 1.7087791, 1.8761711, 1.8232065, 1.822256, 1.7355019, 1.7131758, 1.6857134, 1.6960982, 1.6247797, 1.7129219, 1.6341562, 1.6188858], [7.112707677400386, 2.8679958108421815, 2.010984179259543, 2.1253519327784947, 2.0535318003556755, 2.1014925012665735, 2.0805737974925917, 2.33377240227938, 2.264660333928704, 2.323889649757072, 2.234363795965954, 2.3954496878139904, 2.16695907037983, 2.2643612197932583, 2.3078669970979577, 2.332268426486024, 2.238712715251656, 2.192669998764115, 2.1583278430098094, 2.1546222237041657, 2.0298256208191474, 2.0851457214661364, 2.1422080987097147, 2.3368891687976245, 2.3204894335554895, 2.3181009252989453, 2.443352934831141, 2.6021184470436904, 2.658248329198666, 2.775074736130034, 3.03738223502983, 3.057491488752894, 3.045820161205638, 2.7671533014907967, 2.6878670730080096, 2.6743502389252334, 2.3735578073293024, 2.1581129788865714, 2.2247798810796073, 2.300609225981011, 2.1721979353973326, 2.2082095081473945, 2.2513082727391662, 2.3958650890954782, 2.250419153801765, 2.481460108857401, 2.4319253410123043, 2.420452660084868, 2.285081754595031, 2.525544600723361, 2.4710999905136286, 2.42527827209849, 2.3444151888082128, 2.302896715545598, 2.283334276333728, 2.233490028388123, 2.114898006784621, 2.231240588256476, 2.1784393127547688, 2.132649062605228], [1.8933061, 0.58515024, 0.37898377, 0.3750468, 0.43902162, 0.4167097, 0.4180984, 0.4199218, 0.59979177, 0.6565855, 0.55069715, 0.66471136, 0.602158, 0.5634688, 0.51939267, 0.46367294, 0.43540695, 0.3289852, 0.3413561, 0.38459906, 0.3732717, 0.36168966, 0.38440555, 0.45049983, 0.3913175, 0.37354544, 0.4499613, 0.39622724, 0.45734143, 0.35531312, 0.4371456, 0.44313484, 0.501615, 0.45484868, 0.47894996, 0.49204865, 0.55778235, 0.4799318, 0.5407477, 0.50323874, 0.45648852, 0.3634526, 0.49316823, 0.50973755, 0.5537259, 0.4580775, 0.58132994, 0.5584787, 0.51393026, 0.43620747, 0.5448207, 0.582123, 0.5073426, 0.46667987, 0.44616663, 0.42300957, 0.45472157, 0.5271893, 0.5206788, 0.5458481]]</t>
+          <t>[[5.073095, 1.9258051, 1.4144356, 1.5610487, 1.5366385, 1.6057329, 1.5724618, 1.7557364, 1.6794773, 1.7506785, 1.671003, 1.771811, 1.5886703, 1.7355791, 1.7114211, 1.7517508, 1.716023, 1.679281, 1.6289582, 1.6177058, 1.523226, 1.5643461, 1.58727, 1.7106727, 1.685833, 1.7459403, 1.7635108, 1.9155114, 1.9148469, 2.0410767, 2.1231701, 2.1529045, 2.0839982, 2.0292776, 1.9341229, 1.9469306, 1.7544876, 1.6815878, 1.6932812, 1.7595847, 1.6603019, 1.7570531, 1.6906891, 1.746762, 1.6623455, 1.8355696, 1.7397487, 1.7702466, 1.7146378, 1.8918211, 1.84857, 1.8854984, 1.7662337, 1.765943, 1.7250973, 1.700914, 1.6378447, 1.7482128, 1.6550705, 1.6421427], [7.1131163425592305, 2.8926818128466074, 2.0292187437963807, 2.1326622543233666, 2.0552452113739936, 2.1182229300761155, 2.11994411160918, 2.361114063136431, 2.264608431352112, 2.339687743423223, 2.251120288422633, 2.3891213868233154, 2.168624641247361, 2.2893217285023564, 2.356043503513464, 2.4073110445685066, 2.327984594425209, 2.2663414184176234, 2.223651575973481, 2.173484370633294, 2.025619449766771, 2.06272574836549, 2.124007049146546, 2.302389570439769, 2.2708905297405213, 2.322101866367905, 2.4314424610205485, 2.5749303271302693, 2.632560650017258, 2.8333016749090594, 3.135769254982835, 3.188885107344609, 3.045345137505889, 2.8020067074495967, 2.6781821958116296, 2.661834680234421, 2.4060454839020537, 2.248350280384906, 2.316191845085058, 2.36333481909199, 2.203577522716323, 2.3034298326268696, 2.304314845070526, 2.420936057909084, 2.253450608766183, 2.4836499577702034, 2.4274564355306, 2.4074710868770928, 2.2973417469600466, 2.53285543133582, 2.501267683966566, 2.4919707105332844, 2.3907091711846764, 2.368764723276565, 2.3251284574072084, 2.23242027302682, 2.1330900465803286, 2.2762897859602034, 2.2124489514340024, 2.158644631911678], [1.8933344, 0.5867835, 0.38089868, 0.36321282, 0.42525032, 0.4206939, 0.41878366, 0.42397866, 0.60051376, 0.6587192, 0.5644233, 0.6792292, 0.61320776, 0.58839583, 0.53524566, 0.49281234, 0.46100605, 0.3459819, 0.34927344, 0.4063516, 0.37709188, 0.35503143, 0.38505706, 0.44304854, 0.383022, 0.37625897, 0.4504532, 0.40239215, 0.42876357, 0.35143498, 0.44156614, 0.43918985, 0.48691088, 0.45905972, 0.4643202, 0.4845072, 0.5487226, 0.47954515, 0.52814233, 0.49556533, 0.45104897, 0.36649466, 0.50592506, 0.5013601, 0.5535873, 0.45897642, 0.55769867, 0.51944023, 0.48576358, 0.40736204, 0.53101766, 0.58401257, 0.5184706, 0.48448408, 0.46962404, 0.41221672, 0.4401059, 0.50326294, 0.5096419, 0.5433005]]</t>
         </is>
       </c>
       <c r="G65" t="inlineStr">
         <is>
-          <t>[[1.8756422024121677, 1.1820937099780238, 1.1629020367624172, 1.3194003485529333, 1.3883056115575259, 1.4182697520228977, 1.3932094362922562, 1.5304425257049048, 1.533589552752149, 1.5342823041279405, 1.4568707097838758, 1.5417605676403345, 1.4345123415460361, 1.5084991939814076, 1.4649944227408136, 1.4907402592448065, 1.501208551003261, 1.4673854108709778, 1.3811737262609023, 1.4039643941826925, 1.395561385478558, 1.4145956305876846, 1.4136329857281098, 1.507573727938576, 1.517544770187455, 1.5458800464738987, 1.512414506554377, 1.6488838129523102, 1.7002380618885418, 1.7746507094425286, 1.8183726900284922, 1.7969621484179044, 1.829098223370809, 1.7552978354077988, 1.671465683299271, 1.649239010010089, 1.5498679598090466, 1.454469409607432, 1.44416030760105, 1.4971265032980567, 1.4613402872737895, 1.4943843100958163, 1.4613331681774329, 1.485431995038555, 1.502348741490128, 1.6022257885315283, 1.5488133710819991, 1.523112299588756, 1.5354791769741385, 1.6503029453765172, 1.574553220717462, 1.5958990389624506, 1.5464841836150485, 1.522521724521516, 1.5050199403962161, 1.4644043892479395, 1.4760686526681805, 1.52579718659992, 1.4267904215863763, 1.4157174570365607], [3.178318420458754, 1.80055006500076, 1.641683958728912, 1.7599533312170121, 1.8297223701258907, 1.86132367378803, 1.853887628648685, 2.0321405867313405, 2.040999906545612, 2.0427339464482293, 1.9563592182464247, 2.0566099606522203, 1.9161775633214186, 1.9870669512192451, 1.9585614190769194, 2.00776157090442, 1.9935271394203555, 1.9857600112282636, 1.8651702031642174, 1.9033116455120864, 1.8354317436581071, 1.8520253793351675, 1.878208104437471, 2.0362594486595853, 2.0172186917459536, 2.04824134713758, 2.032566777643488, 2.190699280343132, 2.3038531691604134, 2.4390568634628678, 2.6540024106115183, 2.629773772050095, 2.6789211834124487, 2.4544473316620916, 2.290080625561898, 2.2358988585295467, 2.0612080275796183, 1.9141583821115615, 1.9384840832886348, 1.9759855574478802, 1.9142856431094024, 1.9424879452404606, 1.9784487142550387, 2.02420475621663, 2.0589247923319074, 2.2158295728984694, 2.17881280904067, 2.0408300640374977, 2.0636955371213936, 2.2303128128204026, 2.1103408977505844, 2.129558907254195, 2.0526191615998233, 2.0370163356068454, 2.0390825916948825, 1.924056549385475, 1.9054456944769198, 1.9902817692191865, 1.8793372822811107, 1.8828269065921734], [0.49203713913242975, 0.3114771904561408, 0.3010253027318236, 0.33077470256401575, 0.3923178671930951, 0.3840911447607357, 0.3693096501860028, 0.3644448499486468, 0.5567847895591553, 0.5519923357926757, 0.4791133904600206, 0.5526526542446581, 0.5291420065896824, 0.48818575852160073, 0.4415295333019513, 0.40059779201503787, 0.36529002931405424, 0.28973465908276447, 0.2943383507731046, 0.346159447586192, 0.33825460124162576, 0.3251837685313617, 0.32770222007541844, 0.3880817013279388, 0.3428363047779474, 0.3318850646815356, 0.3901612765370101, 0.3400318779019036, 0.3923571576423574, 0.31404218613690277, 0.3753014250043085, 0.377251124868461, 0.43366429503035, 0.40131798431763477, 0.41592328370190434, 0.4193892676236494, 0.486842685302789, 0.4364150226994636, 0.4569730834036053, 0.426211528288462, 0.41056796160445735, 0.32222265079626833, 0.43811058783993545, 0.4328917069443441, 0.5148710851955047, 0.4108287046066309, 0.5163741813606918, 0.45785868604252233, 0.46171467849374653, 0.3720999693405082, 0.4679036529028119, 0.4942735643133451, 0.4395079799749249, 0.41713178181557153, 0.39401690152795943, 0.3586271408163559, 0.4128036899749845, 0.4618746654103352, 0.44535323029644863, 0.4850923957731059]]</t>
+          <t>[[1.8835970868199894, 1.1853990772455523, 1.1604260119762344, 1.3146799701139156, 1.4031081744486256, 1.4365581198441537, 1.3941654334327342, 1.5201517577542734, 1.5485288337581322, 1.551261106376193, 1.4746683855021918, 1.5381704659459325, 1.4571335226719733, 1.525447454019447, 1.5029427651789904, 1.5243001363060178, 1.577597595788127, 1.5191717544070622, 1.420982960688129, 1.4312523829489114, 1.3969210335357602, 1.39914670073622, 1.4002818993379986, 1.482545466036992, 1.5372050601028477, 1.5528493436149569, 1.5140114516495924, 1.6447721693147497, 1.7229081915365834, 1.8206798671892515, 1.8684979957614443, 1.8117945615053768, 1.8467164421056996, 1.7665874328844096, 1.6717664692009304, 1.6612158095972938, 1.5883392115944717, 1.5160528682205467, 1.4834428169833465, 1.5299600363914239, 1.5101102854883421, 1.5548985423425514, 1.497293980574752, 1.5186424593079182, 1.534368904190597, 1.6417566891187936, 1.53357420015678, 1.5147622089779105, 1.5666687126460008, 1.691632299493687, 1.6279439193724945, 1.6465699579651243, 1.601518404904277, 1.5834131190048413, 1.5323577279150715, 1.4976308170383477, 1.5161409487697068, 1.5706658951521741, 1.4507259737790537, 1.4483112877480786], [3.2051208112312706, 1.8023740690624241, 1.6521227760874702, 1.7627251521748495, 1.8555918050930107, 1.891110201984883, 1.8645233927325884, 2.033445130459244, 2.0764506423191142, 2.050449043582391, 1.9798543405529292, 2.0669233089663708, 1.9653579823475391, 2.016460414275721, 2.0529746644465146, 2.0775373558399313, 2.1100190613120566, 2.049810692290987, 1.896722955623355, 1.9255340765728162, 1.8463168500370013, 1.8538324390439018, 1.8552851089956022, 1.9889889173902002, 2.044406430761085, 2.072230209880812, 2.0304166142781153, 2.1946227903490234, 2.349476542541306, 2.5087770171358, 2.7631353729820596, 2.6436264943025103, 2.676007609215087, 2.439627694758448, 2.265796324691421, 2.250252455031167, 2.1210241321233423, 2.022214248876399, 2.023177382496064, 2.0383512872066953, 1.9822760693290118, 2.031039306661551, 2.0343269522404177, 2.067385130741444, 2.061021708440327, 2.224790817240454, 2.1440026745728122, 2.0543771995969617, 2.104746160962222, 2.274251946980718, 2.173175406029208, 2.1936470045724943, 2.129686863053198, 2.1015348491031713, 2.0712208853020138, 1.9619616983820434, 1.9638295835224728, 2.042134242126927, 1.9179649823770575, 1.9161705178410873], [0.4911623657983834, 0.3123660864757127, 0.29649682801359856, 0.3182017420697394, 0.3895580713129653, 0.38484657220729623, 0.3710530880607366, 0.37481328353025034, 0.563434632063667, 0.5547777553530516, 0.4959382307404393, 0.5803511025687246, 0.5645834269185882, 0.5098058187335206, 0.4540859092445583, 0.4144586599575385, 0.4038591172730241, 0.30914497165930716, 0.3003747053499302, 0.3638444691284303, 0.3459829874373239, 0.3256680905537293, 0.33337196379619044, 0.37824303237024537, 0.34626885065364954, 0.3347347768157706, 0.37947682366613267, 0.3348083002593185, 0.37403393133585333, 0.31437543915782273, 0.38916566562955535, 0.3735084975202484, 0.42078409848303894, 0.3997196667599925, 0.40880151750825783, 0.42186631895035304, 0.475267026508647, 0.4351711776607116, 0.44627615550487226, 0.42648179577593925, 0.4122754288713451, 0.32439465710733295, 0.44348150419115057, 0.4208331279113211, 0.509560903837276, 0.41024305788524107, 0.4768713688783581, 0.40498978590078055, 0.4403448069530158, 0.35958924813595605, 0.4654122770820948, 0.49222185566504706, 0.467600652398934, 0.41520565974186024, 0.39166970468450396, 0.3439710549935415, 0.4078103536377306, 0.4507510982331417, 0.44127816079509563, 0.48657742799208353]]</t>
         </is>
       </c>
       <c r="H65" t="n">
-        <v>73.52875971794128</v>
+        <v>73.99226808547974</v>
       </c>
     </row>
     <row r="66">
@@ -2659,7 +2659,7 @@
         <v>20</v>
       </c>
       <c r="C66" t="n">
-        <v>7.000000000000001</v>
+        <v>7</v>
       </c>
       <c r="D66" t="inlineStr">
         <is>
@@ -2682,7 +2682,7 @@
         </is>
       </c>
       <c r="H66" t="n">
-        <v>73.36197757720947</v>
+        <v>73.74384737014771</v>
       </c>
     </row>
     <row r="67">
@@ -2693,7 +2693,7 @@
         <v>20</v>
       </c>
       <c r="C67" t="n">
-        <v>7.000000000000001</v>
+        <v>7</v>
       </c>
       <c r="D67" t="inlineStr">
         <is>
@@ -2716,7 +2716,7 @@
         </is>
       </c>
       <c r="H67" t="n">
-        <v>73.06948566436768</v>
+        <v>73.64032030105591</v>
       </c>
     </row>
     <row r="68">
@@ -2750,7 +2750,7 @@
         </is>
       </c>
       <c r="H68" t="n">
-        <v>85.3400890827179</v>
+        <v>85.4176619052887</v>
       </c>
     </row>
     <row r="69">
@@ -2784,7 +2784,7 @@
         </is>
       </c>
       <c r="H69" t="n">
-        <v>85.4100124835968</v>
+        <v>85.63734030723572</v>
       </c>
     </row>
     <row r="70">
@@ -2818,7 +2818,7 @@
         </is>
       </c>
       <c r="H70" t="n">
-        <v>85.38838982582092</v>
+        <v>85.4602382183075</v>
       </c>
     </row>
     <row r="71">
@@ -2852,7 +2852,7 @@
         </is>
       </c>
       <c r="H71" t="n">
-        <v>322.7276933193207</v>
+        <v>321.6660017967224</v>
       </c>
     </row>
     <row r="72">
@@ -2886,7 +2886,7 @@
         </is>
       </c>
       <c r="H72" t="n">
-        <v>322.4345486164093</v>
+        <v>328.910578250885</v>
       </c>
     </row>
     <row r="73">
@@ -2920,7 +2920,7 @@
         </is>
       </c>
       <c r="H73" t="n">
-        <v>321.2871990203857</v>
+        <v>323.2202525138855</v>
       </c>
     </row>
     <row r="74">
@@ -2954,7 +2954,7 @@
         </is>
       </c>
       <c r="H74" t="n">
-        <v>68.93726801872253</v>
+        <v>69.53727650642395</v>
       </c>
     </row>
     <row r="75">
@@ -2988,7 +2988,7 @@
         </is>
       </c>
       <c r="H75" t="n">
-        <v>68.82413864135742</v>
+        <v>69.32086062431335</v>
       </c>
     </row>
     <row r="76">
@@ -3022,7 +3022,7 @@
         </is>
       </c>
       <c r="H76" t="n">
-        <v>69.69074535369873</v>
+        <v>69.36438083648682</v>
       </c>
     </row>
     <row r="77">
@@ -3033,7 +3033,7 @@
         <v>40</v>
       </c>
       <c r="C77" t="n">
-        <v>7.000000000000001</v>
+        <v>7</v>
       </c>
       <c r="D77" t="inlineStr">
         <is>
@@ -3056,7 +3056,7 @@
         </is>
       </c>
       <c r="H77" t="n">
-        <v>73.19892191886902</v>
+        <v>74.07844758033752</v>
       </c>
     </row>
     <row r="78">
@@ -3067,7 +3067,7 @@
         <v>40</v>
       </c>
       <c r="C78" t="n">
-        <v>7.000000000000001</v>
+        <v>7</v>
       </c>
       <c r="D78" t="inlineStr">
         <is>
@@ -3090,7 +3090,7 @@
         </is>
       </c>
       <c r="H78" t="n">
-        <v>73.4719717502594</v>
+        <v>73.71294569969177</v>
       </c>
     </row>
     <row r="79">
@@ -3101,7 +3101,7 @@
         <v>40</v>
       </c>
       <c r="C79" t="n">
-        <v>7.000000000000001</v>
+        <v>7</v>
       </c>
       <c r="D79" t="inlineStr">
         <is>
@@ -3124,7 +3124,7 @@
         </is>
       </c>
       <c r="H79" t="n">
-        <v>74.06203699111938</v>
+        <v>73.60500979423523</v>
       </c>
     </row>
     <row r="80">
@@ -3158,7 +3158,7 @@
         </is>
       </c>
       <c r="H80" t="n">
-        <v>85.88542580604553</v>
+        <v>85.76493382453918</v>
       </c>
     </row>
     <row r="81">
@@ -3192,7 +3192,7 @@
         </is>
       </c>
       <c r="H81" t="n">
-        <v>85.48436832427979</v>
+        <v>85.60334944725037</v>
       </c>
     </row>
     <row r="82">
@@ -3226,7 +3226,7 @@
         </is>
       </c>
       <c r="H82" t="n">
-        <v>86.089688539505</v>
+        <v>85.7223494052887</v>
       </c>
     </row>
     <row r="83">
@@ -3260,7 +3260,7 @@
         </is>
       </c>
       <c r="H83" t="n">
-        <v>334.3793883323669</v>
+        <v>319.9351830482483</v>
       </c>
     </row>
     <row r="84">
@@ -3294,7 +3294,7 @@
         </is>
       </c>
       <c r="H84" t="n">
-        <v>329.9834558963776</v>
+        <v>323.5873582363129</v>
       </c>
     </row>
     <row r="85">
@@ -3319,16 +3319,16 @@
       </c>
       <c r="F85" t="inlineStr">
         <is>
-          <t>[[4.558521, 1.6304177, 1.6363814, 1.8194377, 1.9371938, 2.1276674, 2.0963204, 2.217282, 2.1279304, 2.2473245, 2.0759206, 2.0740566, 2.053338, 2.2530608, 2.3042603, 2.2255123, 2.1396759, 2.122911, 2.0586896, 2.1882398, 2.025631, 2.2009585, 2.1537595, 2.200606, 2.2633767, 2.312641, 2.3181562, 2.4078188, 2.378495, 2.498787, 2.4422472, 2.348287, 2.2980895, 2.276669, 2.2394922, 2.4329336, 2.2796707, 2.3244843, 2.368407, 2.289595, 2.116624, 2.250095, 2.2068608, 2.196578, 2.1639678, 2.1913779, 2.2014065, 2.1550121, 2.1705918, 2.2250988, 2.2839782, 2.2495697, 2.240866, 2.266288, 2.1440492, 2.173503, 2.1183052, 2.1797988, 2.13253, 2.206891], [6.130451501146564, 2.1117045784156137, 2.1231369378464837, 2.3539195873491634, 2.5027456465208764, 2.7898624245417323, 2.772593281090801, 2.968749678762318, 2.758192689965302, 2.9113863604571546, 2.653943485316595, 2.6693838898821767, 2.681668630788529, 2.957236037224354, 2.9978378769782577, 2.872021334534357, 2.7639954502217323, 2.784161105005288, 2.674096327399761, 2.854584897624196, 2.60662001949371, 2.845681006477184, 2.8094627086624135, 2.821972556555934, 2.947918374068953, 3.044294310980408, 2.9880130024107463, 3.1348584122755287, 3.042649532708958, 3.2059043177404463, 3.111552640449708, 3.018388973785571, 2.9316882816433774, 2.9004360002763754, 2.8777631666810004, 3.1759809405429973, 2.9326578366729916, 2.9692763012617847, 3.0121775474348302, 2.9301047879902717, 2.714203464007583, 2.934306742531383, 2.8660640334478296, 2.8787382949014706, 2.828867440746288, 2.8015107677170406, 2.8055294547634695, 2.7679080483813823, 2.763771168572953, 2.8391508702752253, 2.9094088215403717, 2.9230752203623642, 2.9160632099579415, 2.9599746306079675, 2.817836361348611, 2.858693359507775, 2.749741628820525, 2.8138947313488023, 2.78907275799059, 2.856225619222479], [90275590000000.0, 44423962000000.0, 44500123000000.0, 37328156000000.0, 41573048000000.0, 40439894000000.0, 5987.7275, 6458.797, 42961484000000.0, 6728.819, 52092895000000.0, 45655293000000.0, 63857523000000.0, 61171590000000.0, 36511040000000.0, 64317957000000.0, 5548.7686, 42920430000000.0, 47544537000000.0, 57371740000000.0, 45279870000000.0, 56620965000000.0, 50891986000000.0, 6210.3477, 6452.974, 67766824000000.0, 36557625000000.0, 39859580000000.0, 52267797000000.0, 49112440000000.0, 54357597000000.0, 51280250000000.0, 53985700000000.0, 69530546000000.0, 60533850000000.0, 47336013000000.0, 43704136000000.0, 57448887000000.0, 54794585000000.0, 60736387000000.0, 5232.749, 59137090000000.0, 35585394000000.0, 6923.136, 43465450000000.0, 49927690000000.0, 40952390000000.0, 40144652000000.0, 53428122000000.0, 44620067000000.0, 4740.598, 37405270000000.0, 49158375000000.0, 35846870000000.0, 48601190000000.0, 44784173000000.0, 41216637000000.0, 50861210000000.0, 4692.7197, 68377846000000.0]]</t>
+          <t>[[4.558521, 1.6304177, 1.6363814, 1.8194526, 1.9324026, 2.1096175, 2.071026, 2.1929166, 2.1235886, 2.2549791, 2.0728972, 2.08316, 2.043092, 2.2228208, 2.2971227, 2.2266438, 2.121589, 2.1221814, 2.033617, 2.1919835, 2.0073473, 2.186947, 2.1422646, 2.202098, 2.261195, 2.3152945, 2.3416557, 2.4332612, 2.4073403, 2.5131545, 2.4462423, 2.3400216, 2.2655516, 2.2736523, 2.2253983, 2.4191806, 2.256983, 2.3104632, 2.356329, 2.2860062, 2.107324, 2.2413957, 2.2149189, 2.1968055, 2.1484668, 2.1847448, 2.1918774, 2.1506088, 2.1706588, 2.2111943, 2.2820973, 2.2402651, 2.2234738, 2.2607605, 2.144056, 2.2022355, 2.1560044, 2.193702, 2.141809, 2.1889882], [6.130451501146564, 2.1117045784156137, 2.1231369378464837, 2.353951188300092, 2.4967445158015384, 2.765002250601489, 2.7410074939256535, 2.9403656313078423, 2.7604713482509036, 2.9189448224217553, 2.6566001212553894, 2.681020599724336, 2.654217649376409, 2.9129461446092755, 2.9824642435697974, 2.8642752926823407, 2.7555890075727922, 2.773742057304133, 2.6446410569083385, 2.8708020950928423, 2.5966017339453087, 2.8502808081169175, 2.800687439862439, 2.83007980988994, 2.945426958931073, 3.045305835918183, 3.0361648513708386, 3.183346154817921, 3.1094252999229264, 3.2309296912215064, 3.11906235225835, 3.002972878246307, 2.8914600712596683, 2.8995341156940593, 2.8637708216775652, 3.1592771913083215, 2.905039873752307, 2.955570883300859, 3.0066170831159833, 2.933779694090378, 2.700452861954352, 2.9211522804797343, 2.858380754557535, 2.8725793018466783, 2.795671171970754, 2.7839925723853725, 2.785707223974087, 2.7623941979493987, 2.7606427849820037, 2.821746292643115, 2.9069139275971856, 2.921910086844396, 2.885955172713383, 2.954746668973098, 2.825774085067681, 2.9117974281172336, 2.7924238193540307, 2.8304720249730915, 2.788508683471402, 2.8169486572440094], [90275590000000.0, 44423962000000.0, 44500123000000.0, 37327108000000.0, 41247243000000.0, 39088400000000.0, 5901.7783, 6377.605, 40900567000000.0, 6760.2695, 51652410000000.0, 46074870000000.0, 64361515000000.0, 60108315000000.0, 36732704000000.0, 64577140000000.0, 5485.638, 41362427000000.0, 47803796000000.0, 57333550000000.0, 43200933000000.0, 57895220000000.0, 51204554000000.0, 6138.94, 6645.9453, 66793075000000.0, 35728164000000.0, 37970145000000.0, 55902850000000.0, 49881410000000.0, 56051730000000.0, 50983413000000.0, 52415830000000.0, 70854654000000.0, 60935240000000.0, 45840500000000.0, 42847270000000.0, 58028460000000.0, 55523332000000.0, 59714990000000.0, 5245.8994, 60032817000000.0, 36066598000000.0, 7114.9785, 42762594000000.0, 48643670000000.0, 39972070000000.0, 39434565000000.0, 53261432000000.0, 47499960000000.0, 4691.8564, 38909860000000.0, 48245480000000.0, 35317260000000.0, 46848463000000.0, 45069480000000.0, 42845200000000.0, 51704480000000.0, 4807.2686, 69666043000000.0]]</t>
         </is>
       </c>
       <c r="G85" t="inlineStr">
         <is>
-          <t>[[0.3535994579988184, 0.7241359899341901, 1.1167281672514444, 1.3574175252797587, 1.5108460573620848, 1.5536126994267534, 1.6070500236846765, 1.6248532168007614, 1.6210156930856343, 1.6562147367608862, 1.5712344291554476, 1.573487012664082, 1.6092802640637207, 1.6738502925872378, 1.7255722547811752, 1.6895740012716043, 1.6633334885186284, 1.5949699198332528, 1.5689950453480057, 1.6268247135788434, 1.5801361820887987, 1.6207922709053355, 1.6308578621712981, 1.7028963922085254, 1.7781325923204216, 1.6862477858815221, 1.779217158060606, 1.8214181797166165, 1.8662700586526035, 1.7826396263151367, 1.8612760555089805, 1.7826399167480895, 1.7754327706229596, 1.7033275522039086, 1.7577000446029734, 1.8309614545210011, 1.773532230970919, 1.7360740438026623, 1.8190349385179196, 1.7356084010249007, 1.6549977093590649, 1.67581864860889, 1.6974055207957497, 1.692658866245203, 1.7289280151661297, 1.6894559582579154, 1.692982877590144, 1.658253661341723, 1.7268241353420168, 1.684780229483152, 1.8069533379311713, 1.7332358949093787, 1.7425504582165026, 1.7142143056506671, 1.6833316409319412, 1.6415378022416567, 1.6649047152587009, 1.6129830260864366, 1.6513805930876007, 1.6430309233531066], [0.6744606173121641, 1.051782822715275, 1.4683284385850066, 1.7561059730009008, 1.9523417172317221, 1.9923581340460739, 2.104301496633524, 2.10059437857737, 2.082665876770174, 2.1221550584096316, 2.022491257562753, 2.0192674049880286, 2.0810742926514654, 2.1700438082501576, 2.2417429478991004, 2.190066443612987, 2.1531013871017533, 2.08939509306804, 2.0164821221170524, 2.106565708416101, 2.0204554579501472, 2.089172684862626, 2.128723921122484, 2.198960610503345, 2.314023730113284, 2.19782757135707, 2.293818461304613, 2.3594261333818953, 2.395284957488434, 2.2800338253450074, 2.358504412270075, 2.289230595863587, 2.272108907219146, 2.1675363406101193, 2.25519017988251, 2.358056462859518, 2.2594746366799527, 2.2206571427239243, 2.3328158896136255, 2.210328258909105, 2.1271421477903756, 2.170512328093144, 2.178940975967256, 2.207072676037736, 2.2188845931884336, 2.1538954161615287, 2.15935933148881, 2.1330808909247816, 2.190426007310975, 2.144618036855365, 2.2980193797506887, 2.240773715370123, 2.256776810757492, 2.210525145847985, 2.1911067772551998, 2.135441598452439, 2.15061169889406, 2.078042111801517, 2.1530643104291163, 2.109594014524987], [8811595942570.566, 20048872249455.773, 30621828059473.992, 27972589718619.344, 32495137810859.36, 29138492662238.137, 4747.547090438417, 4893.856598711544, 33200107652718.324, 5047.999132731415, 39332667240972.47, 33531207948371.824, 51728226067430.41, 45110178847053.445, 28600739564548.566, 49461152671656.234, 4414.035094066067, 35361770414529.83, 40748258645804.086, 43894713175107.19, 34688369406181.785, 41178096953793.51, 42234886464324.35, 4901.831599892989, 5256.22722256234, 47423380322628.75, 28567247696164.73, 30737327828141.36, 41080353506830.69, 36917084414550.24, 43636757900441.164, 40360882645213.82, 42861845606111.516, 54154939101493.78, 47225086378746.66, 38906734451975.12, 34429059560024.406, 46340255584071.59, 42547357199396.664, 44643046507012.195, 4279.937280635689, 44790727450532.93, 25855592144709.55, 5400.474453419004, 35492342766914.32, 40843786666356.19, 32665028800652.86, 33034252195611.555, 41773100633144.016, 32719223978801.047, 4068.639417351103, 30079633253303.5, 40230068611105.14, 29023982940552.86, 39880817140094.586, 35458871980176.15, 30994622056255.8, 38011032923202.79, 3703.6528790610996, 52261216354758.234]]</t>
+          <t>[[0.3535994579988184, 0.7241359899341901, 1.1167281672514444, 1.3393310710540856, 1.4935996079324378, 1.533192496875885, 1.5775917954284493, 1.601036956913702, 1.6242703352750065, 1.653586813137214, 1.5686207157211627, 1.558953570886079, 1.6022368414910804, 1.6518619167216677, 1.7145693760033083, 1.6612902968107461, 1.662511201843334, 1.577932043635463, 1.586130461672835, 1.6307082649768434, 1.569652569152412, 1.6033910384954053, 1.6376630016548457, 1.6792954921006027, 1.768167003892265, 1.700700918000164, 1.800541999195135, 1.824527846929561, 1.866826925693978, 1.8160975633862266, 1.8530143580427505, 1.748715132562793, 1.741431073760882, 1.6888573217410359, 1.7531038666057146, 1.804442213714998, 1.7495669876858477, 1.7276298908642542, 1.821995921166895, 1.7212925886755315, 1.6446566024697908, 1.6815066151583256, 1.713649518450761, 1.6647563807123118, 1.7008447677113276, 1.6708075591232385, 1.674684193678587, 1.6479179276832558, 1.7112889397545792, 1.6797581885358, 1.7871664215538798, 1.688495846897512, 1.7397751449652068, 1.689806150615679, 1.6958436285783145, 1.651650336814322, 1.677781416525102, 1.619037474465925, 1.6162726574859758, 1.6094207284634257], [0.6744606173121641, 1.051782822715275, 1.4683284385850066, 1.7342206104205393, 1.9317855580985754, 1.968010654366295, 2.0673067176650566, 2.080688779021054, 2.0882830888794786, 2.1118823545170238, 2.019562469555296, 2.0065930575074873, 2.065716404709577, 2.143653396097656, 2.2153537765980515, 2.144185953517513, 2.139767739521201, 2.0546787265248465, 2.034187002051052, 2.127588392065368, 2.0283510331853565, 2.080795747815717, 2.136945950378888, 2.1712678879926846, 2.298205233341238, 2.235891519563252, 2.3393187774880864, 2.3805845102107783, 2.4185062982145973, 2.3164160288226943, 2.357938415796496, 2.243514252901192, 2.2279788744220483, 2.152746989495866, 2.257271176376858, 2.3306429241345774, 2.243913402085742, 2.214415799069278, 2.3390437629360585, 2.2127094085692383, 2.1168702129774823, 2.1748508187821556, 2.1844221945141764, 2.1786420581429127, 2.1773611874830645, 2.1288203246382076, 2.134800131405384, 2.1181120784454777, 2.1646806912458927, 2.1321661670453778, 2.2767888945354295, 2.190883769982281, 2.249753542186557, 2.192845129940631, 2.2310571888066146, 2.1527886300810195, 2.1531426209607716, 2.0638906016668765, 2.0997975693392807, 2.0595289476862], [8811595942570.566, 20048872249455.773, 30621828059473.992, 27857823837547.87, 31549578075794.89, 26745950832367.617, 4685.028368682312, 4838.283695907288, 32294514035521.18, 4884.698375921011, 37572990185117.27, 32154372642011.83, 51791168734641.59, 45647822124936.625, 28442984863861.316, 49415981327717.92, 4409.113582878713, 32018285571198.17, 41541026269001.945, 44722916446269.664, 34048317562309.44, 42224916344798.88, 41850081056601.555, 4769.186778058793, 5376.055309544731, 44769507522405.94, 27722257881240.973, 28985216594222.965, 43830970670460.664, 39981636524620.164, 43027338954665.37, 38680858122434.555, 41887424488273.42, 56801468652366.63, 49607242950623.625, 36814075754752.625, 34631230219790.395, 46660489594024.79, 42966630717424.016, 43911378901657.32, 4259.167369030829, 48696580937377.33, 26357530156168.723, 5300.806370885347, 34926317311772.82, 38268103363235.586, 30649323306112.61, 32767444109543.465, 39467581701668.07, 32534338014873.25, 3928.4101575032405, 30865003721264.38, 39893924294584.31, 28889623820287.14, 40671686737029.88, 34169780963829.746, 32888451922196.434, 37968122638797.086, 3805.3682928039775, 52302025922544.95]]</t>
         </is>
       </c>
       <c r="H85" t="n">
-        <v>326.7849879264832</v>
+        <v>320.5623655319214</v>
       </c>
     </row>
     <row r="86">
@@ -3362,7 +3362,7 @@
         </is>
       </c>
       <c r="H86" t="n">
-        <v>69.92344999313354</v>
+        <v>71.5664005279541</v>
       </c>
     </row>
     <row r="87">
@@ -3396,7 +3396,7 @@
         </is>
       </c>
       <c r="H87" t="n">
-        <v>70.02119255065918</v>
+        <v>70.50922012329102</v>
       </c>
     </row>
     <row r="88">
@@ -3430,7 +3430,7 @@
         </is>
       </c>
       <c r="H88" t="n">
-        <v>69.48956418037415</v>
+        <v>70.98592162132263</v>
       </c>
     </row>
     <row r="89">
@@ -3441,7 +3441,7 @@
         <v>60</v>
       </c>
       <c r="C89" t="n">
-        <v>7.000000000000001</v>
+        <v>7</v>
       </c>
       <c r="D89" t="inlineStr">
         <is>
@@ -3464,7 +3464,7 @@
         </is>
       </c>
       <c r="H89" t="n">
-        <v>73.93929052352905</v>
+        <v>74.64642286300659</v>
       </c>
     </row>
     <row r="90">
@@ -3475,7 +3475,7 @@
         <v>60</v>
       </c>
       <c r="C90" t="n">
-        <v>7.000000000000001</v>
+        <v>7</v>
       </c>
       <c r="D90" t="inlineStr">
         <is>
@@ -3498,7 +3498,7 @@
         </is>
       </c>
       <c r="H90" t="n">
-        <v>73.53656673431396</v>
+        <v>74.88768815994263</v>
       </c>
     </row>
     <row r="91">
@@ -3509,7 +3509,7 @@
         <v>60</v>
       </c>
       <c r="C91" t="n">
-        <v>7.000000000000001</v>
+        <v>7</v>
       </c>
       <c r="D91" t="inlineStr">
         <is>
@@ -3532,7 +3532,7 @@
         </is>
       </c>
       <c r="H91" t="n">
-        <v>73.61027693748474</v>
+        <v>74.57135415077209</v>
       </c>
     </row>
     <row r="92">
@@ -3566,7 +3566,7 @@
         </is>
       </c>
       <c r="H92" t="n">
-        <v>85.84422039985657</v>
+        <v>86.65659713745117</v>
       </c>
     </row>
     <row r="93">
@@ -3600,7 +3600,7 @@
         </is>
       </c>
       <c r="H93" t="n">
-        <v>85.89660263061523</v>
+        <v>86.5163586139679</v>
       </c>
     </row>
     <row r="94">
@@ -3634,7 +3634,7 @@
         </is>
       </c>
       <c r="H94" t="n">
-        <v>85.76026344299316</v>
+        <v>86.46704959869385</v>
       </c>
     </row>
     <row r="95">
@@ -3668,7 +3668,7 @@
         </is>
       </c>
       <c r="H95" t="n">
-        <v>328.4584407806396</v>
+        <v>322.7815232276917</v>
       </c>
     </row>
     <row r="96">
@@ -3702,7 +3702,7 @@
         </is>
       </c>
       <c r="H96" t="n">
-        <v>328.5216827392578</v>
+        <v>323.3651471138</v>
       </c>
     </row>
     <row r="97">
@@ -3736,7 +3736,7 @@
         </is>
       </c>
       <c r="H97" t="n">
-        <v>328.2876949310303</v>
+        <v>322.2067997455597</v>
       </c>
     </row>
     <row r="98">
@@ -3770,7 +3770,7 @@
         </is>
       </c>
       <c r="H98" t="n">
-        <v>69.77376747131348</v>
+        <v>70.95067596435547</v>
       </c>
     </row>
     <row r="99">
@@ -3804,7 +3804,7 @@
         </is>
       </c>
       <c r="H99" t="n">
-        <v>69.97797799110413</v>
+        <v>70.94309854507446</v>
       </c>
     </row>
     <row r="100">
@@ -3838,7 +3838,7 @@
         </is>
       </c>
       <c r="H100" t="n">
-        <v>69.5993709564209</v>
+        <v>70.64625859260559</v>
       </c>
     </row>
     <row r="101">
@@ -3849,7 +3849,7 @@
         <v>80</v>
       </c>
       <c r="C101" t="n">
-        <v>7.000000000000001</v>
+        <v>7</v>
       </c>
       <c r="D101" t="inlineStr">
         <is>
@@ -3872,7 +3872,7 @@
         </is>
       </c>
       <c r="H101" t="n">
-        <v>73.83445739746094</v>
+        <v>75.25896239280701</v>
       </c>
     </row>
     <row r="102">
@@ -3883,7 +3883,7 @@
         <v>80</v>
       </c>
       <c r="C102" t="n">
-        <v>7.000000000000001</v>
+        <v>7</v>
       </c>
       <c r="D102" t="inlineStr">
         <is>
@@ -3906,7 +3906,7 @@
         </is>
       </c>
       <c r="H102" t="n">
-        <v>74.00452184677124</v>
+        <v>74.94765663146973</v>
       </c>
     </row>
     <row r="103">
@@ -3917,7 +3917,7 @@
         <v>80</v>
       </c>
       <c r="C103" t="n">
-        <v>7.000000000000001</v>
+        <v>7</v>
       </c>
       <c r="D103" t="inlineStr">
         <is>
@@ -3940,7 +3940,7 @@
         </is>
       </c>
       <c r="H103" t="n">
-        <v>75.14914584159851</v>
+        <v>75.00066637992859</v>
       </c>
     </row>
     <row r="104">
@@ -3965,16 +3965,16 @@
       </c>
       <c r="F104" t="inlineStr">
         <is>
-          <t>[[5.0775547, 1.3816898, 1.266952, 1.4809926, 1.4268498, 1.4857769, 1.4603847, 1.6424154, 1.5859302, 1.608431, 1.5284894, 1.602404, 1.444843, 1.5467522, 1.5191765, 1.570859, 1.4867383, 1.4446917, 1.4073362, 1.4616935, 1.3878778, 1.4681007, 1.497864, 1.6091415, 1.5546044, 1.5870242, 1.5688331, 1.7728091, 1.7509896, 1.8354017, 1.9065145, 1.9413797, 1.8336607, 1.7705711, 1.7324016, 1.7676427, 1.5936255, 1.4828378, 1.518908, 1.6118965, 1.5180274, 1.6092825, 1.5382291, 1.6157383, 1.5247275, 1.6566777, 1.5836548, 1.6162288, 1.5581651, 1.6960304, 1.6338896, 1.6605076, 1.5609148, 1.5765324, 1.5467384, 1.5790114, 1.5093542, 1.5955312, 1.4912374, 1.5171933], [7.11506710018169, 2.0058069565859578, 1.7394655458086952, 1.9681866763285432, 1.8749842325183386, 1.9276280088753084, 1.9415902678012757, 2.196142616664663, 2.10763478021223, 2.1160063316812954, 2.0495840301895067, 2.158984123217542, 1.938164812286187, 2.0372377613021606, 2.079823767642216, 2.137782862278969, 1.984665616599102, 1.917087018178665, 1.896137115397561, 1.9770587403751252, 1.8441905125821458, 1.9255491662376505, 1.9991180740414887, 2.161330278272468, 2.069980695514687, 2.0892509974575093, 2.1261498201464404, 2.389096937311838, 2.387127680482811, 2.492572144867503, 2.7411072605750126, 2.7739583990364673, 2.638447331969672, 2.4421700953511993, 2.4105475554761235, 2.4260759896361477, 2.174249243239725, 2.0020810267831757, 2.0683743599699156, 2.166406677003936, 2.017417642833946, 2.116073596900349, 2.098276852773487, 2.2674398585443183, 2.092834842010673, 2.2570666496904828, 2.193650998220968, 2.1584172069301992, 2.087496057381019, 2.2706402221135846, 2.1909401137761204, 2.2159942921795652, 2.101838614891571, 2.086031222291741, 2.0881791660347706, 2.057919009847698, 1.9769954282662416, 2.0838042934875456, 1.9988428583099764, 2.0062099844961616], [1.8978608, 0.4802366, 0.33833516, 0.35349253, 0.39147466, 0.38867867, 0.37305018, 0.39232773, 0.5517716, 0.5598215, 0.49096447, 0.5697027, 0.5114362, 0.5183512, 0.45822942, 0.4161049, 0.38738, 0.29856476, 0.3090317, 0.37069783, 0.35392234, 0.33015454, 0.361544, 0.42824653, 0.36033714, 0.33722654, 0.3960973, 0.35434666, 0.40782884, 0.32438117, 0.40154204, 0.41709715, 0.4606195, 0.44926372, 0.44635502, 0.47317296, 0.5456228, 0.43855307, 0.48204952, 0.4397356, 0.4150295, 0.32037422, 0.46064124, 0.44744974, 0.49510255, 0.40559384, 0.48717222, 0.42933354, 0.4314828, 0.3493134, 0.4763481, 0.49165806, 0.44549444, 0.42295906, 0.4118086, 0.37670484, 0.3898529, 0.48949108, 0.46433634, 0.53061473]]</t>
+          <t>[[5.0775547, 1.3816898, 1.266952, 1.4810557, 1.4275322, 1.4888501, 1.4551619, 1.6321778, 1.573013, 1.6122149, 1.5338364, 1.6105974, 1.4615086, 1.5648838, 1.5258952, 1.5686481, 1.490435, 1.4628294, 1.4267669, 1.4787534, 1.3861462, 1.4517504, 1.4940305, 1.6007636, 1.5479052, 1.585392, 1.5761076, 1.7728716, 1.734475, 1.8237494, 1.8758662, 1.91597, 1.8306946, 1.7665589, 1.7090662, 1.768115, 1.6281551, 1.5358515, 1.5622195, 1.6395147, 1.5319688, 1.6102877, 1.5417738, 1.598533, 1.5016388, 1.6357598, 1.5546318, 1.593397, 1.5556582, 1.6895928, 1.6246495, 1.6660663, 1.5677607, 1.5804527, 1.5590006, 1.5921731, 1.5352445, 1.6220465, 1.5144024, 1.5259824], [7.11506710018169, 2.0058069565859578, 1.7394655458086952, 1.9682537846179393, 1.8751202862621001, 1.9301990649485792, 1.9366160191245412, 2.186445145357465, 2.101065878349557, 2.1307148102026683, 2.0651513599777425, 2.180198691526461, 1.965037099376411, 2.0629297444542796, 2.0839860910767887, 2.125818095085931, 1.9850374452724844, 1.942809796858354, 1.925500876423278, 1.996646035787809, 1.837269401353382, 1.9081327177429557, 1.9917994700996773, 2.1553763126076606, 2.0571412494251993, 2.092148353261705, 2.1372285057001728, 2.3799089595468144, 2.3296561102796023, 2.440909129075437, 2.6783803526528045, 2.725825169068156, 2.629024871371892, 2.419991825499797, 2.352872565966127, 2.40517728600193, 2.2062936276020717, 2.058717669642523, 2.131678129358717, 2.202913855857588, 2.0313707755936115, 2.1179889133440573, 2.0934043712873187, 2.233699136164515, 2.0653671219099525, 2.22956854029081, 2.164115712306914, 2.129142874070302, 2.083936324276175, 2.271944375008672, 2.1840299058131243, 2.2259201461713194, 2.120427878943546, 2.09714381034179, 2.111414961392164, 2.0870767404131394, 2.0098448683053425, 2.118259622995684, 2.032633501011034, 2.0140709615667265], [1.8978608, 0.4802366, 0.33833516, 0.35351124, 0.3937338, 0.39305583, 0.37301794, 0.39403284, 0.55582005, 0.57342833, 0.50292516, 0.5830607, 0.5278153, 0.53061867, 0.46297893, 0.43089157, 0.38014758, 0.29331502, 0.30804133, 0.37308598, 0.3537074, 0.33330935, 0.362967, 0.4204943, 0.35600078, 0.3421125, 0.40190837, 0.36820197, 0.4042017, 0.32509544, 0.39501694, 0.41065848, 0.46855012, 0.45022523, 0.44278127, 0.46900263, 0.5494208, 0.4511112, 0.49358374, 0.45251647, 0.4265314, 0.324206, 0.46083456, 0.45000404, 0.5007085, 0.39447954, 0.47197014, 0.4170339, 0.43170142, 0.35114896, 0.48002073, 0.49456045, 0.45259073, 0.42494604, 0.42178276, 0.38932714, 0.39894742, 0.50125027, 0.4767392, 0.5343618]]</t>
         </is>
       </c>
       <c r="G104" t="inlineStr">
         <is>
-          <t>[[1.1829127856212451, 0.8675676856843174, 1.006468613882435, 1.1740301618306819, 1.2472817361134687, 1.2709233954036132, 1.2541380995887392, 1.363997898467669, 1.3874565135847141, 1.3785229591523431, 1.2871071053588776, 1.3152637117102048, 1.273753603740513, 1.309983359036101, 1.2671783519257447, 1.275079220553743, 1.2874615134656164, 1.2382793316673053, 1.1887522688507632, 1.218838224652377, 1.2370170899069812, 1.2388824031125718, 1.2612990889095963, 1.3252787183632018, 1.3524747868650449, 1.3124740080928057, 1.3170937140223744, 1.440237208646221, 1.4897942276100282, 1.5547703383274432, 1.5960772901077611, 1.5546276843425322, 1.5824586342927518, 1.4791091951637991, 1.4267977625601382, 1.4347272134419737, 1.3863609239034849, 1.2750236886535102, 1.293905077465968, 1.3517775035085022, 1.342472404388448, 1.3453800665219509, 1.312480549560522, 1.3330012595455742, 1.3284133047612168, 1.4193786377089919, 1.3419947452266268, 1.3238872458213011, 1.3562594611189407, 1.4229958513984853, 1.3619349372977683, 1.3724681607725566, 1.358958089999045, 1.3541548519792865, 1.3164339335483155, 1.3059910094628127, 1.330810078243161, 1.3602121783670922, 1.2702371539460482, 1.2666590857647206], [1.9446756626834742, 1.2274242694090873, 1.3770429480948994, 1.5439389521996494, 1.6230701720336191, 1.6492179850342543, 1.6526935974173624, 1.8079737654400982, 1.827463622196292, 1.804482413445711, 1.7189914685372478, 1.7590599097836384, 1.69169522639691, 1.7357604857066773, 1.7050761869609643, 1.695977787923355, 1.6927180172499545, 1.639224641662958, 1.5896846412113772, 1.6157973848495448, 1.630757790999835, 1.6222913276066622, 1.665313255942444, 1.758709981312235, 1.7705118842587064, 1.6971206974630417, 1.7507743054476783, 1.9078778954417952, 1.9755711927746735, 2.0968743310519913, 2.302734397885071, 2.2255380236329674, 2.279934655007702, 2.053503442664044, 1.9181439723504572, 1.933187257837857, 1.8486449519440482, 1.7011797121020045, 1.7430676018822366, 1.795044892269487, 1.7766936315823616, 1.7589685505660548, 1.7839933300437703, 1.838529899090074, 1.794403805870954, 1.9199702332274968, 1.8292577033491377, 1.7634011063930621, 1.7949315044323828, 1.9039701399895013, 1.8131410853049674, 1.813795500968331, 1.785793866531351, 1.7856242379735097, 1.7655556332777929, 1.7170995403392018, 1.7190585664025244, 1.7738166716494437, 1.6823701302123437, 1.6655162482250883], [0.328129796654603, 0.23912549321911172, 0.2582760565197023, 0.2939150978353112, 0.3418816928234229, 0.3365250676353337, 0.3210087895971301, 0.32587524473513363, 0.46409736203526325, 0.45326146211837376, 0.4078525117243803, 0.45636267540566716, 0.4435908451062964, 0.4352166022258761, 0.37804273439180036, 0.3388340119066284, 0.31597697637007344, 0.25331532266335255, 0.25534600268204316, 0.30731148990962764, 0.3148077941320895, 0.28153416940248155, 0.30147935695396305, 0.348961916180674, 0.3050535999968646, 0.276690870822332, 0.3392371277260981, 0.29210489219341523, 0.3408171144058803, 0.27405336536312835, 0.3326970241397696, 0.33731859011168336, 0.39658737920142995, 0.38042537796506737, 0.37719858306057436, 0.37477491597544615, 0.46039352520020466, 0.3658422693013114, 0.3989895814308651, 0.3583458425414766, 0.3549345188379691, 0.2688734317260439, 0.3933501502118864, 0.36357892382802015, 0.42001112073955416, 0.34887506749340774, 0.39903314327869716, 0.34106687030121213, 0.3656806737081235, 0.2810574494686763, 0.37593737356242024, 0.3998572340030409, 0.37120826087957565, 0.3586006953313753, 0.3353085045803118, 0.3071077395466022, 0.33647604523992736, 0.42229853844583026, 0.3877287757537153, 0.41215127282199876]]</t>
+          <t>[[1.1829127856212451, 0.8675676856843174, 1.006468613882435, 1.1770053576206028, 1.254748552388869, 1.2677342314381916, 1.240301739481758, 1.3674970406364122, 1.3863703091485384, 1.3839898466420668, 1.2999512318142827, 1.3412796758623697, 1.292908249713664, 1.3364437593238414, 1.2702686466116888, 1.2910588967547103, 1.3167069986529092, 1.2686657565848256, 1.2105529959481076, 1.2310352773960842, 1.2328371411770658, 1.2420647617554466, 1.2522251698095348, 1.3242162709679213, 1.344818931376851, 1.3163490959662196, 1.3247474065441995, 1.4281456479059682, 1.4865271541380538, 1.545689924374972, 1.5679917066647306, 1.556220299583205, 1.5817217011593734, 1.4753519617410509, 1.419795977409248, 1.4776531628143728, 1.425136604323107, 1.3260645744697406, 1.3249899741567484, 1.3840746050595294, 1.3493589955649241, 1.3432867531976025, 1.3009983892225705, 1.320206650415396, 1.3121426834266097, 1.3867917218086439, 1.3219467439749704, 1.3273377716505284, 1.350362113243319, 1.4236521872934804, 1.362772586493619, 1.3822641086008902, 1.3663379079559006, 1.3607833711322002, 1.3522392439889483, 1.3439457201785303, 1.358450698900882, 1.3913319079523088, 1.2731325444282426, 1.2772270978157687], [1.9446756626834742, 1.2274242694090873, 1.3770429480948994, 1.5456554483241465, 1.6299514267202708, 1.6513952183857976, 1.6443012551725096, 1.8224600921468264, 1.8294804456581935, 1.8182188357979112, 1.7389472418027498, 1.8005619287601868, 1.7219378707413888, 1.7606103784861922, 1.7057484350938603, 1.7205397455337461, 1.739040932912716, 1.683042440896974, 1.6234414280623868, 1.626476513044894, 1.6229140682056982, 1.6308401103658035, 1.6573472723857088, 1.7599129098569481, 1.7645327633289305, 1.7086634760929795, 1.7597558946352443, 1.8761252115359401, 1.9453520359399217, 2.0626448732433995, 2.2307609032744655, 2.215078438941047, 2.2654228204183617, 2.0212566359924797, 1.9086522161592532, 1.9822450557501228, 1.8904361655448234, 1.7685187363348742, 1.787447636142422, 1.8292031700656106, 1.779348780967635, 1.748056849455936, 1.7491290941200852, 1.819484356047309, 1.7697355762537534, 1.8869350651969423, 1.8108131373155174, 1.772085044276211, 1.7911719858487118, 1.9085614262158888, 1.820304439997528, 1.8394836551292117, 1.7979419229880333, 1.8012042516367823, 1.8250795412816625, 1.7779383402881106, 1.758263966304532, 1.8144568010788749, 1.6890817909761469, 1.6732879144115957], [0.328129796654603, 0.23912549321911172, 0.2582760565197023, 0.2982464510200063, 0.3464175245106658, 0.340886785279061, 0.3220527726163438, 0.3382819413026225, 0.4676962335248399, 0.4709844043481882, 0.4187531071822152, 0.4754436762463887, 0.46395371690998427, 0.4418899338211735, 0.38323908013538455, 0.3494870626798406, 0.31815826777249506, 0.2530511480682128, 0.2574560730596146, 0.3175335201437322, 0.3165492673452179, 0.28609920026181246, 0.2964652449882567, 0.3488869120317344, 0.30884588119075024, 0.29000903233930453, 0.3496766776455089, 0.3038207497078524, 0.3440025661328177, 0.2800803671845525, 0.3308680970158229, 0.3420582527345207, 0.39748827408720105, 0.378058255282758, 0.37250772146255007, 0.3890913646783929, 0.47187055359436086, 0.3758244573768861, 0.4165700909501676, 0.373065600504142, 0.36625443829498733, 0.2692071499140852, 0.3898600681048233, 0.36677500040178523, 0.42084966752752856, 0.3364602363111175, 0.3867504675510673, 0.3423845685190725, 0.37231695863143566, 0.2878083159850928, 0.39222695338233987, 0.4027479159491153, 0.38671514168959364, 0.3630695390797492, 0.3540589158665966, 0.32265305560644153, 0.34829612033305574, 0.43088458467466395, 0.38904944982859685, 0.4207385037574948]]</t>
         </is>
       </c>
       <c r="H104" t="n">
-        <v>86.344158411026</v>
+        <v>87.16152811050415</v>
       </c>
     </row>
     <row r="105">
@@ -4008,7 +4008,7 @@
         </is>
       </c>
       <c r="H105" t="n">
-        <v>86.57615280151367</v>
+        <v>87.75206017494202</v>
       </c>
     </row>
     <row r="106">
@@ -4042,7 +4042,7 @@
         </is>
       </c>
       <c r="H106" t="n">
-        <v>86.23919868469238</v>
+        <v>87.02403092384338</v>
       </c>
     </row>
     <row r="107">
@@ -4076,7 +4076,7 @@
         </is>
       </c>
       <c r="H107" t="n">
-        <v>326.8273425102234</v>
+        <v>324.3738660812378</v>
       </c>
     </row>
     <row r="108">
@@ -4110,7 +4110,7 @@
         </is>
       </c>
       <c r="H108" t="n">
-        <v>327.993287563324</v>
+        <v>325.4768600463867</v>
       </c>
     </row>
     <row r="109">
@@ -4144,7 +4144,7 @@
         </is>
       </c>
       <c r="H109" t="n">
-        <v>328.5528566837311</v>
+        <v>324.6317353248596</v>
       </c>
     </row>
     <row r="110">
@@ -4178,7 +4178,7 @@
         </is>
       </c>
       <c r="H110" t="n">
-        <v>69.3266167640686</v>
+        <v>71.85860633850098</v>
       </c>
     </row>
     <row r="111">
@@ -4212,7 +4212,7 @@
         </is>
       </c>
       <c r="H111" t="n">
-        <v>69.48262739181519</v>
+        <v>70.67766189575195</v>
       </c>
     </row>
     <row r="112">
@@ -4246,7 +4246,7 @@
         </is>
       </c>
       <c r="H112" t="n">
-        <v>70.02726459503174</v>
+        <v>70.46662974357605</v>
       </c>
     </row>
     <row r="113">
@@ -4257,7 +4257,7 @@
         <v>100</v>
       </c>
       <c r="C113" t="n">
-        <v>7.000000000000001</v>
+        <v>7</v>
       </c>
       <c r="D113" t="inlineStr">
         <is>
@@ -4280,7 +4280,7 @@
         </is>
       </c>
       <c r="H113" t="n">
-        <v>73.93777894973755</v>
+        <v>74.88792443275452</v>
       </c>
     </row>
     <row r="114">
@@ -4291,7 +4291,7 @@
         <v>100</v>
       </c>
       <c r="C114" t="n">
-        <v>7.000000000000001</v>
+        <v>7</v>
       </c>
       <c r="D114" t="inlineStr">
         <is>
@@ -4314,7 +4314,7 @@
         </is>
       </c>
       <c r="H114" t="n">
-        <v>74.0268702507019</v>
+        <v>75.14762592315674</v>
       </c>
     </row>
     <row r="115">
@@ -4325,7 +4325,7 @@
         <v>100</v>
       </c>
       <c r="C115" t="n">
-        <v>7.000000000000001</v>
+        <v>7</v>
       </c>
       <c r="D115" t="inlineStr">
         <is>
@@ -4348,7 +4348,7 @@
         </is>
       </c>
       <c r="H115" t="n">
-        <v>73.77096152305603</v>
+        <v>74.82279562950134</v>
       </c>
     </row>
     <row r="116">
@@ -4382,7 +4382,7 @@
         </is>
       </c>
       <c r="H116" t="n">
-        <v>86.36158633232117</v>
+        <v>87.46140670776367</v>
       </c>
     </row>
     <row r="117">
@@ -4416,7 +4416,7 @@
         </is>
       </c>
       <c r="H117" t="n">
-        <v>87.08450961112976</v>
+        <v>87.27143049240112</v>
       </c>
     </row>
     <row r="118">
@@ -4450,7 +4450,7 @@
         </is>
       </c>
       <c r="H118" t="n">
-        <v>86.35645961761475</v>
+        <v>87.0214512348175</v>
       </c>
     </row>
     <row r="119">
@@ -4484,7 +4484,7 @@
         </is>
       </c>
       <c r="H119" t="n">
-        <v>327.9380025863647</v>
+        <v>323.5828008651733</v>
       </c>
     </row>
     <row r="120">
@@ -4518,7 +4518,7 @@
         </is>
       </c>
       <c r="H120" t="n">
-        <v>328.6780877113342</v>
+        <v>323.4280455112457</v>
       </c>
     </row>
     <row r="121">
@@ -4552,7 +4552,7 @@
         </is>
       </c>
       <c r="H121" t="n">
-        <v>327.6416070461273</v>
+        <v>326.2665910720825</v>
       </c>
     </row>
     <row r="122">
@@ -4586,7 +4586,7 @@
         </is>
       </c>
       <c r="H122" t="n">
-        <v>70.05331945419312</v>
+        <v>70.79439496994019</v>
       </c>
     </row>
     <row r="123">
@@ -4620,7 +4620,7 @@
         </is>
       </c>
       <c r="H123" t="n">
-        <v>68.74752020835876</v>
+        <v>69.53839921951294</v>
       </c>
     </row>
     <row r="124">
@@ -4654,7 +4654,7 @@
         </is>
       </c>
       <c r="H124" t="n">
-        <v>68.62899374961853</v>
+        <v>69.39174056053162</v>
       </c>
     </row>
     <row r="125">
@@ -4665,7 +4665,7 @@
         <v>20</v>
       </c>
       <c r="C125" t="n">
-        <v>7.000000000000001</v>
+        <v>7</v>
       </c>
       <c r="D125" t="inlineStr">
         <is>
@@ -4688,7 +4688,7 @@
         </is>
       </c>
       <c r="H125" t="n">
-        <v>73.09641408920288</v>
+        <v>73.71901750564575</v>
       </c>
     </row>
     <row r="126">
@@ -4699,7 +4699,7 @@
         <v>20</v>
       </c>
       <c r="C126" t="n">
-        <v>7.000000000000001</v>
+        <v>7</v>
       </c>
       <c r="D126" t="inlineStr">
         <is>
@@ -4722,7 +4722,7 @@
         </is>
       </c>
       <c r="H126" t="n">
-        <v>72.49507308006287</v>
+        <v>73.75569367408752</v>
       </c>
     </row>
     <row r="127">
@@ -4733,7 +4733,7 @@
         <v>20</v>
       </c>
       <c r="C127" t="n">
-        <v>7.000000000000001</v>
+        <v>7</v>
       </c>
       <c r="D127" t="inlineStr">
         <is>
@@ -4756,7 +4756,7 @@
         </is>
       </c>
       <c r="H127" t="n">
-        <v>73.05575561523438</v>
+        <v>73.70232486724854</v>
       </c>
     </row>
     <row r="128">
@@ -4790,7 +4790,7 @@
         </is>
       </c>
       <c r="H128" t="n">
-        <v>84.62871861457825</v>
+        <v>85.63036942481995</v>
       </c>
     </row>
     <row r="129">
@@ -4824,7 +4824,7 @@
         </is>
       </c>
       <c r="H129" t="n">
-        <v>84.71101832389832</v>
+        <v>85.71828150749207</v>
       </c>
     </row>
     <row r="130">
@@ -4858,7 +4858,7 @@
         </is>
       </c>
       <c r="H130" t="n">
-        <v>84.87654662132263</v>
+        <v>85.90883302688599</v>
       </c>
     </row>
     <row r="131">
@@ -4892,7 +4892,7 @@
         </is>
       </c>
       <c r="H131" t="n">
-        <v>325.5631768703461</v>
+        <v>321.3048992156982</v>
       </c>
     </row>
     <row r="132">
@@ -4926,7 +4926,7 @@
         </is>
       </c>
       <c r="H132" t="n">
-        <v>326.658703327179</v>
+        <v>322.0758168697357</v>
       </c>
     </row>
     <row r="133">
@@ -4960,7 +4960,7 @@
         </is>
       </c>
       <c r="H133" t="n">
-        <v>325.2440745830536</v>
+        <v>322.6834032535553</v>
       </c>
     </row>
     <row r="134">
@@ -4994,7 +4994,7 @@
         </is>
       </c>
       <c r="H134" t="n">
-        <v>69.37653946876526</v>
+        <v>69.41958951950073</v>
       </c>
     </row>
     <row r="135">
@@ -5028,7 +5028,7 @@
         </is>
       </c>
       <c r="H135" t="n">
-        <v>68.5999596118927</v>
+        <v>69.59615993499756</v>
       </c>
     </row>
     <row r="136">
@@ -5062,7 +5062,7 @@
         </is>
       </c>
       <c r="H136" t="n">
-        <v>68.55016446113586</v>
+        <v>69.49475526809692</v>
       </c>
     </row>
     <row r="137">
@@ -5073,7 +5073,7 @@
         <v>40</v>
       </c>
       <c r="C137" t="n">
-        <v>7.000000000000001</v>
+        <v>7</v>
       </c>
       <c r="D137" t="inlineStr">
         <is>
@@ -5096,7 +5096,7 @@
         </is>
       </c>
       <c r="H137" t="n">
-        <v>73.13688182830811</v>
+        <v>73.77384424209595</v>
       </c>
     </row>
     <row r="138">
@@ -5107,7 +5107,7 @@
         <v>40</v>
       </c>
       <c r="C138" t="n">
-        <v>7.000000000000001</v>
+        <v>7</v>
       </c>
       <c r="D138" t="inlineStr">
         <is>
@@ -5130,7 +5130,7 @@
         </is>
       </c>
       <c r="H138" t="n">
-        <v>72.79800844192505</v>
+        <v>73.84292387962341</v>
       </c>
     </row>
     <row r="139">
@@ -5141,7 +5141,7 @@
         <v>40</v>
       </c>
       <c r="C139" t="n">
-        <v>7.000000000000001</v>
+        <v>7</v>
       </c>
       <c r="D139" t="inlineStr">
         <is>
@@ -5164,7 +5164,7 @@
         </is>
       </c>
       <c r="H139" t="n">
-        <v>72.94774842262268</v>
+        <v>73.66429591178894</v>
       </c>
     </row>
     <row r="140">
@@ -5198,7 +5198,7 @@
         </is>
       </c>
       <c r="H140" t="n">
-        <v>84.66786217689514</v>
+        <v>86.59467887878418</v>
       </c>
     </row>
     <row r="141">
@@ -5232,7 +5232,7 @@
         </is>
       </c>
       <c r="H141" t="n">
-        <v>85.035231590271</v>
+        <v>86.68570065498352</v>
       </c>
     </row>
     <row r="142">
@@ -5266,7 +5266,7 @@
         </is>
       </c>
       <c r="H142" t="n">
-        <v>84.92612552642822</v>
+        <v>85.76719927787781</v>
       </c>
     </row>
     <row r="143">
@@ -5300,7 +5300,7 @@
         </is>
       </c>
       <c r="H143" t="n">
-        <v>330.2938480377197</v>
+        <v>320.4872658252716</v>
       </c>
     </row>
     <row r="144">
@@ -5334,7 +5334,7 @@
         </is>
       </c>
       <c r="H144" t="n">
-        <v>325.1651771068573</v>
+        <v>321.4845337867737</v>
       </c>
     </row>
     <row r="145">
@@ -5368,7 +5368,7 @@
         </is>
       </c>
       <c r="H145" t="n">
-        <v>325.6153123378754</v>
+        <v>320.924192905426</v>
       </c>
     </row>
     <row r="146">
@@ -5393,16 +5393,16 @@
       </c>
       <c r="F146" t="inlineStr">
         <is>
-          <t>[[5.076458, 1.8790193, 1.4371778, 1.5622207, 1.5483305, 1.5741372, 1.5368236, 1.7346897, 1.6637203, 1.7045819, 1.6169895, 1.704187, 1.5259866, 1.6516889, 1.649271, 1.7070472, 1.6739218, 1.606772, 1.5541703, 1.6002077, 1.4956291, 1.5069813, 1.5557722, 1.6675527, 1.6633117, 1.6551613, 1.6752278, 1.8697453, 1.8850833, 1.994792, 2.0426676, 2.0820765, 1.971409, 1.909542, 1.8608692, 1.9290988, 1.7437029, 1.6904223, 1.7058893, 1.7510344, 1.6401018, 1.6852474, 1.6457442, 1.7366484, 1.6223603, 1.7888938, 1.6917462, 1.7205434, 1.6957127, 1.8557698, 1.8300198, 1.8672817, 1.7685722, 1.7894895, 1.7540642, 1.7188121, 1.6589411, 1.7539129, 1.6711192, 1.6957455], [7.11399312361502, 2.900066565703321, 2.0333498151559355, 2.066775889227941, 2.0564328747160436, 2.0335648477840147, 2.0573364124180284, 2.3240756463626284, 2.2135130637321723, 2.2452039465416416, 2.1904942319750953, 2.304435276518859, 2.072697830789623, 2.184445892187764, 2.2270621826575887, 2.3268769266313707, 2.277584423087489, 2.158410689785433, 2.136317241541234, 2.219799062381515, 2.0325532693674138, 2.00147264622854, 2.0825996124147057, 2.267339859830905, 2.2750869482842666, 2.2129269333475983, 2.300220570146629, 2.5313345812571018, 2.605113312641909, 2.7680245889387405, 2.9480764033485407, 2.9645896269963132, 2.7947864939532407, 2.622475272790286, 2.554257791292782, 2.6383563346446532, 2.3882556218852096, 2.2884340432555206, 2.369902712277789, 2.382404730253987, 2.2114376944610386, 2.23450859043931, 2.2525887961037796, 2.4231560057239756, 2.2317483041012682, 2.466516474283887, 2.390519083706087, 2.3360449724767367, 2.2773886622192823, 2.5095568143315483, 2.4829965281959625, 2.499936961332911, 2.4171410347159648, 2.444472781171221, 2.4204254734769775, 2.2810507909462396, 2.1973324642611765, 2.302478416913297, 2.2581627386018948, 2.2639840332924015], [1.8977177, 0.5618236, 0.3621888, 0.3580896, 0.4625717, 0.4439843, 0.40754157, 0.43105847, 0.6039264, 0.6439731, 0.5563913, 0.66244316, 0.60714793, 0.5797986, 0.52487487, 0.48565906, 0.46200487, 0.35219857, 0.36940134, 0.44253796, 0.39095587, 0.36051786, 0.37542602, 0.46107763, 0.39868528, 0.3652579, 0.41631413, 0.37635994, 0.43369064, 0.35332608, 0.4514497, 0.46308672, 0.50795144, 0.47515953, 0.49147162, 0.505555, 0.55112314, 0.50399005, 0.5795659, 0.5022284, 0.48477075, 0.34857848, 0.48929366, 0.49952677, 0.54729027, 0.47249335, 0.5689715, 0.51717067, 0.47447494, 0.39431462, 0.53409296, 0.56410104, 0.5347859, 0.49763268, 0.46503407, 0.41680035, 0.4389089, 0.52868384, 0.521286, 0.5886209]]</t>
+          <t>[[5.076603, 1.8813992, 1.4459801, 1.5612348, 1.5452902, 1.5793561, 1.5300782, 1.725541, 1.6503353, 1.6839423, 1.6056947, 1.6985549, 1.5133882, 1.6330863, 1.6299323, 1.6982028, 1.6425881, 1.5681728, 1.5288539, 1.5826176, 1.4810258, 1.5097058, 1.5887115, 1.7049936, 1.7102301, 1.6759243, 1.6996968, 1.8957057, 1.8956316, 2.0097866, 2.021662, 2.0854998, 1.9697113, 1.9080164, 1.8487109, 1.8663406, 1.7412995, 1.7066337, 1.7219145, 1.7914467, 1.6682098, 1.700898, 1.6461002, 1.7428148, 1.6383253, 1.8112726, 1.7160841, 1.7544597, 1.7102629, 1.8742855, 1.7956582, 1.8390985, 1.7471993, 1.754158, 1.7253095, 1.7121725, 1.676177, 1.7479744, 1.658704, 1.6779287], [7.114169539281629, 2.9041983633259147, 2.0433138087316323, 2.0660116183017965, 2.0556475930902014, 2.0576944721410735, 2.0550745610356858, 2.3180191574555753, 2.2046123921708176, 2.244721578992282, 2.1933860063846833, 2.2911278062235385, 2.0356183543344204, 2.139369512891405, 2.1926219376482345, 2.30145771852482, 2.230997266801077, 2.1100978036785087, 2.096160184679698, 2.182186321425936, 1.9922341733962776, 2.026967978519543, 2.1368539826664117, 2.3172063619678096, 2.32858681418763, 2.227879720190913, 2.3241323759554566, 2.5599267646625736, 2.58800698072739, 2.7335054595373607, 2.8317141861845396, 2.9178613849788486, 2.7622888130487615, 2.585831285583033, 2.5381379777153366, 2.58576489935688, 2.416198378167888, 2.30525123037999, 2.3751316034094625, 2.4233836735565117, 2.2566667969598924, 2.2647124458666665, 2.243026948424254, 2.424865451501535, 2.269154502601629, 2.5028075665803855, 2.4411404152146665, 2.39289468967611, 2.2819211834695645, 2.516184868914775, 2.4284617775918584, 2.4567684645591146, 2.368058752490956, 2.3883018425380316, 2.3730916839262286, 2.2748746229563728, 2.2192498302264125, 2.288050196617196, 2.2245943706967664, 2.212382568863704], [1.8977145, 0.56236744, 0.3627751, 0.3652293, 0.45906603, 0.43758938, 0.41701603, 0.43816498, 0.60802126, 0.6504699, 0.55671996, 0.6497413, 0.58514905, 0.5720266, 0.50810355, 0.4788155, 0.45949876, 0.3380315, 0.34180236, 0.4160389, 0.38377777, 0.3495015, 0.3912924, 0.4775913, 0.42265862, 0.36482808, 0.41137928, 0.36925527, 0.42843622, 0.35862148, 0.45313308, 0.48688427, 0.5100648, 0.477263, 0.47364306, 0.4741284, 0.5439353, 0.49949345, 0.5731361, 0.51252186, 0.4804379, 0.36017212, 0.4933673, 0.49477354, 0.55078804, 0.4877572, 0.5834067, 0.5360765, 0.47920597, 0.3962631, 0.52647126, 0.57201636, 0.5189895, 0.50444365, 0.47085023, 0.42897412, 0.4597365, 0.5250655, 0.53275746, 0.60663915]]</t>
         </is>
       </c>
       <c r="G146" t="inlineStr">
         <is>
-          <t>[[1.9150980178413828, 1.203311095289399, 1.1688085343335024, 1.3467991116864324, 1.3685781279056837, 1.413404585316077, 1.3927161218064132, 1.5238583194176412, 1.504166670501386, 1.52675428963322, 1.432826281843123, 1.4822748253943712, 1.3909423571647264, 1.4677845589141283, 1.4625047419679023, 1.5033536791395703, 1.5012963509756756, 1.4518562657053022, 1.399881499788645, 1.3953317013899, 1.3457710322465972, 1.3562072424263494, 1.3775394867959194, 1.477132445207683, 1.4604193175980051, 1.4567846620488663, 1.4829543657196966, 1.6390814723473504, 1.6813241062677966, 1.772621247979602, 1.8069848379119657, 1.7462455873375955, 1.7519453898566395, 1.6869242328257388, 1.6479404670182822, 1.659434704118729, 1.5886982535320824, 1.5168333634636513, 1.4883129217534035, 1.5376292003376797, 1.4897495355634096, 1.4977639158712013, 1.4966441943675133, 1.509036300342705, 1.4838400781801742, 1.587229197380481, 1.5006183694394852, 1.5124068885800683, 1.5307542428990264, 1.6572649940150406, 1.620842182597661, 1.6534287530833296, 1.608234881486283, 1.5981445943799466, 1.5715130985892332, 1.5083280126229721, 1.5008847164340262, 1.578149307134369, 1.4957520628962866, 1.4692239248971353], [3.08706643351503, 1.7403791313827794, 1.5825193731488598, 1.7903401422901077, 1.787838724873965, 1.8291691599400806, 1.844879015673038, 2.0189552506804826, 1.9884890483375843, 2.0226920235332226, 1.9079010287308362, 1.9944052152990892, 1.876869234419346, 1.9190856280106419, 1.9605949318337639, 2.0451499485766553, 1.9910958015881146, 1.9473108543856608, 1.9158365248223412, 1.8992562503969528, 1.7797858248771015, 1.796361738363951, 1.846619570901859, 2.012909469600058, 1.9286444307918529, 1.9465569070198323, 1.9835041693554227, 2.2007445944278166, 2.2748841337744423, 2.4052322629207605, 2.5967301855953218, 2.4585447866575416, 2.47890867848595, 2.2996634664960536, 2.2167436423148215, 2.230233720352034, 2.156026709778232, 2.0639801818671315, 2.0524951951171277, 2.0776221782365534, 1.994393408937314, 1.9648747215885947, 2.0301766786853235, 2.0633498161939285, 2.0496712313373715, 2.198316405071439, 2.095323379639115, 2.0468487815906973, 2.0577808897234844, 2.2428477760544, 2.1834989929847666, 2.218132316746829, 2.182192921927202, 2.1794438485863163, 2.155625336658443, 2.0099900918394473, 1.9636671532236523, 2.0672819528497683, 2.004740054565488, 1.9305949896582668], [0.582554854149639, 0.33085414154697895, 0.29271066217905883, 0.3326322238339868, 0.403520993673567, 0.4027315806427556, 0.3719354973353931, 0.37016225328426783, 0.5470525867979692, 0.5791135188268062, 0.4847902459469189, 0.554068751267187, 0.5404691037586067, 0.48871692086350216, 0.4503234992272381, 0.42900936049963473, 0.3999487929481144, 0.32487184211368153, 0.329125877680823, 0.3745110413224011, 0.34223791689221905, 0.329188627004225, 0.3280163993416491, 0.40628073730693853, 0.34465900975142855, 0.3189232310247028, 0.36759343402677463, 0.3353367311384533, 0.3829259602745785, 0.32583557862833706, 0.40642373792802006, 0.3811954313857945, 0.45010785920003066, 0.4012091376835155, 0.42371929505840705, 0.4396640158252339, 0.48371081760211815, 0.4661493325572759, 0.46561197132765936, 0.4366345804795221, 0.42067494325195603, 0.3127856606673417, 0.44138498938862714, 0.4333331616656495, 0.5100494332480194, 0.4136147691013304, 0.4938469573861913, 0.43917464891863955, 0.4070444859644151, 0.34068781762126427, 0.4543966247982785, 0.489986138288392, 0.4661465126778321, 0.40633711169884534, 0.418721300599219, 0.3694723075648642, 0.3871858345281934, 0.47608867825126633, 0.45993860092511885, 0.48084131863796875]]</t>
+          <t>[[1.9195385281954456, 1.2061447592799643, 1.1677123771328906, 1.3448166167858706, 1.3663756858244336, 1.4049025539267201, 1.3813699162538886, 1.512398739230481, 1.4868815311575352, 1.5268227452142258, 1.421325307664926, 1.4893805460442815, 1.37588653933719, 1.4562631683384022, 1.434231791648628, 1.4877718251816565, 1.4672506664863423, 1.4210859251451489, 1.3962954441720283, 1.3974928646457339, 1.3491114856650948, 1.366523765794111, 1.408753227735896, 1.5154635896831532, 1.4810478384900267, 1.4810591905880537, 1.5106190891809599, 1.6626090999804237, 1.6743248745152681, 1.7562049041075605, 1.7797945205744068, 1.7449409220367127, 1.7436935032025545, 1.6788073667660723, 1.593649256173482, 1.6355491250667225, 1.5771477208520783, 1.5340580737202714, 1.5292063999656007, 1.582495217118628, 1.4913987102834785, 1.5134789247579816, 1.5028604152778648, 1.5187308971853695, 1.5036203940368993, 1.6091790318307946, 1.5339692348589142, 1.5230552059317812, 1.536367697450078, 1.6539933281537904, 1.5829048596540365, 1.6306418943474414, 1.5898574248441293, 1.5748599508334884, 1.556629224122119, 1.5221814704082453, 1.5107827427902625, 1.572870132398532, 1.462713380655424, 1.4465781895920886], [3.0935581398979273, 1.7411958888270678, 1.5783680302633147, 1.7912034988990508, 1.792003249960897, 1.8353338896485552, 1.8377230117925374, 2.004906259475426, 1.9846039596272478, 2.0311567150338794, 1.900776520534041, 1.9721484294675535, 1.8484169408591473, 1.893787970659424, 1.9263792137576696, 2.0312656876311173, 1.9527973695279857, 1.9152690535037245, 1.8945224757965604, 1.879216814471295, 1.7955154584085753, 1.8229006048554397, 1.8867707791342403, 2.056414609271094, 1.9492652308146354, 1.9650551463004458, 2.0177350725133554, 2.214659270890757, 2.227721401879403, 2.326751784732568, 2.4788578031793156, 2.409534463411433, 2.418388970204366, 2.258580430040294, 2.148877427596122, 2.2329275879503334, 2.159923606859237, 2.071233466774469, 2.1042565833072144, 2.1245231974226475, 1.9980539626038178, 1.9861850048144378, 2.0326142629699437, 2.0816381157001556, 2.0828644997652006, 2.2381806090487926, 2.1424013959564143, 2.054331360619742, 2.0487526103715634, 2.2210861938299633, 2.1169511832290477, 2.1682310102939946, 2.1367158495596743, 2.139370790132833, 2.1232543243208424, 2.0257705386664475, 1.9662653272099562, 2.052913586159559, 1.9386972069600055, 1.8960988598329944], [0.585570078412383, 0.3339591786598618, 0.2916428199437641, 0.3273588163648913, 0.39504695439604054, 0.40260750977406967, 0.37583042277908346, 0.3742688955871917, 0.5610679812770034, 0.5869298921722711, 0.476679828976311, 0.5469819778141282, 0.5195311579017949, 0.4860620371443224, 0.4343130462390265, 0.4183025809532804, 0.3988889300171468, 0.3019832521566005, 0.3097384178044288, 0.36865841871803506, 0.34819993196665905, 0.3189322812143759, 0.34325552005924104, 0.4187274433149226, 0.3495565062642141, 0.3163695786372432, 0.37225238594429033, 0.3248594739396959, 0.3824690765314127, 0.3233402699807107, 0.41100127725672403, 0.4053775846087856, 0.4402332167349783, 0.4115888071806948, 0.40318960528993275, 0.4236583986416843, 0.4830368465171758, 0.4571732361662954, 0.4679036541814057, 0.4569778056063529, 0.41240737579393877, 0.3218305469461232, 0.44565006079173186, 0.43319793394559075, 0.5241476465272381, 0.4248451377405897, 0.5109593347533673, 0.4481993227312868, 0.41029634116311897, 0.34675173559934835, 0.4484543214761513, 0.4903181780897468, 0.45978274051828333, 0.42108031657437267, 0.42036485553116754, 0.3861136293501013, 0.3991983861084091, 0.4636103784163768, 0.46894686782651585, 0.4888074701099356]]</t>
         </is>
       </c>
       <c r="H146" t="n">
-        <v>69.36297154426575</v>
+        <v>70.37412977218628</v>
       </c>
     </row>
     <row r="147">
@@ -5436,7 +5436,7 @@
         </is>
       </c>
       <c r="H147" t="n">
-        <v>69.23680806159973</v>
+        <v>70.82114577293396</v>
       </c>
     </row>
     <row r="148">
@@ -5470,7 +5470,7 @@
         </is>
       </c>
       <c r="H148" t="n">
-        <v>69.86499905586243</v>
+        <v>70.2780556678772</v>
       </c>
     </row>
     <row r="149">
@@ -5481,7 +5481,7 @@
         <v>60</v>
       </c>
       <c r="C149" t="n">
-        <v>7.000000000000001</v>
+        <v>7</v>
       </c>
       <c r="D149" t="inlineStr">
         <is>
@@ -5504,7 +5504,7 @@
         </is>
       </c>
       <c r="H149" t="n">
-        <v>73.66982197761536</v>
+        <v>74.62006235122681</v>
       </c>
     </row>
     <row r="150">
@@ -5515,7 +5515,7 @@
         <v>60</v>
       </c>
       <c r="C150" t="n">
-        <v>7.000000000000001</v>
+        <v>7</v>
       </c>
       <c r="D150" t="inlineStr">
         <is>
@@ -5538,7 +5538,7 @@
         </is>
       </c>
       <c r="H150" t="n">
-        <v>73.19748854637146</v>
+        <v>74.626056432724</v>
       </c>
     </row>
     <row r="151">
@@ -5549,7 +5549,7 @@
         <v>60</v>
       </c>
       <c r="C151" t="n">
-        <v>7.000000000000001</v>
+        <v>7</v>
       </c>
       <c r="D151" t="inlineStr">
         <is>
@@ -5572,7 +5572,7 @@
         </is>
       </c>
       <c r="H151" t="n">
-        <v>73.15603590011597</v>
+        <v>74.73920345306396</v>
       </c>
     </row>
     <row r="152">
@@ -5606,7 +5606,7 @@
         </is>
       </c>
       <c r="H152" t="n">
-        <v>86.03840398788452</v>
+        <v>86.49382877349854</v>
       </c>
     </row>
     <row r="153">
@@ -5640,7 +5640,7 @@
         </is>
       </c>
       <c r="H153" t="n">
-        <v>85.95462584495544</v>
+        <v>86.55446028709412</v>
       </c>
     </row>
     <row r="154">
@@ -5674,7 +5674,7 @@
         </is>
       </c>
       <c r="H154" t="n">
-        <v>85.74163007736206</v>
+        <v>86.99477076530457</v>
       </c>
     </row>
     <row r="155">
@@ -5708,7 +5708,7 @@
         </is>
       </c>
       <c r="H155" t="n">
-        <v>327.544127702713</v>
+        <v>323.0525455474854</v>
       </c>
     </row>
     <row r="156">
@@ -5742,7 +5742,7 @@
         </is>
       </c>
       <c r="H156" t="n">
-        <v>325.4969835281372</v>
+        <v>326.5902485847473</v>
       </c>
     </row>
     <row r="157">
@@ -5776,7 +5776,7 @@
         </is>
       </c>
       <c r="H157" t="n">
-        <v>328.0387179851532</v>
+        <v>325.2900376319885</v>
       </c>
     </row>
     <row r="158">
@@ -5801,16 +5801,16 @@
       </c>
       <c r="F158" t="inlineStr">
         <is>
-          <t>[[5.0775547, 1.8016684, 1.4385401, 1.5513251, 1.5259157, 1.5666548, 1.5384829, 1.734722, 1.6951426, 1.7043704, 1.6103467, 1.7102337, 1.6003054, 1.7392875, 1.7206305, 1.7536478, 1.7071803, 1.6463809, 1.5629287, 1.5851063, 1.5159876, 1.5761346, 1.6279769, 1.7537539, 1.7261987, 1.7478068, 1.7146453, 1.8853357, 1.8732665, 1.9514292, 2.0018735, 2.0154285, 1.9990461, 1.9878441, 1.893551, 1.9227036, 1.7285272, 1.6402022, 1.6371732, 1.7249916, 1.6288606, 1.6864529, 1.6547686, 1.7388526, 1.6509663, 1.786494, 1.7268329, 1.760797, 1.7011596, 1.8481784, 1.7750028, 1.8196689, 1.7188061, 1.7037188, 1.6982156, 1.6937978, 1.6612256, 1.7641801, 1.652541, 1.6857538], [7.11506710018169, 2.7558725249952034, 1.9860558187202675, 2.084970085606394, 2.0540111284260956, 2.0546068531062818, 2.082507681952661, 2.3549479198164036, 2.280191358767697, 2.2931457139309366, 2.1944304625418507, 2.3284612835202005, 2.2143137464199216, 2.352603719859193, 2.3980279131641593, 2.4383168930191315, 2.308350732602351, 2.2447378295201443, 2.1381933504323243, 2.198493146700455, 2.0590581207298295, 2.118266151117228, 2.19412068770011, 2.369949492065218, 2.330415149753931, 2.2834503849219914, 2.31105408700056, 2.5292964979488137, 2.5426444273130953, 2.629372270608532, 2.844867528636995, 2.8660869929014554, 2.8578023285682166, 2.717575959773241, 2.595412766955901, 2.6431005487328076, 2.3346414191868656, 2.169187241157602, 2.2278328467285524, 2.3154041509294037, 2.157854671742931, 2.2399864957606743, 2.283051184696607, 2.4296783741476027, 2.270781338531003, 2.438885221814078, 2.3995520769792638, 2.3678189181477083, 2.259884105006339, 2.489612839868429, 2.3897735475652455, 2.428255106657163, 2.3305068153293154, 2.3214227864958397, 2.354098147405067, 2.268066038330837, 2.1844905315184366, 2.3423797671017477, 2.2370444404099668, 2.2457756016187207], [1.8978608, 0.56444484, 0.40777096, 0.40135556, 0.4523115, 0.43107966, 0.3933111, 0.41184196, 0.5937599, 0.62888825, 0.52931917, 0.6613284, 0.6304838, 0.6574241, 0.5556755, 0.51342297, 0.48061645, 0.36036703, 0.34768903, 0.40536708, 0.3746855, 0.37722912, 0.41003686, 0.4912644, 0.4326369, 0.39849722, 0.4275773, 0.37752718, 0.44894227, 0.34866863, 0.42428562, 0.425287, 0.49453247, 0.44932246, 0.47908467, 0.4860756, 0.5285759, 0.49479762, 0.54391026, 0.52285707, 0.47704977, 0.37003094, 0.50971985, 0.5211729, 0.5686672, 0.4597364, 0.53666055, 0.48610803, 0.49148536, 0.39469188, 0.53576505, 0.57897, 0.50747913, 0.494686, 0.49304914, 0.4410137, 0.46160024, 0.54747164, 0.5403848, 0.57772195]]</t>
+          <t>[[5.0775547, 1.8016684, 1.4385401, 1.551334, 1.5286902, 1.5615461, 1.5510094, 1.7362189, 1.6869489, 1.6965747, 1.5899699, 1.7124834, 1.5766469, 1.7330452, 1.6994781, 1.7129787, 1.6544192, 1.6051999, 1.5099089, 1.5769861, 1.5264181, 1.5948993, 1.6298761, 1.7464653, 1.70407, 1.7072115, 1.6710683, 1.835534, 1.8427941, 1.9495049, 1.981065, 2.0051358, 1.9623681, 1.925564, 1.8400726, 1.9131733, 1.7265346, 1.6489458, 1.6422609, 1.7446852, 1.6283853, 1.6976599, 1.6581682, 1.7404329, 1.6359432, 1.7707213, 1.6931175, 1.7332757, 1.6646949, 1.8323302, 1.775968, 1.8217229, 1.7047838, 1.7186449, 1.7018471, 1.681579, 1.6475736, 1.7524916, 1.6486869, 1.6522593], [7.11506710018169, 2.7558725249952034, 1.9860558187202675, 2.0849914691485236, 2.059138709073667, 2.0533168848212853, 2.0956431697577695, 2.3476168459411513, 2.267524712037809, 2.280024264524408, 2.1776460227663197, 2.3255915842831105, 2.1822402935915672, 2.3292861193585, 2.365803430396713, 2.3388686146263913, 2.213741075098193, 2.159751260881821, 2.0637738311149487, 2.1725556109897433, 2.0659547251183925, 2.1248937468050446, 2.1927780780588533, 2.3515648319068068, 2.2814461610666923, 2.226871509190601, 2.238416950579385, 2.4639276655094884, 2.5075220433005048, 2.6268243353943133, 2.8061742215874363, 2.8805594388354603, 2.8514511295674563, 2.660139938058009, 2.538753831147722, 2.6618156914822526, 2.3782551192227834, 2.2216175515005947, 2.2488904972514625, 2.335129409896144, 2.1472066786865427, 2.2366766112552305, 2.260221364480718, 2.4150062864233615, 2.2618100373551635, 2.4274262825864263, 2.370460890850657, 2.348902113101432, 2.2478534207596153, 2.4752039507439223, 2.3974648159019036, 2.434628580423609, 2.3339474982377024, 2.328162583425406, 2.3532320603615213, 2.2354834948028333, 2.1710621801650043, 2.326514897010015, 2.212129089817289, 2.200434130403283], [1.8978608, 0.56444484, 0.40777096, 0.40135038, 0.45331335, 0.43009347, 0.39222962, 0.40988386, 0.59922653, 0.6449035, 0.53027225, 0.6469213, 0.6325811, 0.64717484, 0.56687737, 0.49018115, 0.4612505, 0.3536651, 0.3348493, 0.39391643, 0.38263378, 0.38981465, 0.41402152, 0.481163, 0.41666606, 0.3715703, 0.41427344, 0.37337276, 0.43862706, 0.3511672, 0.4205313, 0.41558, 0.5020124, 0.4617763, 0.4656097, 0.49630174, 0.5354482, 0.49342293, 0.5422978, 0.5320089, 0.47619537, 0.3646944, 0.50465906, 0.51011, 0.56495684, 0.44631395, 0.53048944, 0.4850575, 0.47467256, 0.3948582, 0.518709, 0.55658793, 0.5033079, 0.4824469, 0.47830567, 0.41752103, 0.45347366, 0.53337073, 0.53416294, 0.5656769]]</t>
         </is>
       </c>
       <c r="G158" t="inlineStr">
         <is>
-          <t>[[1.8487069697561525, 1.2186432540405925, 1.2023419270223197, 1.3327643070271178, 1.3641480275132158, 1.3836210142503136, 1.4031212304371639, 1.5529509195410194, 1.5172837145306477, 1.4994274458150012, 1.4407180376746291, 1.550753917175142, 1.4630454041272167, 1.5381506498729205, 1.5104192075743554, 1.5520149210114405, 1.541160652425684, 1.456369393903666, 1.4003780928117184, 1.406666971192347, 1.3955668772032699, 1.4170798710666943, 1.4488922793984942, 1.5355664475874429, 1.5109733568906398, 1.5256159979253634, 1.5025412087935401, 1.6334252340807789, 1.656848987974021, 1.7114371164130686, 1.7437440630056467, 1.7245145814528913, 1.795704163177145, 1.720197694839192, 1.6620530716417592, 1.6574795029485658, 1.5475356530061886, 1.442314924504243, 1.4556807217398602, 1.4972579219269826, 1.4725235293746766, 1.5139888518476643, 1.4838682365968554, 1.5255326601808645, 1.4824406805631398, 1.613329776782594, 1.553443349653446, 1.5251921539417876, 1.5328393828688658, 1.6222639746439484, 1.5772872426693751, 1.6027043904330966, 1.5434906068598024, 1.5436434827454497, 1.5296641581595942, 1.518025205365159, 1.515764730620934, 1.5800772949594655, 1.4957841400305882, 1.481870400137797], [2.9295874838508236, 1.7491545767467755, 1.690504711014627, 1.8031132903053777, 1.8046969318349007, 1.8108460880255435, 1.901065249157799, 2.087558963302605, 2.0215236606867983, 1.9894967661330039, 1.9414969237608242, 2.1221287382129996, 2.0095452104360545, 2.0941615858811957, 2.0601449113526558, 2.132708773616507, 2.0967737795303543, 1.9691230253916037, 1.9346738684782487, 1.9352363814617515, 1.8782033435916123, 1.8978310657662167, 1.924451553978208, 2.067581971922886, 2.0053249002794398, 1.9871575914951365, 1.9987973045066443, 2.159975287946206, 2.1905083175568967, 2.282464722233414, 2.453563223663339, 2.4381447483403362, 2.5672790712830786, 2.3287957299418403, 2.2478634522536427, 2.209967524698219, 2.0606495964809906, 1.9156128495263496, 1.962636913668911, 1.9823930869020256, 1.9487945167267746, 1.9920813714801275, 2.0149566776559578, 2.08396196677161, 1.9988380837775095, 2.194376869276825, 2.118744282408242, 2.0393353685265794, 2.0275641624975203, 2.1758750804609694, 2.1270209504970006, 2.1394948246633554, 2.059972899865488, 2.0933440638581247, 2.0978385760060725, 2.020527681268328, 1.989922526616499, 2.080183944082023, 2.0139861948758817, 1.9447973125046876], [0.5706167879509131, 0.36252943860254655, 0.3252707433771813, 0.34635261867904477, 0.3986124015908452, 0.3848280820250129, 0.36161473330702903, 0.36574656176481984, 0.5184873811842345, 0.5286275482393419, 0.48356085887774247, 0.5808452727500819, 0.57410539125672, 0.5645866584559781, 0.47576457751110207, 0.46893781306054044, 0.41886240753008214, 0.2975307186049924, 0.29469327514621774, 0.3531476943823927, 0.3506592135189184, 0.34213818930389617, 0.3630254294644515, 0.4442147745641895, 0.3636365857029996, 0.34430307370261154, 0.3882113226461017, 0.35263225092425693, 0.3890368440641034, 0.30579049273980863, 0.35931262605287634, 0.3638889744450214, 0.43354757561282337, 0.3886518431473694, 0.4129697895651579, 0.4108310952835173, 0.4804129755818309, 0.44078679285340566, 0.47148387967199096, 0.44535679555281876, 0.43523803573592706, 0.33474991075896005, 0.45699497684362556, 0.4460475473821349, 0.5139379754678934, 0.41786583229535484, 0.4617962883304614, 0.417895056631483, 0.4436876692141952, 0.3480402306279154, 0.5004831222727428, 0.5067894860325609, 0.4547793582469672, 0.4608945315429007, 0.4428026275522383, 0.3726309502250008, 0.4037904650110848, 0.4816681004289834, 0.4771692147231919, 0.47701420787237575]]</t>
+          <t>[[1.8487069697561525, 1.2186432540405925, 1.2023419270223197, 1.3362681875629812, 1.3610431199780268, 1.383332254201337, 1.4006711154983555, 1.544536986137184, 1.5116529409185357, 1.4862013345671865, 1.430848764121554, 1.5305438905849065, 1.4380649605764397, 1.5354571068378482, 1.466852034128191, 1.4958461308592261, 1.4991953596889396, 1.4216130621219105, 1.3682787126046936, 1.4041263078196102, 1.4029050210520437, 1.4366224930953262, 1.451566924551325, 1.5248249306807395, 1.4936050760530308, 1.4942490556548196, 1.466578106717616, 1.6052944744195803, 1.6307193976159902, 1.70426564477181, 1.7206219518633294, 1.711687755637747, 1.752311441428038, 1.6765586488454591, 1.6312113481570918, 1.6431293455921752, 1.5515630856512208, 1.4526284109644059, 1.4570889215220133, 1.5090172962738455, 1.4687259948933165, 1.5217419864024302, 1.4822670444288257, 1.5072570060748198, 1.465997264814962, 1.5700858602188172, 1.531088897397906, 1.4980861631433906, 1.5067728497390673, 1.6100210137651207, 1.5758693826945986, 1.5808542292047587, 1.5416128315611555, 1.5384533707306405, 1.5301384083911722, 1.4878124690726942, 1.5135565781827938, 1.5505700028878557, 1.469274437196705, 1.4239073016765278], [2.9295874838508236, 1.7491545767467755, 1.690504711014627, 1.809102343215411, 1.8051823668697655, 1.816157939068318, 1.887428224175767, 2.0850238026315164, 2.021995765993313, 1.9802095927275922, 1.925974250299057, 2.0938748596641314, 1.9789855956986455, 2.0734281108891426, 1.9836612224868262, 2.039685895887729, 2.0079557726287813, 1.900739159970421, 1.8868930653962876, 1.920397052372779, 1.8783125021328424, 1.9065944017875125, 1.9216057174786043, 2.0398633129193677, 1.9655891782029578, 1.9396250828733843, 1.9469291897529337, 2.1283641690000983, 2.1671296258240447, 2.27327512309416, 2.44500512372239, 2.438686769240943, 2.5174780191059187, 2.2802908719506014, 2.2266794835031707, 2.2367049885275887, 2.089557919774929, 1.94552909827619, 1.9663381636369148, 1.990160110222743, 1.9305948912489614, 1.9903524163726791, 1.9887902214096589, 2.0638882585841185, 1.9871944357719407, 2.148135676993936, 2.1058779916085517, 2.0258726754276655, 2.014796200215798, 2.1778285533398347, 2.1285238768826398, 2.1264657930045936, 2.0568447820424267, 2.0695063096998085, 2.080487703230842, 1.982019732424791, 1.9827004291070092, 2.030123266471132, 1.9641849613815405, 1.8752384387605368], [0.5706167879509131, 0.36252943860254655, 0.3252707433771813, 0.3488075971647241, 0.396213929768463, 0.3799208257319715, 0.3590287643084646, 0.3655516030727388, 0.536579947469141, 0.5289798526335797, 0.484249383291315, 0.565268278172663, 0.5748674367239559, 0.5721232021117204, 0.46810445626629826, 0.43416077235004613, 0.4061874541134462, 0.2981576732943888, 0.28819318770643026, 0.3484299017816644, 0.36067387497510583, 0.35300566686544016, 0.35873957434523657, 0.42768765363387395, 0.34846256034369866, 0.32792007641721127, 0.3821089733095307, 0.3353652066961023, 0.3868729082823204, 0.3124619475766314, 0.35737117202358964, 0.3574781219996308, 0.43457412863198347, 0.40436093156049163, 0.4174860754707164, 0.41614236092857776, 0.48715343645595804, 0.42743812454301977, 0.4604038141975258, 0.44396298392618055, 0.4234488358867717, 0.3295830054269292, 0.4533509555084629, 0.427680723215009, 0.5087523741087535, 0.399378116918501, 0.4633537054808028, 0.4299682978166528, 0.4218580827480929, 0.3356691077670024, 0.4750412633377669, 0.4857164248715725, 0.4478575346433221, 0.43722948037761256, 0.4130934800468916, 0.3471470220111205, 0.4055560521683422, 0.4701984426407318, 0.46453529240625974, 0.45101531103304554]]</t>
         </is>
       </c>
       <c r="H158" t="n">
-        <v>69.84853029251099</v>
+        <v>70.40955328941345</v>
       </c>
     </row>
     <row r="159">
@@ -5844,7 +5844,7 @@
         </is>
       </c>
       <c r="H159" t="n">
-        <v>69.71350502967834</v>
+        <v>70.69009232521057</v>
       </c>
     </row>
     <row r="160">
@@ -5878,7 +5878,7 @@
         </is>
       </c>
       <c r="H160" t="n">
-        <v>69.80419492721558</v>
+        <v>70.62770104408264</v>
       </c>
     </row>
     <row r="161">
@@ -5889,7 +5889,7 @@
         <v>80</v>
       </c>
       <c r="C161" t="n">
-        <v>7.000000000000001</v>
+        <v>7</v>
       </c>
       <c r="D161" t="inlineStr">
         <is>
@@ -5912,7 +5912,7 @@
         </is>
       </c>
       <c r="H161" t="n">
-        <v>73.77948594093323</v>
+        <v>74.67466902732849</v>
       </c>
     </row>
     <row r="162">
@@ -5923,7 +5923,7 @@
         <v>80</v>
       </c>
       <c r="C162" t="n">
-        <v>7.000000000000001</v>
+        <v>7</v>
       </c>
       <c r="D162" t="inlineStr">
         <is>
@@ -5946,7 +5946,7 @@
         </is>
       </c>
       <c r="H162" t="n">
-        <v>74.08502054214478</v>
+        <v>74.82100939750671</v>
       </c>
     </row>
     <row r="163">
@@ -5957,7 +5957,7 @@
         <v>80</v>
       </c>
       <c r="C163" t="n">
-        <v>7.000000000000001</v>
+        <v>7</v>
       </c>
       <c r="D163" t="inlineStr">
         <is>
@@ -5980,7 +5980,7 @@
         </is>
       </c>
       <c r="H163" t="n">
-        <v>73.90009880065918</v>
+        <v>74.94943451881409</v>
       </c>
     </row>
     <row r="164">
@@ -6014,7 +6014,7 @@
         </is>
       </c>
       <c r="H164" t="n">
-        <v>86.29679751396179</v>
+        <v>86.92048215866089</v>
       </c>
     </row>
     <row r="165">
@@ -6048,7 +6048,7 @@
         </is>
       </c>
       <c r="H165" t="n">
-        <v>86.67092227935791</v>
+        <v>87.24256777763367</v>
       </c>
     </row>
     <row r="166">
@@ -6082,7 +6082,7 @@
         </is>
       </c>
       <c r="H166" t="n">
-        <v>86.13648366928101</v>
+        <v>86.99406671524048</v>
       </c>
     </row>
     <row r="167">
@@ -6116,7 +6116,7 @@
         </is>
       </c>
       <c r="H167" t="n">
-        <v>327.0216455459595</v>
+        <v>323.267147064209</v>
       </c>
     </row>
     <row r="168">
@@ -6150,7 +6150,7 @@
         </is>
       </c>
       <c r="H168" t="n">
-        <v>327.5132012367249</v>
+        <v>324.3977735042572</v>
       </c>
     </row>
     <row r="169">
@@ -6184,7 +6184,7 @@
         </is>
       </c>
       <c r="H169" t="n">
-        <v>327.4298787117004</v>
+        <v>322.9130461215973</v>
       </c>
     </row>
     <row r="170">
@@ -6218,7 +6218,7 @@
         </is>
       </c>
       <c r="H170" t="n">
-        <v>69.30193638801575</v>
+        <v>71.40942120552063</v>
       </c>
     </row>
     <row r="171">
@@ -6252,7 +6252,7 @@
         </is>
       </c>
       <c r="H171" t="n">
-        <v>69.22593712806702</v>
+        <v>72.92045426368713</v>
       </c>
     </row>
     <row r="172">
@@ -6286,7 +6286,7 @@
         </is>
       </c>
       <c r="H172" t="n">
-        <v>69.39987277984619</v>
+        <v>71.35658240318298</v>
       </c>
     </row>
     <row r="173">
@@ -6297,7 +6297,7 @@
         <v>100</v>
       </c>
       <c r="C173" t="n">
-        <v>7.000000000000001</v>
+        <v>7</v>
       </c>
       <c r="D173" t="inlineStr">
         <is>
@@ -6320,7 +6320,7 @@
         </is>
       </c>
       <c r="H173" t="n">
-        <v>74.24641418457031</v>
+        <v>75.54012751579285</v>
       </c>
     </row>
     <row r="174">
@@ -6331,7 +6331,7 @@
         <v>100</v>
       </c>
       <c r="C174" t="n">
-        <v>7.000000000000001</v>
+        <v>7</v>
       </c>
       <c r="D174" t="inlineStr">
         <is>
@@ -6354,7 +6354,7 @@
         </is>
       </c>
       <c r="H174" t="n">
-        <v>73.70638370513916</v>
+        <v>75.51632690429688</v>
       </c>
     </row>
     <row r="175">
@@ -6365,7 +6365,7 @@
         <v>100</v>
       </c>
       <c r="C175" t="n">
-        <v>7.000000000000001</v>
+        <v>7</v>
       </c>
       <c r="D175" t="inlineStr">
         <is>
@@ -6388,7 +6388,7 @@
         </is>
       </c>
       <c r="H175" t="n">
-        <v>73.77550625801086</v>
+        <v>74.49822759628296</v>
       </c>
     </row>
     <row r="176">
@@ -6422,7 +6422,7 @@
         </is>
       </c>
       <c r="H176" t="n">
-        <v>86.1941556930542</v>
+        <v>87.02034711837769</v>
       </c>
     </row>
     <row r="177">
@@ -6456,7 +6456,7 @@
         </is>
       </c>
       <c r="H177" t="n">
-        <v>86.1381893157959</v>
+        <v>86.98324155807495</v>
       </c>
     </row>
     <row r="178">
@@ -6490,7 +6490,7 @@
         </is>
       </c>
       <c r="H178" t="n">
-        <v>86.48618459701538</v>
+        <v>86.93381953239441</v>
       </c>
     </row>
     <row r="179">
@@ -6515,16 +6515,16 @@
       </c>
       <c r="F179" t="inlineStr">
         <is>
-          <t>[[5.07496, 1.0864481, 1.1878333, 1.4392838, 1.3856453, 1.4037445, 1.3562796, 1.5262983, 1.4261695, 1.4540973, 1.3603482, 1.4749281, 1.3286026, 1.4184183, 1.3860425, 1.4126922, 1.3253504, 1.2893666, 1.2836032, 1.3311517, 1.2840734, 1.3807561, 1.4195292, 1.4899197, 1.3823808, 1.4227055, 1.4298781, 1.5899416, 1.5443045, 1.5967345, 1.6337805, 1.709129, 1.6125848, 1.553339, 1.5151592, 1.5648572, 1.4300543, 1.4171958, 1.4222313, 1.4928666, 1.3571485, 1.432061, 1.3842857, 1.4693537, 1.3665485, 1.5015248, 1.4246664, 1.4404327, 1.3934742, 1.5296886, 1.492133, 1.5254923, 1.4019753, 1.4647429, 1.468321, 1.466304, 1.3823409, 1.4871062, 1.3838333, 1.3784076], [7.1122123673510185, 1.4773895530923127, 1.6041854593076212, 1.8894659225285992, 1.799300306809759, 1.8197938892487038, 1.7844741820447494, 2.0424556634916464, 1.9115105257176062, 1.9417505707300986, 1.844570429966272, 2.0029205217900348, 1.798829781762436, 1.8446738304731598, 1.853068065572809, 1.886647793717002, 1.757695444236208, 1.7203508724468428, 1.7403872644328893, 1.7958436079092754, 1.7078640998939771, 1.8071332600089407, 1.8708393983239955, 1.9798130251523725, 1.8174525375150778, 1.8735643612730575, 1.940317197705832, 2.1408186776191753, 2.0749970033922733, 2.137036287748481, 2.30561484090832, 2.3819711669470807, 2.229581051633244, 2.0864894865252426, 2.0508858790273887, 2.1342908046754356, 1.9303328326925135, 1.8848856042811182, 1.918697552787376, 1.9760696339442119, 1.7864542776641927, 1.8460538662070145, 1.8754445502663248, 2.012417984706984, 1.8356235966272805, 2.046934869487624, 1.9621316989401083, 1.9132638315986608, 1.8747529184939575, 2.065367237346366, 2.00989018268356, 2.0479653053548676, 1.9024710798634488, 1.965355808280083, 2.0039492002052284, 1.9169356599655691, 1.785192576900625, 1.9240672316314127, 1.8236829473184444, 1.8187111289992839], [1.8963157, 0.29936177, 0.32698625, 0.35558832, 0.39127633, 0.3706018, 0.3347722, 0.36820665, 0.494939, 0.5286799, 0.44920927, 0.54209954, 0.47116736, 0.45777714, 0.41273487, 0.38493174, 0.34348902, 0.27913266, 0.29245916, 0.34255248, 0.32945803, 0.31660014, 0.3486256, 0.38583922, 0.31496808, 0.29772198, 0.3670632, 0.3244239, 0.3861444, 0.2966109, 0.36201823, 0.37403375, 0.4210599, 0.3866749, 0.3865578, 0.40447992, 0.46268123, 0.4029068, 0.44773903, 0.3951263, 0.38133153, 0.28264892, 0.42584684, 0.43331915, 0.45551005, 0.37210223, 0.44118872, 0.39166135, 0.38686413, 0.30947706, 0.425204, 0.46288022, 0.39581704, 0.40121603, 0.39126855, 0.34775218, 0.36025837, 0.44779173, 0.42186925, 0.4592419]]</t>
+          <t>[[5.075225, 1.0886656, 1.1886195, 1.433811, 1.3866503, 1.4342765, 1.3898872, 1.547163, 1.4460089, 1.5015194, 1.4064573, 1.5049682, 1.3335804, 1.4417388, 1.3879939, 1.432534, 1.3399152, 1.3280934, 1.3068568, 1.3505629, 1.2898333, 1.3978934, 1.4445492, 1.4906206, 1.3957875, 1.4717658, 1.460744, 1.604432, 1.5642064, 1.6649317, 1.7042426, 1.7384529, 1.6251367, 1.6206424, 1.5817358, 1.6110837, 1.4244761, 1.4339333, 1.4462551, 1.5117817, 1.3491695, 1.448765, 1.4056104, 1.4689176, 1.3790853, 1.5188546, 1.4270092, 1.4452164, 1.4039916, 1.5535017, 1.5029885, 1.5095763, 1.4006506, 1.4668236, 1.4789786, 1.459698, 1.3789386, 1.5176413, 1.3939406, 1.4023985], [7.112541415826392, 1.4801891535948781, 1.6027770112754065, 1.8784951376873626, 1.8074295548341204, 1.860004350595616, 1.8303212072586392, 2.0602786499742094, 1.9381155451372063, 2.0019092983007614, 1.9104771256803372, 2.0438108149355005, 1.8034891220369653, 1.8745903203353123, 1.8611309831738176, 1.9165750633685081, 1.7740027245346874, 1.7761524274041165, 1.7848491780224327, 1.8256216923763058, 1.7169345631246766, 1.8358776326259652, 1.9100389191022658, 1.976700306788942, 1.847719413209972, 1.9435026643154292, 1.994822476168188, 2.1541878611286287, 2.086300479010802, 2.239146333390841, 2.4236404383165344, 2.449999233167879, 2.251242400584932, 2.17477596488386, 2.1515098105456705, 2.2071852908770846, 1.9252576135440995, 1.9190565703076325, 1.9661133079280595, 2.033504936397987, 1.8000754340577896, 1.8974405190414194, 1.907817821198462, 2.0211144740071045, 1.8519271298402324, 2.0660722026265357, 1.9523673457215398, 1.9185330246505543, 1.898572814891284, 2.11085774619042, 2.0441903716043934, 2.0302397343056957, 1.895399008944209, 1.9598039489125483, 2.0182035054862246, 1.9095017261562253, 1.780735276122397, 1.965219875002411, 1.8497131383001646, 1.8465532877897721], [1.8963333, 0.30106774, 0.32644245, 0.35453397, 0.3940994, 0.37673318, 0.34867266, 0.37417537, 0.50502855, 0.5559207, 0.47258872, 0.54799837, 0.46678132, 0.47164384, 0.4106599, 0.378939, 0.3451844, 0.2834035, 0.29750815, 0.34121224, 0.32265896, 0.32250825, 0.3475918, 0.3888145, 0.31998727, 0.3078694, 0.379932, 0.33221766, 0.3910594, 0.31503955, 0.37801063, 0.385034, 0.42535383, 0.40592298, 0.40728417, 0.41409943, 0.4621641, 0.41074315, 0.4524946, 0.41705117, 0.37701938, 0.2897411, 0.43395308, 0.43239707, 0.46253192, 0.38428298, 0.44738263, 0.391715, 0.3898466, 0.3283894, 0.44942257, 0.47183976, 0.40558815, 0.39525402, 0.39407814, 0.33978283, 0.35580677, 0.4674809, 0.44670364, 0.47881895]]</t>
         </is>
       </c>
       <c r="G179" t="inlineStr">
         <is>
-          <t>[[0.7971284483329155, 0.781132308071205, 0.9450562805730081, 1.0986484524121465, 1.1751945411956406, 1.129254662284489, 1.103879060525614, 1.170428233392604, 1.2211499917503998, 1.1512748875136416, 1.0830889394474181, 1.156091061697558, 1.1207728220245894, 1.1368518605400986, 1.083702624667793, 1.0745227786900333, 1.1299986831225333, 1.0407621594559013, 1.0106531466173956, 1.0475333896658483, 1.1131391116313705, 1.1102676925456627, 1.1062689081144277, 1.1128309961659555, 1.156434794247585, 1.1045839328495197, 1.1122423984917122, 1.1838984506958745, 1.2696499801490884, 1.2547955126951744, 1.275077737372873, 1.2722887115021073, 1.3460917088211464, 1.207655929573668, 1.1525163586853717, 1.184817904409383, 1.2217121230153283, 1.1614989617959595, 1.1234716169331431, 1.1404519117042244, 1.1500387001535641, 1.1401282420239505, 1.1078647962287147, 1.1213075772095267, 1.1709559061430372, 1.1849619861542013, 1.131011506908744, 1.095432063993168, 1.1877018730368536, 1.2346020679121763, 1.1868867972804016, 1.1677143233000846, 1.2038738834283715, 1.1944235743752076, 1.1812344652578255, 1.1278951077990538, 1.1944531343070215, 1.175522060384411, 1.0736025645778213, 1.074498063883952], [1.146780284347332, 1.0702517715457334, 1.2639511384243896, 1.4274175033413121, 1.5137089083797732, 1.4645109420629427, 1.448894643696348, 1.5600314676912888, 1.6212579228377832, 1.5094364429102245, 1.4418990037947985, 1.5755930935798705, 1.4869072996302133, 1.4783331218935214, 1.4328164790640967, 1.417290863857707, 1.4807933670575217, 1.3912782562062787, 1.3480551151107225, 1.4005935310726572, 1.4685959110693403, 1.4489669213254341, 1.4341226014729553, 1.463898003993029, 1.5051351423726442, 1.4408545541008204, 1.4715254311240151, 1.5752818247207472, 1.6449074323377706, 1.6645590586804553, 1.77867209945796, 1.7527175213098747, 1.8262944158757626, 1.5965457191219121, 1.5154676955670854, 1.5751444525212972, 1.6224750975988622, 1.5437674295234232, 1.485213517923518, 1.4834867259799347, 1.4896971990434007, 1.461042955392633, 1.4673417463147385, 1.5028848236048193, 1.5668751710075037, 1.6014337474192395, 1.5320073468262843, 1.4557069067226187, 1.5917389399910904, 1.6553225177908648, 1.5907953796169094, 1.562851117033534, 1.612371600539594, 1.588027108199655, 1.5931995398983965, 1.4767232511315673, 1.537525430414327, 1.5180542294239041, 1.4048687172632506, 1.4221530861208551], [0.17802761709358547, 0.2031043816241395, 0.2594423374642068, 0.2740171814473048, 0.3257216450191595, 0.2967197559516182, 0.27148481558801957, 0.290010167072606, 0.4206592924732448, 0.39054505081597146, 0.3477408770727504, 0.41074305952662343, 0.3906134960647376, 0.3568603283373062, 0.321293674662091, 0.29428897926306014, 0.2861746183620265, 0.2201919198210345, 0.22809344846911542, 0.27454500030090956, 0.28342971501282854, 0.2688570453944573, 0.26421464056934413, 0.2866897799942122, 0.2626288246718078, 0.23276370268411167, 0.29587106413558323, 0.23768360895190843, 0.305784517332103, 0.23720317356303305, 0.2794606371451087, 0.27695228637400343, 0.3380518709545887, 0.3085920501348523, 0.30905586843044275, 0.2983284636758239, 0.38435407588448256, 0.326882890759836, 0.34556262078454336, 0.30810862248512927, 0.3329918288335495, 0.23004006924886775, 0.33601791989387986, 0.3281569811811842, 0.38545556815054227, 0.3021767273144588, 0.3307859016197886, 0.28922726444541635, 0.3164698954103617, 0.2395636371632895, 0.30787347397535003, 0.3470495372718936, 0.33525323869698637, 0.3136713298077139, 0.306226139589658, 0.26491859365260223, 0.30160343141611495, 0.3491997951227146, 0.31609327557758604, 0.34495099419865316]]</t>
+          <t>[[0.8010257618518152, 0.7728959300688447, 0.9403339213251091, 1.0901750841416664, 1.2145327751783956, 1.1625747347377555, 1.1315264585671452, 1.1900694381018908, 1.279663611133668, 1.2057092578779527, 1.1167313341967975, 1.1610923267938436, 1.1683667391399675, 1.1465575591987829, 1.1090174742026058, 1.0817065416368654, 1.1842938432121193, 1.081968143625874, 1.03783292479798, 1.0577353024031622, 1.1481783317468233, 1.1266331359424873, 1.108041911842529, 1.1264252683711482, 1.2167478752668073, 1.1506788100972645, 1.1305780883361498, 1.1837734115981404, 1.3424924717381563, 1.3323436731430454, 1.3058664265747686, 1.3014085811097382, 1.4149879432408166, 1.2860452208893518, 1.2094413819434582, 1.1990768825703464, 1.2549582870080613, 1.1753900255812615, 1.1578157931097743, 1.1606095463200232, 1.1841496936153428, 1.1693355043248252, 1.1225757307236088, 1.1268482617935538, 1.2147662628675862, 1.1910289420511202, 1.1399570482172015, 1.107759347448957, 1.2289232368986212, 1.2343739335028034, 1.1808317115387765, 1.1486088445640266, 1.224401640015002, 1.1968137397179939, 1.1766503334337473, 1.131620196672076, 1.233450196849675, 1.2128835672438512, 1.1105529269635004, 1.0937144185166494], [1.1521799874727532, 1.0531127564956317, 1.2553526983918089, 1.4202618480104365, 1.5681146264924106, 1.5054133394383733, 1.481701663959126, 1.578798346466376, 1.7037335259114519, 1.588497906749474, 1.491987124205311, 1.578391573561248, 1.5479351167526096, 1.4929436282822055, 1.4608396734172235, 1.4278028008133585, 1.556066302844428, 1.4453780930899096, 1.3899025426997218, 1.4217561170788722, 1.5145703452318193, 1.475313371474677, 1.4369764077803924, 1.492258446405492, 1.5959676954884723, 1.510422281231225, 1.495553977498471, 1.5671673745192538, 1.7437531770873138, 1.7801236342171645, 1.8392799038979453, 1.7966060302665452, 1.9278385426835074, 1.7087348631249601, 1.5965218015812794, 1.595704915408999, 1.668164767741917, 1.5772876682325554, 1.5561509477771083, 1.5478423408849993, 1.5590273904287741, 1.510080907186862, 1.4928122873505467, 1.517323582603446, 1.619977059897091, 1.593718358001683, 1.5379547243373766, 1.4776042644274294, 1.6518651158323483, 1.665348965602058, 1.5930117180571122, 1.5289770759247736, 1.6264907509640454, 1.5914642256080234, 1.5810678814631962, 1.4837619294503601, 1.5842010638336883, 1.5709502841613339, 1.4607413771773048, 1.4436912914013522], [0.17912116190189417, 0.206129677379553, 0.25508942835710824, 0.28352188079815877, 0.3428023337876224, 0.303488950077094, 0.2900785638317453, 0.285241202104915, 0.4439592163343869, 0.4193265738876392, 0.35855783454136225, 0.3914585713093199, 0.3991717784070379, 0.3629377398647812, 0.32210795694292615, 0.29274411049799826, 0.3003513050436528, 0.22608077570091914, 0.232567944417104, 0.2702264964511107, 0.2903646040769832, 0.26373226636195146, 0.26311301620757416, 0.2862639504351765, 0.2789688633716166, 0.24970171117021078, 0.3015975346165942, 0.24265249242012232, 0.3300821401129423, 0.24856185075211712, 0.28943422661128354, 0.2878253052449072, 0.35321956511667224, 0.3267085782886831, 0.3231032500490172, 0.2953426019280529, 0.40511544404084715, 0.337941197837677, 0.3554623935190406, 0.31102623219711684, 0.3417805103915575, 0.234798055403792, 0.3513684710976086, 0.33790394752552644, 0.4071529231052943, 0.30778012339019767, 0.33076995379163854, 0.29770597032072044, 0.33037501258930096, 0.2550435279049128, 0.32803565860107275, 0.3581147084035778, 0.34938386777014596, 0.3213598843700852, 0.30187042087024285, 0.26470056091082644, 0.3195614668898889, 0.3845564764245725, 0.344390408009918, 0.35574703517155065]]</t>
         </is>
       </c>
       <c r="H179" t="n">
-        <v>327.1454269886017</v>
+        <v>323.6746866703033</v>
       </c>
     </row>
     <row r="180">
@@ -6558,7 +6558,7 @@
         </is>
       </c>
       <c r="H180" t="n">
-        <v>327.2786979675293</v>
+        <v>326.22145819664</v>
       </c>
     </row>
     <row r="181">
@@ -6583,16 +6583,16 @@
       </c>
       <c r="F181" t="inlineStr">
         <is>
-          <t>[[4.5329, 1.6244891, 1.6531825, 1.839576, 1.9335864, 2.0795264, 2.0630038, 2.1570525, 2.0775144, 2.2242486, 2.0516825, 2.0426276, 2.0162237, 2.1883802, 2.2749348, 2.227837, 2.06988, 2.0894482, 2.0473032, 2.1726155, 1.9844275, 2.1450393, 2.0759897, 2.16559, 2.2093313, 2.298282, 2.364558, 2.4202008, 2.3245575, 2.423348, 2.4160585, 2.314957, 2.237081, 2.2329345, 2.196994, 2.3575957, 2.2215447, 2.256998, 2.3284419, 2.2527266, 2.0862184, 2.219164, 2.1776152, 2.1614928, 2.125246, 2.1596234, 2.1543896, 2.1356866, 2.1314852, 2.2062345, 2.2385166, 2.1694803, 2.2016304, 2.2526555, 2.1164632, 2.1592546, 2.1257904, 2.166197, 2.1171453, 2.196943], [6.106633890944122, 2.1018201251754465, 2.1371103656636117, 2.3752468382406113, 2.4830921627766402, 2.7007549678548814, 2.7139370289175706, 2.844789755080391, 2.6811771089476126, 2.8750864098873357, 2.658387345230697, 2.637845173165547, 2.623911859136858, 2.850563522308239, 2.9447890405920947, 2.8554047917875636, 2.665864038873886, 2.749742062349548, 2.6629579105524788, 2.834297483618643, 2.547049580774793, 2.776722684327987, 2.7090677194900388, 2.777409677487562, 2.86561711933213, 3.0019512188917177, 3.0565649638698886, 3.136330928556553, 2.9710888132580435, 3.1047534430709214, 3.0687063738485842, 2.958010069328951, 2.864135947693069, 2.839296311789697, 2.846842834089946, 3.057968835825327, 2.833651711770627, 2.87381769831473, 2.9514311923317553, 2.889619229585827, 2.662077312318381, 2.901913596888045, 2.8028350067681105, 2.828604810278292, 2.749495373289298, 2.7452042117009126, 2.74973096398504, 2.75254443972103, 2.7209776598129976, 2.806688705170549, 2.8586539938501083, 2.832899584012922, 2.8723032369528405, 2.942528985333672, 2.7738805282707526, 2.841282371272814, 2.7573489050742137, 2.8094241807343585, 2.756626381985266, 2.831241134393887], [87905985000000.0, 44742386000000.0, 48558862000000.0, 40123800000000.0, 41725170000000.0, 36847660000000.0, 5465.665, 6508.0273, 42555576000000.0, 6441.617, 51291225000000.0, 44091346000000.0, 67212765000000.0, 59374156000000.0, 35070720000000.0, 61939130000000.0, 5107.308, 43451310000000.0, 46402080000000.0, 58289832000000.0, 45047534000000.0, 55677430000000.0, 52502630000000.0, 6232.616, 6591.414, 70959300000000.0, 37059080000000.0, 40845210000000.0, 56448076000000.0, 51800410000000.0, 58651557000000.0, 50555695000000.0, 53253094000000.0, 65789360000000.0, 58099897000000.0, 46339280000000.0, 45719450000000.0, 54384793000000.0, 55018230000000.0, 58639314000000.0, 5366.014, 57558390000000.0, 36636637000000.0, 6819.663, 45466117000000.0, 49276500000000.0, 39507070000000.0, 41758835000000.0, 51588680000000.0, 44610596000000.0, 4439.8, 34863432000000.0, 48224210000000.0, 37878898000000.0, 46486096000000.0, 50364760000000.0, 44586250000000.0, 50304033000000.0, 4725.2197, 64583460000000.0]]</t>
+          <t>[[4.5329, 1.6244891, 1.6531825, 1.839581, 1.9560621, 2.0928605, 2.0727932, 2.1908236, 2.1566193, 2.2942545, 2.096168, 2.0532668, 2.0656466, 2.2386131, 2.2969468, 2.2351308, 2.1244519, 2.117906, 2.0369072, 2.172, 2.0285707, 2.1734495, 2.101919, 2.180555, 2.2680485, 2.3260543, 2.3747985, 2.4120274, 2.344206, 2.4510307, 2.4229612, 2.3102384, 2.291335, 2.2890313, 2.2287147, 2.3509743, 2.28728, 2.3127775, 2.336736, 2.2593257, 2.1054156, 2.2481644, 2.2075672, 2.1829739, 2.168916, 2.1933463, 2.19798, 2.1664813, 2.2030911, 2.256078, 2.27262, 2.2080123, 2.236137, 2.2818768, 2.1253014, 2.1477134, 2.16731, 2.2095442, 2.1348832, 2.1860213], [6.106633890944122, 2.1018201251754465, 2.1371103656636117, 2.375225558361665, 2.517804735637396, 2.730768495623654, 2.7281444955240644, 2.8926559324444137, 2.801153309901132, 2.956791292278464, 2.6945349414830018, 2.648584232372858, 2.681413367214019, 2.920445056598956, 2.9715373556429414, 2.8616107475610026, 2.749861106832954, 2.794095496334934, 2.6662225552133156, 2.837784095019614, 2.6220282126799472, 2.8174818209964565, 2.7350377614763675, 2.7862645922655647, 2.943328918015944, 3.048734752684156, 3.064586318010493, 3.13940983128121, 2.997461357472115, 3.131233102596779, 3.0901182802641953, 2.971921331162823, 2.95144605593698, 2.921093514935468, 2.8864067022541837, 3.057383720576099, 2.9401958351047113, 2.97360298630362, 2.9746601904412864, 2.8911867987639055, 2.6910079417712205, 2.9385732759715886, 2.836420359633418, 2.8536828923532944, 2.8116618285017854, 2.791134532106677, 2.8070811308907393, 2.7864116819285236, 2.8178758741809866, 2.872757410214001, 2.903398653237964, 2.873570957787275, 2.922973752614224, 2.978083504771006, 2.785119012313521, 2.824718468065114, 2.829588621993373, 2.8656044729448147, 2.7870228893652715, 2.832381275513657], [87905985000000.0, 44742386000000.0, 48558862000000.0, 40121584000000.0, 41464864000000.0, 37055237000000.0, 5564.4604, 6842.6987, 43850630000000.0, 6594.672, 52264614000000.0, 43653947000000.0, 66104236000000.0, 59540884000000.0, 36474137000000.0, 63709733000000.0, 5327.484, 42522480000000.0, 45170716000000.0, 58536785000000.0, 45475047000000.0, 57469984000000.0, 50832976000000.0, 6283.689, 6766.549, 69457406000000.0, 32690032000000.0, 40324300000000.0, 55616916000000.0, 49841216000000.0, 56573167000000.0, 51012160000000.0, 53330047000000.0, 65871456000000.0, 58478626000000.0, 47208490000000.0, 46564990000000.0, 55839574000000.0, 51577843000000.0, 58468360000000.0, 5463.6353, 56373120000000.0, 36933500000000.0, 6889.3594, 44489423000000.0, 48700034000000.0, 40679640000000.0, 39766400000000.0, 53135993000000.0, 46722010000000.0, 4634.382, 34743260000000.0, 48538503000000.0, 39356570000000.0, 46782660000000.0, 49345100000000.0, 44531383000000.0, 50791566000000.0, 4681.0054, 63301346000000.0]]</t>
         </is>
       </c>
       <c r="G181" t="inlineStr">
         <is>
-          <t>[[0.4077524491819644, 0.9327384843164139, 1.2236997059698704, 1.386211819953354, 1.5092489682375678, 1.5496238189941647, 1.574579852736404, 1.5601175688127413, 1.586765423368035, 1.6380827988794529, 1.5596205451718521, 1.5298361098633069, 1.5690228783152662, 1.6255467283241891, 1.7308887257882466, 1.6425340388901837, 1.6210364481269253, 1.587882600255613, 1.583123140227332, 1.6098766882102105, 1.5349560775179458, 1.5647297052616833, 1.6107775484256197, 1.6402211876109911, 1.746937755999879, 1.7235243951342536, 1.8311332602897155, 1.7944109126619914, 1.7743016501615745, 1.774924739422849, 1.8214420051474458, 1.7531013052861941, 1.7556566140657415, 1.6784772217001234, 1.6972469588202364, 1.7506654200256706, 1.728841036158654, 1.691483886545886, 1.7856308544063602, 1.6818686035807673, 1.6404006064820331, 1.677558755178855, 1.6950544984274674, 1.6544651162325585, 1.7010634926704646, 1.6298764697056898, 1.674529267800217, 1.6426108566223943, 1.708427983884407, 1.6766326615236855, 1.7362593582293266, 1.6545631185691325, 1.7004242185353613, 1.7140224195720835, 1.6879378982854687, 1.6376211045639038, 1.676950683684324, 1.6125126499231677, 1.6355799871217427, 1.6291634256247716], [0.7513564109080847, 1.2636409273441025, 1.5997429325074861, 1.7890336250441714, 1.9259940520060506, 1.9870562396691842, 2.030104320398769, 1.9927410451847383, 2.0308286986406103, 2.1110707273602523, 2.0132203834440072, 1.9752344358061926, 2.0100644985038967, 2.0967275381504464, 2.2394146431286335, 2.112492319336176, 2.1033585200095035, 2.0838587630104857, 2.0322023162490206, 2.0749674348285194, 1.968556671932162, 2.022773962660784, 2.099187407233697, 2.1086255774827287, 2.2638725149617382, 2.235646767006334, 2.3597745396334715, 2.3026450067604323, 2.269114353466097, 2.2712956608377164, 2.309130824264483, 2.244513410216435, 2.2431544143493736, 2.142010289550913, 2.1966567846310046, 2.2569586700988777, 2.1963600893075235, 2.1345758155020547, 2.2857998650914104, 2.1372187752940417, 2.091822064334871, 2.1653374525727314, 2.159614343454294, 2.1627389741578145, 2.191396062001774, 2.078392053935086, 2.1478643577042558, 2.1135146221526537, 2.1749522320522434, 2.132981329380383, 2.204960958159153, 2.16017782687096, 2.204859215354934, 2.225421322273336, 2.1948144936746132, 2.1405830505511863, 2.169361531560083, 2.0736097843877306, 2.121717497727047, 2.0990460356029206], [9395803734297.346, 26981225775886.45, 38331914268170.79, 28015522492055.465, 32989370262452.793, 27949296946145.668, 4411.960961424415, 5127.006581429194, 32131535411348.38, 4620.540681027891, 36833626026304.08, 31565828077370.855, 52767521927580.664, 45407179791260.79, 29719480030298.9, 48826317259866.33, 4211.1796229410975, 35069935804101.605, 38056979301062.89, 43710666974266.56, 33993418824288.227, 41872155327919.61, 41619382883700.53, 5042.641409926974, 5214.474126738396, 51645465098927.68, 30858394600497.188, 26949148731741.62, 45298279553076.29, 37915290136314.016, 47438353361308.59, 39746274815138.68, 44313541239333.12, 52962157454313.97, 45625186395211.85, 36127211318104.25, 35899455560036.445, 45191735010521.48, 43644743965298.94, 44683742861945.04, 4360.6923527822655, 46303886584188.414, 29326273845320.766, 5640.8405991646505, 37975465621476.72, 39092749842981.1, 33057941732501.12, 33921014390761.992, 42182804607259.61, 34078334770932.477, 3607.921907782924, 28088015090423.77, 37410004229692.555, 30910553598450.223, 40841172663278.58, 36893123674446.51, 36407074485451.62, 39297543645147.6, 3819.265948034796, 50769613893836.25]]</t>
+          <t>[[0.4077524491819644, 0.9327384843164139, 1.2236997059698704, 1.4347608145065083, 1.537869823436419, 1.5476548749163221, 1.5991016721707578, 1.6817722498272654, 1.6743880019018555, 1.6802689445213475, 1.5851666171655567, 1.5975174049151986, 1.6167793367661132, 1.6330824379707247, 1.7428298288839013, 1.7230950912005611, 1.6874959779216525, 1.5952085477133044, 1.570555641565696, 1.6725519105749374, 1.5753366973592298, 1.5750894857320685, 1.6149840024935675, 1.7256395674710492, 1.8025345131641386, 1.7555205234494662, 1.8295022430418362, 1.842410702065901, 1.821237008851251, 1.7875531864195084, 1.848491307756238, 1.8275088059198399, 1.82599200880849, 1.7248824118476518, 1.7186463497287763, 1.837899426721065, 1.7974276921658194, 1.7002204352229915, 1.7902109328402156, 1.7401059875517446, 1.682157141210278, 1.7146389806387219, 1.7231989166306991, 1.7311545693966048, 1.7336194785016605, 1.6681173822731488, 1.7117018544415883, 1.734954775247507, 1.778975371726841, 1.7125901150747156, 1.75734884519827, 1.7373049023072173, 1.7580902055393481, 1.7228927189568348, 1.6891412888515243, 1.6922367500330113, 1.7250365016550917, 1.6536148023263402, 1.6583462427067015, 1.667610250437327], [0.7513564109080847, 1.2636409273441025, 1.5997429325074861, 1.8505605219913215, 1.9662670835928524, 1.9900075228192033, 2.0635292895467168, 2.155404547614531, 2.1517546790334308, 2.1550127509590613, 2.0378726925225306, 2.0539338987457163, 2.0632139342273135, 2.1188322963826547, 2.252953617361027, 2.2156901824696953, 2.1925841681495952, 2.090718266232921, 2.0288921535288007, 2.16612194994977, 2.0258228295415903, 2.049580916993541, 2.105245254946718, 2.2035535176863066, 2.353016101990068, 2.287197114668708, 2.344266960993375, 2.3637828863993913, 2.309784572082543, 2.2871959481889714, 2.3489340701991934, 2.345135262080998, 2.33867531090955, 2.203108276050018, 2.2222777970137417, 2.3759255476769034, 2.3005123571553088, 2.1490201088883216, 2.2760797674914452, 2.2084000073075374, 2.1463679407322247, 2.1994741456254348, 2.2005584321650504, 2.249783727799772, 2.2336403137304424, 2.1291693820827997, 2.1901471840120785, 2.2277386188243753, 2.278854761461309, 2.179520112174684, 2.2356178345610944, 2.263441833012177, 2.2832821257877614, 2.2353766467931053, 2.1950942448109005, 2.2193046861627375, 2.240433915638346, 2.1414084971355494, 2.1567161670025286, 2.1435377403156397], [9395803734297.346, 26981225775886.45, 38331914268170.79, 29834306011192.504, 34018048858059.707, 28045124347061.754, 4509.874655870728, 5408.881454763695, 32844542167439.04, 4804.913220677426, 38112847093521.15, 32838432236166.375, 51605636099401.35, 45037071655730.74, 28365434726301.43, 51373242542539.45, 4471.71377916425, 33916495652110.902, 37677720067441.48, 44254099108869.52, 34608487808015.207, 43060727991315.51, 39050750096195.21, 5184.27981681108, 5348.410679723613, 51419959864120.86, 25662819060236.63, 28426773034458.074, 44345028418417.445, 36719227904152.4, 46380874572057.0, 42529110600033.086, 44704332426681.74, 54117678616534.4, 44579161507100.195, 38105459370076.87, 36839873740231.375, 45995762829398.47, 40498592444910.42, 45768453617641.23, 4454.305124371979, 44781561934857.57, 27715359505249.84, 5780.700710918484, 36527938203501.445, 38172526769123.9, 32743811615338.344, 35330948388197.086, 43428126680615.16, 33165240916172.793, 3715.6186170752085, 28337830464418.93, 38071135142848.57, 32111710435334.977, 40823623304927.414, 38698660944854.25, 36105145864453.53, 38193235601758.5, 3643.7653501498494, 49935034072365.234]]</t>
         </is>
       </c>
       <c r="H181" t="n">
-        <v>327.5309414863586</v>
+        <v>324.4310398101807</v>
       </c>
     </row>
     <row r="182">
@@ -6626,7 +6626,7 @@
         </is>
       </c>
       <c r="H182" t="n">
-        <v>69.11024856567383</v>
+        <v>70.65718674659729</v>
       </c>
     </row>
     <row r="183">
@@ -6660,7 +6660,7 @@
         </is>
       </c>
       <c r="H183" t="n">
-        <v>67.97270059585571</v>
+        <v>69.53059458732605</v>
       </c>
     </row>
     <row r="184">
@@ -6694,7 +6694,7 @@
         </is>
       </c>
       <c r="H184" t="n">
-        <v>68.87146806716919</v>
+        <v>69.42592835426331</v>
       </c>
     </row>
     <row r="185">
@@ -6705,7 +6705,7 @@
         <v>20</v>
       </c>
       <c r="C185" t="n">
-        <v>7.000000000000001</v>
+        <v>7</v>
       </c>
       <c r="D185" t="inlineStr">
         <is>
@@ -6728,7 +6728,7 @@
         </is>
       </c>
       <c r="H185" t="n">
-        <v>72.6257107257843</v>
+        <v>73.60163688659668</v>
       </c>
     </row>
     <row r="186">
@@ -6739,7 +6739,7 @@
         <v>20</v>
       </c>
       <c r="C186" t="n">
-        <v>7.000000000000001</v>
+        <v>7</v>
       </c>
       <c r="D186" t="inlineStr">
         <is>
@@ -6762,7 +6762,7 @@
         </is>
       </c>
       <c r="H186" t="n">
-        <v>72.81003928184509</v>
+        <v>73.69893550872803</v>
       </c>
     </row>
     <row r="187">
@@ -6773,7 +6773,7 @@
         <v>20</v>
       </c>
       <c r="C187" t="n">
-        <v>7.000000000000001</v>
+        <v>7</v>
       </c>
       <c r="D187" t="inlineStr">
         <is>
@@ -6796,7 +6796,7 @@
         </is>
       </c>
       <c r="H187" t="n">
-        <v>72.46509504318237</v>
+        <v>73.55613923072815</v>
       </c>
     </row>
     <row r="188">
@@ -6830,7 +6830,7 @@
         </is>
       </c>
       <c r="H188" t="n">
-        <v>84.66568803787231</v>
+        <v>85.48549008369446</v>
       </c>
     </row>
     <row r="189">
@@ -6864,7 +6864,7 @@
         </is>
       </c>
       <c r="H189" t="n">
-        <v>84.81693720817566</v>
+        <v>85.82599282264709</v>
       </c>
     </row>
     <row r="190">
@@ -6898,7 +6898,7 @@
         </is>
       </c>
       <c r="H190" t="n">
-        <v>84.73835253715515</v>
+        <v>85.56319236755371</v>
       </c>
     </row>
     <row r="191">
@@ -6932,7 +6932,7 @@
         </is>
       </c>
       <c r="H191" t="n">
-        <v>324.2212653160095</v>
+        <v>322.4668703079224</v>
       </c>
     </row>
     <row r="192">
@@ -6966,7 +6966,7 @@
         </is>
       </c>
       <c r="H192" t="n">
-        <v>326.3231692314148</v>
+        <v>323.1975317001343</v>
       </c>
     </row>
     <row r="193">
@@ -7000,7 +7000,7 @@
         </is>
       </c>
       <c r="H193" t="n">
-        <v>325.969710111618</v>
+        <v>321.1692624092102</v>
       </c>
     </row>
     <row r="194">
@@ -7034,7 +7034,7 @@
         </is>
       </c>
       <c r="H194" t="n">
-        <v>68.11950635910034</v>
+        <v>69.74126482009888</v>
       </c>
     </row>
     <row r="195">
@@ -7068,7 +7068,7 @@
         </is>
       </c>
       <c r="H195" t="n">
-        <v>68.4783775806427</v>
+        <v>69.3146665096283</v>
       </c>
     </row>
     <row r="196">
@@ -7102,7 +7102,7 @@
         </is>
       </c>
       <c r="H196" t="n">
-        <v>68.23014163970947</v>
+        <v>69.55644679069519</v>
       </c>
     </row>
     <row r="197">
@@ -7113,7 +7113,7 @@
         <v>40</v>
       </c>
       <c r="C197" t="n">
-        <v>7.000000000000001</v>
+        <v>7</v>
       </c>
       <c r="D197" t="inlineStr">
         <is>
@@ -7136,7 +7136,7 @@
         </is>
       </c>
       <c r="H197" t="n">
-        <v>72.28749251365662</v>
+        <v>73.88552761077881</v>
       </c>
     </row>
     <row r="198">
@@ -7147,7 +7147,7 @@
         <v>40</v>
       </c>
       <c r="C198" t="n">
-        <v>7.000000000000001</v>
+        <v>7</v>
       </c>
       <c r="D198" t="inlineStr">
         <is>
@@ -7170,7 +7170,7 @@
         </is>
       </c>
       <c r="H198" t="n">
-        <v>72.3434956073761</v>
+        <v>73.6018853187561</v>
       </c>
     </row>
     <row r="199">
@@ -7181,7 +7181,7 @@
         <v>40</v>
       </c>
       <c r="C199" t="n">
-        <v>7.000000000000001</v>
+        <v>7</v>
       </c>
       <c r="D199" t="inlineStr">
         <is>
@@ -7204,7 +7204,7 @@
         </is>
       </c>
       <c r="H199" t="n">
-        <v>72.55155563354492</v>
+        <v>73.62861847877502</v>
       </c>
     </row>
     <row r="200">
@@ -7238,7 +7238,7 @@
         </is>
       </c>
       <c r="H200" t="n">
-        <v>85.27397799491882</v>
+        <v>85.90097451210022</v>
       </c>
     </row>
     <row r="201">
@@ -7272,7 +7272,7 @@
         </is>
       </c>
       <c r="H201" t="n">
-        <v>84.75529932975769</v>
+        <v>86.43465352058411</v>
       </c>
     </row>
     <row r="202">
@@ -7306,7 +7306,7 @@
         </is>
       </c>
       <c r="H202" t="n">
-        <v>84.81388211250305</v>
+        <v>85.64972877502441</v>
       </c>
     </row>
     <row r="203">
@@ -7331,16 +7331,16 @@
       </c>
       <c r="F203" t="inlineStr">
         <is>
-          <t>[[5.0711823, 1.159384, 1.2456795, 1.4876317, 1.4165751, 1.4662161, 1.4365265, 1.5952394, 1.5289392, 1.5594518, 1.4599717, 1.5764911, 1.4233754, 1.5141997, 1.4903978, 1.4998314, 1.4181112, 1.3669623, 1.3642582, 1.4378655, 1.353877, 1.4257189, 1.5045707, 1.5894932, 1.5214316, 1.5291072, 1.5280479, 1.6919796, 1.6353041, 1.7149998, 1.7442887, 1.8088688, 1.685203, 1.6578163, 1.6499692, 1.7114525, 1.5311173, 1.4960647, 1.4754682, 1.5480171, 1.4004463, 1.5001459, 1.4507941, 1.5542467, 1.4687843, 1.6277254, 1.548513, 1.5917411, 1.514022, 1.6397824, 1.5761447, 1.6030293, 1.4952117, 1.5582864, 1.5186424, 1.5006459, 1.4425863, 1.575451, 1.506432, 1.5307708], [7.1056341033536325, 1.5851680599128044, 1.6866668481160747, 1.9507596150314928, 1.8372473406791257, 1.9028827130912442, 1.9036221761490297, 2.135865538026001, 2.040452622147537, 2.066752702193745, 1.9777400312619713, 2.129960049536627, 1.9272405886710393, 1.9974196000324393, 2.000205387059935, 2.0102217057590765, 1.88651718421387, 1.8354566877882414, 1.8618693570566605, 1.9557049000974709, 1.8204519193901159, 1.8716834936747144, 2.0000776037419126, 2.139233101839902, 2.0233041137562995, 2.0147767167109816, 2.067244880554599, 2.2576928552520172, 2.179502527188654, 2.306871006997579, 2.4795253611715924, 2.544913537106209, 2.352600983611977, 2.250067497936401, 2.268051006153987, 2.3661379863909224, 2.0925761106223972, 1.9982651100040802, 2.010551751165886, 2.0758414664990354, 1.8578651773670094, 1.9514360984017975, 1.9695112784983493, 2.1426569073084294, 2.0064648807284007, 2.2269317856110664, 2.162797578832655, 2.1337919676038575, 2.0516184814438816, 2.2051965159689844, 2.1147868492270265, 2.1437351993683795, 2.0194699778014664, 2.0640569647831013, 2.0652603404644325, 1.968237189459687, 1.8796425247202444, 2.050343959144309, 2.0216128101183033, 2.026626254147277], [1.889838, 0.31851566, 0.34751835, 0.36384037, 0.40009993, 0.38307154, 0.3574665, 0.38631222, 0.52374446, 0.57190543, 0.47763857, 0.58462095, 0.5093024, 0.4889275, 0.43022224, 0.41487065, 0.38326368, 0.3007576, 0.31865358, 0.37798837, 0.35343736, 0.3344223, 0.38408718, 0.4415596, 0.355084, 0.32901186, 0.40108544, 0.35614237, 0.40294072, 0.3274203, 0.39813116, 0.4018105, 0.4579487, 0.41709253, 0.43291432, 0.44063565, 0.49796346, 0.4222278, 0.4766678, 0.4415863, 0.40722218, 0.29923674, 0.43005556, 0.46550325, 0.50187033, 0.42177245, 0.5026973, 0.45206335, 0.4340111, 0.35274863, 0.4806279, 0.5180155, 0.4199667, 0.42732897, 0.42035496, 0.36849716, 0.37749028, 0.46218646, 0.46940914, 0.5263209]]</t>
+          <t>[[5.0711823, 1.1593369, 1.2486655, 1.4734718, 1.4436296, 1.4817349, 1.4290961, 1.5836864, 1.5096953, 1.5435574, 1.4741697, 1.593404, 1.402348, 1.5129291, 1.4738191, 1.4843282, 1.4158975, 1.3743398, 1.3672783, 1.4411916, 1.3663287, 1.442285, 1.524138, 1.567174, 1.4831637, 1.51706, 1.512722, 1.6938776, 1.6480135, 1.7418889, 1.7539574, 1.8231485, 1.6902127, 1.6073045, 1.6065587, 1.6440456, 1.495258, 1.4874706, 1.4953485, 1.567288, 1.4083824, 1.4872023, 1.422947, 1.5206251, 1.4025422, 1.5655601, 1.4779899, 1.5260897, 1.4646095, 1.5889225, 1.5614586, 1.5909965, 1.4871025, 1.5431554, 1.5060335, 1.4890132, 1.4339058, 1.5658946, 1.4554161, 1.4679248], [7.1056341033536325, 1.5851624196826937, 1.6931520398903745, 1.9280055820574225, 1.879363513907628, 1.9151237192851163, 1.9126612302348989, 2.1215425301091106, 2.002978134127339, 2.056725365323002, 2.0130133453927344, 2.1746646885717684, 1.9043775022995437, 1.9755153973403459, 1.9912260839794516, 1.9835979712532625, 1.891665211927664, 1.84651655407573, 1.8505916706086987, 1.9618210340881375, 1.8178082705535923, 1.904578241933848, 2.0194342053116063, 2.0992551708859635, 1.991946815462477, 2.016362255019975, 2.048689409329398, 2.2579330887320195, 2.207340509133219, 2.344901755578824, 2.489584110105598, 2.5783547039005272, 2.386865090037208, 2.2183984827247603, 2.2005792072085217, 2.264550842314108, 2.04378865056719, 1.9805107037014964, 2.034529166525602, 2.0977453571623257, 1.8727412924237556, 1.9303822367173773, 1.9263736827237654, 2.0911157462559316, 1.9131703691608168, 2.1386850295685624, 2.0361506106836025, 2.028552332736425, 1.968526857839641, 2.1392074680734408, 2.102878541378469, 2.1185951198807245, 1.992260321987821, 2.021215094723212, 2.0348804601852297, 1.9452025600757732, 1.8620211580961243, 2.0314889620556893, 1.9422314001325296, 1.9385563216628272], [1.889838, 0.3185654, 0.34626693, 0.35512275, 0.4139158, 0.39938676, 0.37097046, 0.3879315, 0.54088676, 0.5799143, 0.51615274, 0.6130018, 0.5524462, 0.51504207, 0.45305687, 0.39972663, 0.38081273, 0.30397362, 0.32214665, 0.38318056, 0.36509192, 0.33851534, 0.36867306, 0.43121338, 0.33900887, 0.33631805, 0.39107195, 0.35470307, 0.41468874, 0.33250126, 0.4076099, 0.41306284, 0.45191583, 0.3998563, 0.42706615, 0.4178427, 0.45277146, 0.39111438, 0.4701228, 0.45285723, 0.38942227, 0.28929627, 0.4257413, 0.46099454, 0.481965, 0.39811686, 0.45483938, 0.41727075, 0.42412177, 0.3413999, 0.45622647, 0.4943621, 0.43607324, 0.40887284, 0.41325763, 0.36354753, 0.3800988, 0.4512068, 0.4406714, 0.512848]]</t>
         </is>
       </c>
       <c r="G203" t="inlineStr">
         <is>
-          <t>[[0.9844370079508789, 0.9127901648325687, 1.0478243953898971, 1.1722499636115087, 1.265794302432729, 1.2595158949725753, 1.23059210682055, 1.3177674073084678, 1.3569600280102223, 1.3089150645889434, 1.244952013554432, 1.2904105727705288, 1.2539380752087947, 1.247087151355226, 1.2298829919406953, 1.2173255033521577, 1.2482982992912846, 1.172436486745442, 1.1696004621536151, 1.1816509862028879, 1.2035089295794577, 1.2072853376563224, 1.264746862419461, 1.2770312345923711, 1.292585432512203, 1.2724393240367515, 1.2773983986400346, 1.351150351529783, 1.4128477990419184, 1.417295031095038, 1.447014813184835, 1.4268627526725783, 1.4775453367158033, 1.3961713031573932, 1.3685066118969738, 1.3714616894673521, 1.3607417291922383, 1.255141485766848, 1.2180449647740506, 1.2425901542275501, 1.251530503249748, 1.2663303392875065, 1.2568830226734307, 1.2678283185905994, 1.2985124235006595, 1.3717037049826142, 1.3197779496136213, 1.263428172478178, 1.3316273861853378, 1.357148075858435, 1.3105009137351933, 1.3047221483969458, 1.32678732339379, 1.3109066139888392, 1.2747624486430498, 1.2298198522199386, 1.289285479863892, 1.3502566742465338, 1.2746987215422831, 1.2587076254518563], [1.3722988821198931, 1.2374845186961207, 1.3855834549463493, 1.5211417561647453, 1.6348478279368903, 1.6373661195350642, 1.6217561943313776, 1.7394828330680248, 1.780465638566941, 1.7226841380674858, 1.6522177967075615, 1.7313267131731624, 1.6743107941377435, 1.6237336134462323, 1.6250464645383313, 1.6060354743614167, 1.6552934280276979, 1.566058167476466, 1.5688766767792408, 1.5851022176063987, 1.589722095113126, 1.576577747973223, 1.6502666561832793, 1.6823610870461179, 1.6886182872551103, 1.6618061156291906, 1.6790612730917236, 1.7656155681315229, 1.8490658800557358, 1.8758856887254798, 2.0018013700583217, 1.9742300589669655, 2.0438559914508914, 1.8912458184901377, 1.8315056135325025, 1.867418651457664, 1.807767273588613, 1.6695745233255497, 1.6217067575091246, 1.6496980899768223, 1.6409997364604996, 1.6262379828063223, 1.6681696719240653, 1.7263974824698458, 1.7652411545775546, 1.8761256877151795, 1.8179857115767335, 1.7007110674911048, 1.7717787848288737, 1.8061800848762086, 1.7448530690068933, 1.7383527251059956, 1.763426641322936, 1.7218750293737575, 1.7115217292727374, 1.6138985842519986, 1.6607003543594363, 1.755511681940193, 1.6954409970748847, 1.657413467009789], [0.2411120669784347, 0.25761502663614805, 0.2948413716035007, 0.30292742019011987, 0.35856819856440175, 0.3334183343681388, 0.30368858215918726, 0.31774326853829854, 0.46351766830805624, 0.46136126682926226, 0.3904535324221452, 0.46576332464951586, 0.4294338590704799, 0.37370812851904683, 0.3639003700667538, 0.33589432219346965, 0.3319611663793007, 0.24747491843005964, 0.27491160172640206, 0.305667965126761, 0.3180421865050654, 0.30501971703803027, 0.31504187363004876, 0.3437592826683894, 0.2881934364221265, 0.28180083387320365, 0.3496115218964144, 0.2801191777017628, 0.3460841483595594, 0.2811452536491045, 0.32786649180994565, 0.3214918046819616, 0.3834123664151832, 0.3605208101322902, 0.35811911457659573, 0.34854386966635953, 0.43808663300090944, 0.3668089015790859, 0.39182604906952995, 0.3583268422985761, 0.35529301334725066, 0.2617048971115138, 0.357008320277521, 0.3830753560929466, 0.4385254976882706, 0.35711053605058385, 0.4018621347025249, 0.3636306855687698, 0.37159094860216335, 0.29761769830052304, 0.3872669460332672, 0.3910782562787684, 0.3790271988354242, 0.3508698568780554, 0.3496003567675299, 0.2939318620756401, 0.32844381775306447, 0.3968340327886569, 0.41732793146760205, 0.4132704882261714]]</t>
+          <t>[[0.9844370079508789, 0.8983214633696543, 1.0195132329257726, 1.1851237727462762, 1.274706507079229, 1.261747630063901, 1.217002411878831, 1.3138010142704648, 1.3403397738380305, 1.2997825837719448, 1.2636573943956981, 1.286164327889348, 1.2446311790567741, 1.2672825437101456, 1.191478891259668, 1.1998806400208333, 1.2419301971946695, 1.1772989420381321, 1.1740678781302987, 1.194225020755301, 1.217098113120839, 1.2308663844696623, 1.2196621192483863, 1.2422846392871787, 1.28441266928769, 1.2597485900889194, 1.2534845612002197, 1.3553013445155253, 1.4302896293147898, 1.4172568258273666, 1.4645807203061472, 1.4277477394316633, 1.4458790767594318, 1.3368003882535004, 1.3115154671133895, 1.3098421409071554, 1.3306931898893644, 1.2661379688698824, 1.2376053893623657, 1.2616349217415623, 1.2371921156639463, 1.2253917771426361, 1.1974864591944234, 1.214085927863683, 1.2595422959576223, 1.298785215355218, 1.2408602971640996, 1.237430623089731, 1.278727282014488, 1.2961965170590475, 1.2703781054545866, 1.2823902906149822, 1.301705041340722, 1.2847113964330619, 1.245999959010312, 1.217092193344768, 1.294501248558604, 1.3120958530668954, 1.2006169814624106, 1.186694849703347], [1.3722988821198931, 1.2199445969582279, 1.350524083924265, 1.5382459487999998, 1.6495898506198883, 1.6372656626072877, 1.60703176486246, 1.725282661165741, 1.7665302131607792, 1.7243706903147176, 1.699474575800942, 1.725373117004816, 1.6597668722482826, 1.6384352296719022, 1.5609952965620342, 1.587426323381402, 1.646299242064341, 1.5759019761983488, 1.5658525362855131, 1.5878013608805315, 1.5992377406908695, 1.6065161199211022, 1.59343069473326, 1.650085456614914, 1.6823680810639936, 1.6507837198148971, 1.6398024136425031, 1.7819199105968366, 1.872764615327044, 1.8980609353497193, 2.050124017833079, 2.0195034603738415, 2.029330162712259, 1.8356198715126102, 1.745944449506625, 1.7695364024283977, 1.7806385523763917, 1.6781037267353072, 1.6638507221901782, 1.6735725993182187, 1.6159091635842642, 1.5726446559536902, 1.6048934243499071, 1.6369332895480764, 1.697731949154252, 1.7478641111242048, 1.6860990939720608, 1.636962921610507, 1.7059262511342494, 1.744531346098607, 1.6801593950950402, 1.6877827152794682, 1.7070833269909853, 1.6910342389451005, 1.664782074591365, 1.5836117190170784, 1.6704510472962857, 1.6980889872277125, 1.5775253972385705, 1.5517146751078639], [0.2411120669784347, 0.2508047109394108, 0.28483219193701365, 0.3032151832552028, 0.3617720067165348, 0.346393806459791, 0.30767624719465786, 0.32515197707655014, 0.48533702497436376, 0.4894674002093942, 0.4358148490800201, 0.4822671010867831, 0.4667234493797014, 0.4068974364982126, 0.3622092602400084, 0.32081962228446576, 0.3215621545621991, 0.25199759777650343, 0.2728122169748271, 0.3124465057712337, 0.3253944913267065, 0.3017459274276147, 0.30128794776997514, 0.3269177163669378, 0.30217819666487133, 0.2875772647534676, 0.32494020881066643, 0.2946435759313731, 0.35783801477480925, 0.2764624838517834, 0.3284424187770792, 0.3429167021593431, 0.37930523173836633, 0.3438247385713976, 0.348880349724538, 0.3141292750430828, 0.39255846427264185, 0.34906388297096674, 0.38697383853380674, 0.36444022826803313, 0.3302708404580658, 0.24246222262181902, 0.3604490344112831, 0.353544969906912, 0.4167087256256956, 0.3364054217914134, 0.36764090867356497, 0.3385762092381336, 0.36273143904707783, 0.27777600814314374, 0.3479351137889147, 0.3955028909593998, 0.3739313275939315, 0.3405699255861498, 0.33209516091664265, 0.27682051776788863, 0.3236090984324118, 0.37710480771950655, 0.37298896146119276, 0.37932571866876663]]</t>
         </is>
       </c>
       <c r="H203" t="n">
-        <v>325.7150530815125</v>
+        <v>321.4461724758148</v>
       </c>
     </row>
     <row r="204">
@@ -7374,7 +7374,7 @@
         </is>
       </c>
       <c r="H204" t="n">
-        <v>325.5139963626862</v>
+        <v>321.0416054725647</v>
       </c>
     </row>
     <row r="205">
@@ -7408,7 +7408,7 @@
         </is>
       </c>
       <c r="H205" t="n">
-        <v>324.9640040397644</v>
+        <v>323.1704525947571</v>
       </c>
     </row>
     <row r="206">
@@ -7442,7 +7442,7 @@
         </is>
       </c>
       <c r="H206" t="n">
-        <v>69.0746111869812</v>
+        <v>70.23433017730713</v>
       </c>
     </row>
     <row r="207">
@@ -7476,7 +7476,7 @@
         </is>
       </c>
       <c r="H207" t="n">
-        <v>68.9776337146759</v>
+        <v>70.42535138130188</v>
       </c>
     </row>
     <row r="208">
@@ -7510,7 +7510,7 @@
         </is>
       </c>
       <c r="H208" t="n">
-        <v>72.30320405960083</v>
+        <v>73.20618987083435</v>
       </c>
     </row>
     <row r="209">
@@ -7521,7 +7521,7 @@
         <v>60</v>
       </c>
       <c r="C209" t="n">
-        <v>7.000000000000001</v>
+        <v>7</v>
       </c>
       <c r="D209" t="inlineStr">
         <is>
@@ -7544,7 +7544,7 @@
         </is>
       </c>
       <c r="H209" t="n">
-        <v>85.85925722122192</v>
+        <v>81.55287599563599</v>
       </c>
     </row>
     <row r="210">
@@ -7555,7 +7555,7 @@
         <v>60</v>
       </c>
       <c r="C210" t="n">
-        <v>7.000000000000001</v>
+        <v>7</v>
       </c>
       <c r="D210" t="inlineStr">
         <is>
@@ -7578,7 +7578,7 @@
         </is>
       </c>
       <c r="H210" t="n">
-        <v>82.84956192970276</v>
+        <v>75.50188159942627</v>
       </c>
     </row>
     <row r="211">
@@ -7589,7 +7589,7 @@
         <v>60</v>
       </c>
       <c r="C211" t="n">
-        <v>7.000000000000001</v>
+        <v>7</v>
       </c>
       <c r="D211" t="inlineStr">
         <is>
@@ -7612,7 +7612,7 @@
         </is>
       </c>
       <c r="H211" t="n">
-        <v>74.40022397041321</v>
+        <v>74.5383198261261</v>
       </c>
     </row>
     <row r="212">
@@ -7637,16 +7637,16 @@
       </c>
       <c r="F212" t="inlineStr">
         <is>
-          <t>[[5.076458, 1.2991183, 1.295927, 1.5152006, 1.4764956, 1.5292184, 1.4834211, 1.6522456, 1.5693568, 1.6144571, 1.5116315, 1.6044054, 1.4748893, 1.601777, 1.5872883, 1.6199266, 1.5149225, 1.4646176, 1.4225833, 1.459795, 1.392708, 1.4831175, 1.5339648, 1.6384567, 1.5872693, 1.6119349, 1.6047798, 1.7754213, 1.7242755, 1.845734, 1.8718954, 1.9132279, 1.8310722, 1.7937917, 1.7325113, 1.7957686, 1.5714431, 1.5342029, 1.5403432, 1.6084962, 1.4810398, 1.5378976, 1.524626, 1.5730681, 1.4878999, 1.6558167, 1.5498605, 1.5898772, 1.551383, 1.6854748, 1.6476039, 1.6935511, 1.5821201, 1.6153505, 1.6097351, 1.6082501, 1.5301684, 1.6228417, 1.5396835, 1.5501], [7.11399312361502, 1.8471267941650715, 1.808558618191957, 2.0297203760222953, 1.9554046144838169, 1.9935768817612833, 1.9834810781612477, 2.2219626579752143, 2.105253247501236, 2.1401840089851327, 2.0610915490130677, 2.1782977961954404, 2.001918587735622, 2.110741857671796, 2.164811868752919, 2.206819399228067, 1.9979883448286597, 1.9444895769361255, 1.9292658912841592, 1.97516579716743, 1.8547913288469067, 1.9519226035189443, 2.0382167187465923, 2.2111855088097236, 2.137530352282159, 2.136104739603639, 2.1841047913908826, 2.39122799517751, 2.3293520362895053, 2.469838928345372, 2.701206562870413, 2.7125622720206524, 2.5990975647799597, 2.4714452782341074, 2.414093609952001, 2.4800013785204595, 2.1574471508992614, 2.074148058360171, 2.106062371927057, 2.1616989063142116, 1.9623176003994987, 2.0220332041050706, 2.0859381857881596, 2.178755366044651, 2.010704599689655, 2.254889050818298, 2.187657922766317, 2.1362576449164243, 2.1068873677757822, 2.282338235560778, 2.2268227943727004, 2.262778025874094, 2.1485617861777766, 2.18738719104352, 2.2028140667041063, 2.146066696168667, 2.0121634871342584, 2.114434398298285, 2.067048922944837, 2.0688047280808517], [1.8977177, 0.34714296, 0.31734908, 0.37246463, 0.4202499, 0.4227581, 0.38706586, 0.39483353, 0.5391655, 0.58785856, 0.50514174, 0.60535365, 0.54557776, 0.55441546, 0.48792794, 0.44429868, 0.40618387, 0.3122942, 0.3342226, 0.3820515, 0.36189663, 0.34845462, 0.37427947, 0.44484225, 0.3508412, 0.3251019, 0.3832132, 0.35026774, 0.40884823, 0.3372362, 0.39322746, 0.42690924, 0.48059323, 0.4594382, 0.46483353, 0.47148144, 0.5250969, 0.45789596, 0.5142458, 0.47313598, 0.42410627, 0.32157207, 0.47207972, 0.47669804, 0.5026328, 0.42816347, 0.48990673, 0.4565635, 0.4411445, 0.3709147, 0.5014748, 0.5175003, 0.4634287, 0.44893184, 0.45652872, 0.4036688, 0.40721726, 0.49875578, 0.4799121, 0.54266673]]</t>
+          <t>[[5.0766263, 1.3038175, 1.2926126, 1.5195786, 1.4932599, 1.5466598, 1.4898875, 1.6479254, 1.5796027, 1.6318345, 1.5384159, 1.6178603, 1.5020645, 1.6242334, 1.5828598, 1.6062071, 1.4888827, 1.4602925, 1.4502631, 1.4765972, 1.4147371, 1.4789792, 1.5366557, 1.6106453, 1.5244908, 1.5651706, 1.5786432, 1.7636223, 1.7056079, 1.7853991, 1.8405352, 1.8796682, 1.8122057, 1.8113439, 1.7480792, 1.7957191, 1.59957, 1.5438664, 1.5758651, 1.6370151, 1.4914294, 1.5928838, 1.5449431, 1.6008004, 1.4765298, 1.6309657, 1.5561672, 1.6038592, 1.5656722, 1.7179698, 1.7052654, 1.7372615, 1.6099324, 1.649786, 1.6033171, 1.5859858, 1.528845, 1.6206867, 1.536532, 1.5427098], [7.114197958417571, 1.8590169609982845, 1.8084797174414804, 2.0445876991604215, 1.9744623055858015, 2.021929204529645, 1.9972923547100223, 2.204687551907999, 2.134924098325074, 2.200801408625949, 2.1310593103025313, 2.2103175719613004, 2.0427882039978646, 2.1593654074780155, 2.1688376944893415, 2.181427619938157, 1.9903436243322212, 1.95858879316971, 1.9744978664770165, 2.0150015406448873, 1.8886979425755683, 1.954636866022724, 2.040510927432319, 2.15789345293166, 2.034493541633216, 2.075092138979353, 2.13856607811236, 2.3823915203491826, 2.299950441572906, 2.3714752141794113, 2.6106591633905447, 2.6653077020556113, 2.56541286618367, 2.481948435226996, 2.4153630478572166, 2.4589874776588845, 2.1812916530359363, 2.0833147683905895, 2.1754958891920713, 2.2110982775781656, 1.9915972863832563, 2.08283359891789, 2.106449953090913, 2.2236009678426285, 2.011185243843165, 2.209703404300959, 2.1513375978517226, 2.15164832426724, 2.1234197911975996, 2.339071665448392, 2.3270172965829437, 2.3511160493260816, 2.2142270691308683, 2.2638776683984374, 2.2163129505182724, 2.128200589040512, 1.9940056974698839, 2.12329178759993, 2.0555476139820184, 2.047387794149552], [1.897731, 0.34873992, 0.3176559, 0.36143184, 0.4080313, 0.41432235, 0.38779584, 0.40546045, 0.5581325, 0.5997551, 0.52878994, 0.6104512, 0.5653447, 0.57604164, 0.48875663, 0.4530192, 0.39320305, 0.3072695, 0.33099538, 0.37193245, 0.35067227, 0.337896, 0.36638948, 0.41884488, 0.3327824, 0.32217687, 0.39308122, 0.36126462, 0.43031946, 0.3409142, 0.40581328, 0.40721732, 0.4553583, 0.44282746, 0.45531502, 0.47529334, 0.52677494, 0.46302518, 0.51790136, 0.47125438, 0.42493093, 0.331635, 0.47539142, 0.4650119, 0.48980862, 0.42822382, 0.5053378, 0.4587685, 0.44061354, 0.36765543, 0.509576, 0.5350836, 0.47341293, 0.46972573, 0.45499125, 0.3906842, 0.3818469, 0.49373168, 0.5048567, 0.541305]]</t>
         </is>
       </c>
       <c r="G212" t="inlineStr">
         <is>
-          <t>[[1.2237736405072541, 1.0233500534914748, 1.1100466984831416, 1.2537597424392668, 1.3195267908279045, 1.334553394841056, 1.2891262503679963, 1.4074758700379628, 1.4242894589352604, 1.3781863476248717, 1.3069006353240862, 1.3716760580462957, 1.329346956531441, 1.3980783136396617, 1.3626086298618902, 1.3559536305665925, 1.345928895845568, 1.2821757707619021, 1.2445782835077663, 1.266576098182944, 1.2683026532682318, 1.299754050140463, 1.3266624234050413, 1.3975113693058325, 1.3967055007410234, 1.3869876172097237, 1.3666412853019267, 1.4661721880813723, 1.5200025314731302, 1.5761207986766992, 1.565589566307518, 1.572777838074296, 1.6344477487680455, 1.5347922230007869, 1.4806645305348578, 1.4774377588896728, 1.4135160550968309, 1.3431616854704345, 1.3254888279472954, 1.3396330253996938, 1.3013283486709846, 1.3632282490227372, 1.3061191264646625, 1.3377139281989703, 1.3564891918915225, 1.4302164152086598, 1.342245188292677, 1.3274187295003397, 1.3820813047159681, 1.444496200916258, 1.4170904985903328, 1.4209588239047055, 1.3939857398172333, 1.4038277594570403, 1.4004449740574092, 1.372956737228899, 1.374903523461911, 1.433260356606035, 1.3414269416746096, 1.3371496809061774], [1.76977680930259, 1.4286500303918992, 1.5313050051042028, 1.6689756043411201, 1.7315848138604637, 1.748075882967749, 1.6996672716594101, 1.8711513017424284, 1.895348622130457, 1.8215444933494265, 1.740187712662521, 1.864627393970789, 1.7855261196384362, 1.837399600220467, 1.8500705467253724, 1.7928149961891873, 1.766977059047108, 1.7041395740016967, 1.6645978409087012, 1.699698498691224, 1.6793542143785323, 1.710403647874349, 1.7413935442343729, 1.862485480869424, 1.8453906568486655, 1.8188803675173033, 1.8199900698693405, 1.938552996209774, 1.981591163224048, 2.1168667162919483, 2.213975010852859, 2.1969231114666905, 2.315717624144014, 2.109491757542024, 2.0046260133998826, 1.9982927381578202, 1.8984825162080197, 1.8065827696326202, 1.778158424170095, 1.7622366747059703, 1.7062388561384936, 1.7802902375371, 1.7472205454517837, 1.80465493357523, 1.824458215681113, 1.9584060212357879, 1.8506670002229566, 1.8008889447352139, 1.8541790315944662, 1.946808608770666, 1.8991483577563135, 1.8811978654228918, 1.883384100074113, 1.8752130226677162, 1.8969252171735917, 1.8129808273256143, 1.7844235668575295, 1.8630328967470564, 1.7970727270152898, 1.7677930346347919], [0.2867305145984586, 0.26059776696710824, 0.293246883091686, 0.3248536698922028, 0.38783419848686845, 0.3809952499144376, 0.3304692323207573, 0.33478169312061895, 0.4873146057535174, 0.48472552636592775, 0.42305557354708956, 0.5020561193267754, 0.4954109507854989, 0.4739834423210371, 0.4122497535012045, 0.3674880058972064, 0.3484986995349819, 0.2656058420081503, 0.2860060958313304, 0.3374010109237852, 0.32676602825674916, 0.31152571594454886, 0.3218183714269247, 0.34986006614230963, 0.30176471365509094, 0.27138872909538436, 0.3302737185355579, 0.30416722878098384, 0.35257701883351533, 0.2868252277825524, 0.34501891334129153, 0.3504804999105103, 0.424399505180073, 0.4003844917952218, 0.3974245393972608, 0.3849709466119819, 0.4628034550985559, 0.40982095852355016, 0.4289731793860013, 0.3924588400027801, 0.3845842113254057, 0.28718084972348035, 0.408086660189267, 0.4011859645246552, 0.4440676015066468, 0.35760641835930435, 0.4246328708706242, 0.3668726582245739, 0.39480618348359897, 0.31741977805190585, 0.40986562501711576, 0.43011298741286985, 0.39138277789186754, 0.3919561074794159, 0.38123516737002616, 0.32734385029593127, 0.3606210817009607, 0.43458518165403637, 0.40095996834924574, 0.44313564556631396]]</t>
+          <t>[[1.2272220092238504, 1.0138283391355325, 1.111891925652212, 1.2779808247749311, 1.3390178144120284, 1.3579274538632669, 1.2847334206938281, 1.4339490133277535, 1.4328488010016267, 1.4137455217518131, 1.3203727313568412, 1.3997019717179788, 1.3481894922186857, 1.3988690957808825, 1.3564569056133078, 1.3389841694336013, 1.348170474493849, 1.2814781974519653, 1.277675945574465, 1.283177020531747, 1.2714788268320671, 1.3012265009066772, 1.3006978458339757, 1.3260696189545957, 1.3336097130594167, 1.3461429920573935, 1.3570343437785157, 1.4203732873401875, 1.4779453979846158, 1.5245937865221393, 1.554398196913893, 1.5456665475310392, 1.6348658126829358, 1.5574391086213246, 1.4833020640678936, 1.5030699180850648, 1.4337044282730986, 1.3697837163842568, 1.345592281382086, 1.3891286911338132, 1.3363520511239173, 1.3932662867805812, 1.3256744748277056, 1.3329396325187248, 1.340053899687645, 1.398281812739351, 1.3642149686791076, 1.355717780066831, 1.4090155496913197, 1.4893761204374685, 1.4537458466667112, 1.4407846110294975, 1.4413356450641694, 1.418341090711023, 1.4072501410675284, 1.3396038335926133, 1.3863703739945292, 1.4191824173845486, 1.3365169468099436, 1.3532247912643733], [1.7806166666418457, 1.4275610592909127, 1.545793917058559, 1.7004185960072657, 1.7561895989748881, 1.7823310799607448, 1.7056661417032235, 1.9206013241523692, 1.9291076411441992, 1.9085663948096894, 1.7863435574474518, 1.9033341430749369, 1.8207537355167385, 1.8747770055036046, 1.8410306904759186, 1.7985199184214624, 1.785821531785063, 1.7258174447351926, 1.7265842324156453, 1.7341160191500118, 1.6875150977001772, 1.7114643525668756, 1.7006466157803344, 1.7561299773898293, 1.7556966799353824, 1.7704003930269738, 1.8116624612890486, 1.8808660797656231, 1.9189908824053177, 2.0258427360337703, 2.184522380605581, 2.17649967918295, 2.30948612323607, 2.1180946755491443, 1.9907529357763458, 2.0203154785962725, 1.93295768744402, 1.8542545631331715, 1.8245662699985676, 1.8439285482070034, 1.762881932172157, 1.8128505854027805, 1.774649534455988, 1.7993600306843014, 1.8170172122457118, 1.888778569383579, 1.8408442200985273, 1.8390107072988138, 1.8939893139592705, 2.01730034565293, 1.9723864829415247, 1.9510349373932427, 1.969325095000431, 1.9126069210536858, 1.9202433524243936, 1.7756504881198687, 1.7907244926434278, 1.8548969137212092, 1.775720020343794, 1.786480179410375], [0.2882473736837522, 0.25562979593664886, 0.28465025024748075, 0.3111359273835714, 0.37962713925622366, 0.37921086401761506, 0.3432837165896557, 0.35304313111380914, 0.49200484040890746, 0.5083891988983652, 0.42583683894454555, 0.49941406647477415, 0.5114041775770192, 0.4868366540931652, 0.4070383229850985, 0.3674875065464696, 0.3395711800011044, 0.26043497042152997, 0.28305623916723727, 0.32291243295583255, 0.3090998170933049, 0.2977822327787736, 0.3031097651844429, 0.32966492947401116, 0.2786866182782253, 0.2794268906119069, 0.34628787225582974, 0.30400714943170615, 0.3698667546146169, 0.2961148115055881, 0.34564779685504987, 0.32823923498190893, 0.40452744986857997, 0.3957905626968886, 0.3968981438670415, 0.39864807888660336, 0.4772621886505671, 0.4179751629592933, 0.4395455481462965, 0.383598642885595, 0.3808465355095681, 0.29195474715643704, 0.4008960343262424, 0.3824994425425919, 0.44039242817617713, 0.36272686535067766, 0.42269375019151745, 0.36973930467395055, 0.3952750913385202, 0.3157078686385773, 0.42250442713530867, 0.4441447139455274, 0.4244687793577605, 0.39092446526116914, 0.37967799789358675, 0.3034917765210935, 0.3477173579246804, 0.4372760778385014, 0.4175602742639977, 0.44718806277929984]]</t>
         </is>
       </c>
       <c r="H212" t="n">
-        <v>86.14155459403992</v>
+        <v>86.71411180496216</v>
       </c>
     </row>
     <row r="213">
@@ -7680,7 +7680,7 @@
         </is>
       </c>
       <c r="H213" t="n">
-        <v>86.16844844818115</v>
+        <v>86.8479642868042</v>
       </c>
     </row>
     <row r="214">
@@ -7714,7 +7714,7 @@
         </is>
       </c>
       <c r="H214" t="n">
-        <v>86.1387996673584</v>
+        <v>86.80755019187927</v>
       </c>
     </row>
     <row r="215">
@@ -7748,7 +7748,7 @@
         </is>
       </c>
       <c r="H215" t="n">
-        <v>327.4912667274475</v>
+        <v>323.8546886444092</v>
       </c>
     </row>
     <row r="216">
@@ -7782,7 +7782,7 @@
         </is>
       </c>
       <c r="H216" t="n">
-        <v>327.0921959877014</v>
+        <v>322.9021940231323</v>
       </c>
     </row>
     <row r="217">
@@ -7816,7 +7816,7 @@
         </is>
       </c>
       <c r="H217" t="n">
-        <v>328.8577075004578</v>
+        <v>325.094589471817</v>
       </c>
     </row>
     <row r="218">
@@ -7850,7 +7850,7 @@
         </is>
       </c>
       <c r="H218" t="n">
-        <v>69.44987010955811</v>
+        <v>70.79872536659241</v>
       </c>
     </row>
     <row r="219">
@@ -7884,7 +7884,7 @@
         </is>
       </c>
       <c r="H219" t="n">
-        <v>69.46473908424377</v>
+        <v>70.65080308914185</v>
       </c>
     </row>
     <row r="220">
@@ -7918,7 +7918,7 @@
         </is>
       </c>
       <c r="H220" t="n">
-        <v>69.48912477493286</v>
+        <v>71.07676339149475</v>
       </c>
     </row>
     <row r="221">
@@ -7929,7 +7929,7 @@
         <v>80</v>
       </c>
       <c r="C221" t="n">
-        <v>7.000000000000001</v>
+        <v>7</v>
       </c>
       <c r="D221" t="inlineStr">
         <is>
@@ -7952,7 +7952,7 @@
         </is>
       </c>
       <c r="H221" t="n">
-        <v>73.90432095527649</v>
+        <v>74.83955025672913</v>
       </c>
     </row>
     <row r="222">
@@ -7963,7 +7963,7 @@
         <v>80</v>
       </c>
       <c r="C222" t="n">
-        <v>7.000000000000001</v>
+        <v>7</v>
       </c>
       <c r="D222" t="inlineStr">
         <is>
@@ -7986,7 +7986,7 @@
         </is>
       </c>
       <c r="H222" t="n">
-        <v>73.9368155002594</v>
+        <v>75.41791963577271</v>
       </c>
     </row>
     <row r="223">
@@ -7997,7 +7997,7 @@
         <v>80</v>
       </c>
       <c r="C223" t="n">
-        <v>7.000000000000001</v>
+        <v>7</v>
       </c>
       <c r="D223" t="inlineStr">
         <is>
@@ -8020,7 +8020,7 @@
         </is>
       </c>
       <c r="H223" t="n">
-        <v>73.81151652336121</v>
+        <v>75.59369969367981</v>
       </c>
     </row>
     <row r="224">
@@ -8054,7 +8054,7 @@
         </is>
       </c>
       <c r="H224" t="n">
-        <v>86.15715456008911</v>
+        <v>87.35227465629578</v>
       </c>
     </row>
     <row r="225">
@@ -8088,7 +8088,7 @@
         </is>
       </c>
       <c r="H225" t="n">
-        <v>86.29781818389893</v>
+        <v>86.81513500213623</v>
       </c>
     </row>
     <row r="226">
@@ -8122,7 +8122,7 @@
         </is>
       </c>
       <c r="H226" t="n">
-        <v>86.56866669654846</v>
+        <v>87.55300331115723</v>
       </c>
     </row>
     <row r="227">
@@ -8147,16 +8147,16 @@
       </c>
       <c r="F227" t="inlineStr">
         <is>
-          <t>[[5.0775547, 1.136226, 1.2031386, 1.447394, 1.4107287, 1.4361873, 1.380189, 1.536635, 1.4653444, 1.5017005, 1.417064, 1.5069973, 1.3511528, 1.4527149, 1.4075888, 1.4148073, 1.3403214, 1.3186601, 1.3002543, 1.3594207, 1.2873391, 1.3709542, 1.4402242, 1.5167472, 1.4397411, 1.4571407, 1.473511, 1.6320794, 1.5807792, 1.6591994, 1.6959378, 1.7588676, 1.6694955, 1.6231275, 1.566462, 1.6088871, 1.4528394, 1.441017, 1.4364486, 1.5343707, 1.371303, 1.4724746, 1.3977903, 1.4813542, 1.3878736, 1.527375, 1.4478143, 1.4973543, 1.4376826, 1.575933, 1.5205454, 1.5308981, 1.4264444, 1.495066, 1.4783819, 1.4492421, 1.3963429, 1.513602, 1.4102892, 1.4072971], [7.11506710018169, 1.5431374759409222, 1.6236474203432094, 1.8984801362198815, 1.857466736260789, 1.871940851088125, 1.8426847451703772, 2.0556825034431165, 1.9569119780661268, 1.9994804184248844, 1.9221707248343358, 2.0346666212011075, 1.8284684209143804, 1.906104785828766, 1.9011376413304664, 1.907847626133879, 1.78047524719258, 1.7657755559686503, 1.7699719147690014, 1.8412936383765166, 1.7156480019839226, 1.802893535494134, 1.8985124110131906, 2.025002246431588, 1.920257383817331, 1.91941632806722, 2.0024584918536212, 2.1825051093287486, 2.111643270991708, 2.247443972558613, 2.444258587688207, 2.519618684892764, 2.3926956085632867, 2.2233384732935724, 2.1375937056497314, 2.2048936602842373, 1.9644864859093107, 1.8978980282965066, 1.9301534236941926, 2.0319063740059065, 1.788368523610854, 1.904467139824135, 1.8901688837356196, 2.031253990756296, 1.886225728762974, 2.0877105378295155, 2.0164270505604547, 2.002853741779942, 1.9477333417769374, 2.1294931145310625, 2.0650786261564598, 2.070172575054803, 1.9075863015986656, 1.9773254128415594, 2.000282267678896, 1.8910072507714222, 1.8078287372832549, 1.9789004765910896, 1.8796011101838979, 1.8543508273903002], [1.8978608, 0.31098658, 0.32330397, 0.34923047, 0.40179518, 0.37586397, 0.3399124, 0.38263854, 0.5191719, 0.54879034, 0.47067845, 0.54681146, 0.47311485, 0.49127623, 0.4338414, 0.3879275, 0.3542509, 0.28337196, 0.2954787, 0.34999105, 0.32637015, 0.31298655, 0.34011203, 0.402966, 0.33023313, 0.30809656, 0.3828551, 0.3397471, 0.3988228, 0.32563442, 0.3684566, 0.3803082, 0.43856594, 0.42662328, 0.40979168, 0.419058, 0.48614118, 0.41884696, 0.45340455, 0.4236091, 0.38800448, 0.29227152, 0.4256826, 0.426393, 0.463612, 0.39023718, 0.46815264, 0.4337041, 0.41543323, 0.3328133, 0.46079147, 0.47759667, 0.39786562, 0.40496144, 0.40246922, 0.34071377, 0.37651715, 0.45509624, 0.4388772, 0.47292602]]</t>
+          <t>[[5.0775547, 1.136226, 1.2031386, 1.4473175, 1.4273791, 1.4690738, 1.412972, 1.56653, 1.4988978, 1.504849, 1.4024364, 1.5098178, 1.3679144, 1.4813886, 1.4482784, 1.4399307, 1.3690507, 1.3206768, 1.3064191, 1.3541784, 1.3075198, 1.3908671, 1.4393094, 1.5029063, 1.4319364, 1.450898, 1.4552711, 1.6135024, 1.5745696, 1.6564429, 1.6930149, 1.7380071, 1.6589099, 1.6289873, 1.5750902, 1.614583, 1.4348971, 1.4358299, 1.4497385, 1.5349165, 1.4002103, 1.4934211, 1.4220556, 1.4903991, 1.3943057, 1.552033, 1.4701893, 1.4718845, 1.4628515, 1.5859196, 1.546907, 1.5399263, 1.4478297, 1.5076851, 1.4570857, 1.452203, 1.4109881, 1.5138105, 1.3843744, 1.4191589], [7.11506710018169, 1.5431374759409222, 1.6236474203432094, 1.8983948000277657, 1.8746867236049778, 1.9117814777467104, 1.875600972820932, 2.0794711234712615, 1.982557049732576, 1.998179560904672, 1.899006573818855, 2.036334672248131, 1.8484049725673468, 1.9390454435251547, 1.9469698544535816, 1.9440052588552608, 1.8118901377713688, 1.7770080249328248, 1.7767317504246156, 1.8355327403516153, 1.7328291181037494, 1.8300780598610915, 1.897477711884648, 1.9993280235560065, 1.8746542293892081, 1.9072753149970945, 1.9651546649391132, 2.1603840437081074, 2.098831160284191, 2.2344181083308725, 2.423487366508231, 2.4780925272368997, 2.363691310143873, 2.2336260200509686, 2.154458559527869, 2.2092326030678633, 1.9387996990393297, 1.9103121391606812, 1.975421923222924, 2.0662589065719805, 1.8505311177772554, 1.947441988412757, 1.937396508190812, 2.0597542490248038, 1.8860027463130433, 2.107924011764603, 2.0504119831236625, 1.9885787291658996, 1.9841843761287685, 2.1589811415809423, 2.113115060868085, 2.0751448753061847, 1.9492177714802152, 2.0073380559111684, 1.9654086990092507, 1.9093713064204825, 1.8286216256902401, 1.9650680990285248, 1.8314664901512994, 1.8704318028437592], [1.8978608, 0.31098658, 0.32330397, 0.34928724, 0.4032302, 0.3812522, 0.3462346, 0.38193914, 0.5224648, 0.55249447, 0.47490123, 0.5547281, 0.50228983, 0.4866019, 0.44438848, 0.39597455, 0.3608348, 0.27364066, 0.28992227, 0.33949897, 0.33561763, 0.3110543, 0.34224418, 0.3842101, 0.31854293, 0.30451056, 0.37736684, 0.34071153, 0.40115198, 0.31255808, 0.37359855, 0.384122, 0.45044392, 0.41832986, 0.41790304, 0.42026606, 0.48127216, 0.41294688, 0.45864883, 0.4398564, 0.39729428, 0.30296993, 0.4440454, 0.4378703, 0.46616143, 0.38960668, 0.4782645, 0.42969316, 0.40716934, 0.32666597, 0.4491153, 0.47617173, 0.4181293, 0.42498752, 0.40661436, 0.35585493, 0.36780232, 0.45615622, 0.43205804, 0.47385123]]</t>
         </is>
       </c>
       <c r="G227" t="inlineStr">
         <is>
-          <t>[[0.9335209502408268, 0.8458673356102864, 0.9735548074046748, 1.140363428408489, 1.2110037728168817, 1.1813469061044002, 1.1290113733437108, 1.2406808164779801, 1.2824865330019488, 1.2249741445094864, 1.1451806992827083, 1.1893018153130082, 1.1697982223940389, 1.1481351768240053, 1.1160278121294005, 1.1264728625479088, 1.1688692674333276, 1.0917970672541435, 1.0557731183466783, 1.0956514853462864, 1.1318550476342393, 1.1495664830437249, 1.1611226439011846, 1.1741043776633422, 1.210215361675747, 1.1746162838775827, 1.1851246157632302, 1.2566210046507833, 1.34374750238308, 1.3312156067936245, 1.3642364431312328, 1.3674117107221775, 1.4373120087560265, 1.3157225174244593, 1.2375563514002481, 1.2772188990731388, 1.269456103254271, 1.2008696028480654, 1.163925860530529, 1.1785683167363157, 1.202807623480517, 1.179782060426925, 1.1538139475863223, 1.175553396601411, 1.2147780851491425, 1.2393478811601555, 1.2173095075562865, 1.1755991442411544, 1.2573051918000515, 1.2714676264722775, 1.229998107603104, 1.1909999423710078, 1.242065731002334, 1.233037251930128, 1.197894028639131, 1.1596898922394876, 1.2325928307688252, 1.2302207686140383, 1.1240468171626363, 1.1254615358054683], [1.32038622003922, 1.1403177240756333, 1.2929347118172183, 1.5018939531087319, 1.5861408858151917, 1.5457561031598952, 1.4962498514434195, 1.63771900476754, 1.698246436179851, 1.6057975039648191, 1.5258062468364204, 1.595141164963214, 1.5727952382951436, 1.5005483962303061, 1.4841903441324715, 1.4948486748874952, 1.5447334723145374, 1.4591508961727737, 1.4195521818614314, 1.4773433532964841, 1.4981806665704893, 1.5023857942392367, 1.5108293387201261, 1.5568926581771199, 1.5709640983453819, 1.5417045856904934, 1.5846619984311192, 1.6488700744879146, 1.759092858245044, 1.7816636198652624, 1.9595507864619357, 1.951684341555855, 2.0336373754967636, 1.7678868770840321, 1.6345324380346167, 1.704252394617005, 1.660729299982112, 1.5720352365583754, 1.5390501970640555, 1.5380928590840317, 1.5602054742499185, 1.5213568227393035, 1.5406461726483753, 1.5948249820790998, 1.6322108905590724, 1.6768615368204058, 1.6623367255316708, 1.5530316654721095, 1.6880599903098765, 1.697698756598065, 1.6592839432265487, 1.577229585515514, 1.6361819675236466, 1.6291046923655241, 1.6126653972567653, 1.5199612269029716, 1.5933477871461206, 1.6048372062058702, 1.4729359529025923, 1.492234591891189], [0.22323357068688865, 0.21691194105956782, 0.2626416304545296, 0.2909630062936461, 0.34041450197520606, 0.31724354179551056, 0.2786307950431037, 0.3106212280255135, 0.4556024803888395, 0.4401157068476852, 0.3635449309113339, 0.4197992934192395, 0.39488030468789104, 0.3817226701954116, 0.3542637224465402, 0.30664308342975977, 0.29744988081432966, 0.22222987667781638, 0.23962018863070236, 0.28964362536518445, 0.2798733109109587, 0.27182540973958125, 0.27620384716393054, 0.3042626435773578, 0.2734470543736123, 0.2564302300376258, 0.31052760414177893, 0.2696299922600655, 0.33743130306848784, 0.2647268305709255, 0.29029244988810365, 0.2938574839047838, 0.387394954852313, 0.34405739739087265, 0.3133709198892715, 0.3254208525846425, 0.41224984918036484, 0.33942288772958723, 0.3642448912755633, 0.3130501165031895, 0.3491236504938038, 0.2412930253012894, 0.3425217308613015, 0.3508404654169803, 0.4035381243975576, 0.33381913972116106, 0.39565470399229985, 0.32829152012137236, 0.3546735842788459, 0.2754429369423842, 0.36518349524771676, 0.3362891988898661, 0.34352245350707683, 0.31971933123837876, 0.31482335163544667, 0.2647593891575166, 0.3281891603278938, 0.3611708663634005, 0.33979507591594127, 0.35633240331216637]]</t>
+          <t>[[0.9335209502408268, 0.8458673356102864, 0.9735548074046748, 1.155316346359035, 1.2468649738646276, 1.2077140861600524, 1.1653118368411663, 1.2910705066477257, 1.3040832085846656, 1.2371393038579335, 1.1576173454215706, 1.2193462302591127, 1.1863165669576123, 1.2141143098373188, 1.1416914739024808, 1.1429606199755908, 1.1896789170389643, 1.0923611175236303, 1.0563191890766532, 1.1268837049024194, 1.1529858553780912, 1.1378365176400869, 1.1413235446636256, 1.1888180773821133, 1.2042645064015531, 1.1582311629682747, 1.1624791585988852, 1.2527713119549275, 1.3371349438203184, 1.3167032265633054, 1.3658241998854586, 1.3765740424224429, 1.429773946189004, 1.3059640942497828, 1.250889395553636, 1.2716145532564729, 1.2573632219456818, 1.2031105125187074, 1.1835977663673047, 1.2223126763544092, 1.2213917422031122, 1.212031841839797, 1.1562578185078607, 1.190050749342104, 1.235340200607604, 1.2508052605425815, 1.1998581815059326, 1.1915230382545534, 1.2834322567108125, 1.30888124189437, 1.2261965607031868, 1.2316091629772705, 1.2651257202049357, 1.2142574604577425, 1.1967709088151484, 1.2037790154617196, 1.2404037756003565, 1.2375842831745194, 1.1258928429198276, 1.156656529718471], [1.32038622003922, 1.1403177240756333, 1.2929347118172183, 1.5225523192117925, 1.6287686579830314, 1.5701834176031697, 1.5335016434973212, 1.6895803919532602, 1.7123383050338374, 1.6272938971302455, 1.5418635006127683, 1.6394102521941327, 1.5834427104170736, 1.584388195543277, 1.5138813857955802, 1.5129275433905263, 1.5699071579501112, 1.466113537785705, 1.4165321976244805, 1.5041554044725465, 1.5248308390405025, 1.4883030378438413, 1.47922017478087, 1.5674079174245972, 1.5539401920369795, 1.5185623989672146, 1.533332523325811, 1.6581298070737833, 1.7511272392232533, 1.7640002846784015, 1.9393828255872492, 1.9494664963465878, 2.0084589070349517, 1.7913330109711112, 1.662405647174258, 1.700949657043023, 1.6586237086447322, 1.6058344893819434, 1.5881180102048815, 1.613927110547268, 1.598399005715658, 1.566045805402108, 1.550794253960914, 1.6135438055717732, 1.6516286762218977, 1.6860481482702905, 1.6358456765641618, 1.5857576055764273, 1.7281446773469709, 1.7753334190968122, 1.6591567703137517, 1.6336342874987042, 1.667347481070637, 1.5996640317190558, 1.6003852946060853, 1.5741790733665317, 1.5918642666143918, 1.5945414845191073, 1.4773499407933082, 1.5187057444515526], [0.22323357068688865, 0.21691194105956782, 0.2626416304545296, 0.28910089291137536, 0.3437963988604174, 0.3131935452126425, 0.28568511356963966, 0.32593516071966094, 0.4513219220739407, 0.45293831898147946, 0.36701053641430603, 0.452808502456416, 0.41456645197062675, 0.3896717208785628, 0.35213241697602643, 0.31909773216843235, 0.3049678031672804, 0.2246986376418727, 0.23841158486911357, 0.2915583991971193, 0.2835049097393461, 0.26268517743712155, 0.2605591115365069, 0.28590782930594283, 0.27161061034918305, 0.25040125870348984, 0.3101761401423547, 0.26114328757858646, 0.3379356715303991, 0.2592826418128922, 0.30488092960132807, 0.29861485871976173, 0.3784917644602469, 0.3404325035184208, 0.3218971254292664, 0.3196093052995597, 0.40748449025240374, 0.35053069235302703, 0.37295765701673994, 0.3535836305798023, 0.3528900741924037, 0.24911864395064945, 0.35123682714529236, 0.35531743808000904, 0.3966350203778835, 0.33016452486215186, 0.3757624663358745, 0.320296317923074, 0.3476362756049209, 0.26853616561467697, 0.3415566489334177, 0.38416783032845075, 0.36749406844927, 0.31089033050959697, 0.32787246683092497, 0.2844751467792504, 0.3143315611293458, 0.362955136728743, 0.3344387490795829, 0.3769287496762099]]</t>
         </is>
       </c>
       <c r="H227" t="n">
-        <v>340.1713373661041</v>
+        <v>325.8793396949768</v>
       </c>
     </row>
     <row r="228">
@@ -8190,7 +8190,7 @@
         </is>
       </c>
       <c r="H228" t="n">
-        <v>328.4981434345245</v>
+        <v>324.4244456291199</v>
       </c>
     </row>
     <row r="229">
@@ -8224,7 +8224,7 @@
         </is>
       </c>
       <c r="H229" t="n">
-        <v>326.8274784088135</v>
+        <v>325.0582172870636</v>
       </c>
     </row>
     <row r="230">
@@ -8258,7 +8258,7 @@
         </is>
       </c>
       <c r="H230" t="n">
-        <v>69.46369028091431</v>
+        <v>70.75689148902893</v>
       </c>
     </row>
     <row r="231">
@@ -8292,7 +8292,7 @@
         </is>
       </c>
       <c r="H231" t="n">
-        <v>69.42470383644104</v>
+        <v>70.50633668899536</v>
       </c>
     </row>
     <row r="232">
@@ -8326,7 +8326,7 @@
         </is>
       </c>
       <c r="H232" t="n">
-        <v>69.44791531562805</v>
+        <v>70.31151986122131</v>
       </c>
     </row>
     <row r="233">
@@ -8337,7 +8337,7 @@
         <v>100</v>
       </c>
       <c r="C233" t="n">
-        <v>7.000000000000001</v>
+        <v>7</v>
       </c>
       <c r="D233" t="inlineStr">
         <is>
@@ -8360,7 +8360,7 @@
         </is>
       </c>
       <c r="H233" t="n">
-        <v>73.62355947494507</v>
+        <v>74.96495151519775</v>
       </c>
     </row>
     <row r="234">
@@ -8371,7 +8371,7 @@
         <v>100</v>
       </c>
       <c r="C234" t="n">
-        <v>7.000000000000001</v>
+        <v>7</v>
       </c>
       <c r="D234" t="inlineStr">
         <is>
@@ -8394,7 +8394,7 @@
         </is>
       </c>
       <c r="H234" t="n">
-        <v>73.67363595962524</v>
+        <v>74.88202524185181</v>
       </c>
     </row>
     <row r="235">
@@ -8405,7 +8405,7 @@
         <v>100</v>
       </c>
       <c r="C235" t="n">
-        <v>7.000000000000001</v>
+        <v>7</v>
       </c>
       <c r="D235" t="inlineStr">
         <is>
@@ -8428,7 +8428,7 @@
         </is>
       </c>
       <c r="H235" t="n">
-        <v>73.84198188781738</v>
+        <v>74.75844955444336</v>
       </c>
     </row>
     <row r="236">
@@ -8462,7 +8462,7 @@
         </is>
       </c>
       <c r="H236" t="n">
-        <v>86.7164740562439</v>
+        <v>86.98901438713074</v>
       </c>
     </row>
     <row r="237">
@@ -8496,7 +8496,7 @@
         </is>
       </c>
       <c r="H237" t="n">
-        <v>86.27677440643311</v>
+        <v>86.99670743942261</v>
       </c>
     </row>
     <row r="238">
@@ -8530,7 +8530,7 @@
         </is>
       </c>
       <c r="H238" t="n">
-        <v>86.70595335960388</v>
+        <v>87.00978541374207</v>
       </c>
     </row>
     <row r="239">
@@ -8564,7 +8564,7 @@
         </is>
       </c>
       <c r="H239" t="n">
-        <v>327.5038826465607</v>
+        <v>325.6607387065887</v>
       </c>
     </row>
     <row r="240">
@@ -8598,7 +8598,7 @@
         </is>
       </c>
       <c r="H240" t="n">
-        <v>328.8642904758453</v>
+        <v>326.1527924537659</v>
       </c>
     </row>
     <row r="241">
@@ -8632,7 +8632,7 @@
         </is>
       </c>
       <c r="H241" t="n">
-        <v>329.1196932792664</v>
+        <v>325.901127576828</v>
       </c>
     </row>
     <row r="242">
@@ -8666,7 +8666,7 @@
         </is>
       </c>
       <c r="H242" t="n">
-        <v>69.32206249237061</v>
+        <v>70.29250931739807</v>
       </c>
     </row>
     <row r="243">
@@ -8677,7 +8677,7 @@
         <v>20</v>
       </c>
       <c r="C243" t="n">
-        <v>7.000000000000001</v>
+        <v>7</v>
       </c>
       <c r="D243" t="inlineStr">
         <is>
@@ -8700,7 +8700,7 @@
         </is>
       </c>
       <c r="H243" t="n">
-        <v>72.61595106124878</v>
+        <v>73.69603800773621</v>
       </c>
     </row>
     <row r="244">
@@ -8734,7 +8734,7 @@
         </is>
       </c>
       <c r="H244" t="n">
-        <v>84.61346244812012</v>
+        <v>85.6652729511261</v>
       </c>
     </row>
     <row r="245">
@@ -8768,7 +8768,7 @@
         </is>
       </c>
       <c r="H245" t="n">
-        <v>324.8668870925903</v>
+        <v>325.4684693813324</v>
       </c>
     </row>
     <row r="246">
@@ -8802,7 +8802,7 @@
         </is>
       </c>
       <c r="H246" t="n">
-        <v>68.62318873405457</v>
+        <v>69.57052826881409</v>
       </c>
     </row>
     <row r="247">
@@ -8836,7 +8836,7 @@
         </is>
       </c>
       <c r="H247" t="n">
-        <v>68.60042786598206</v>
+        <v>69.47937417030334</v>
       </c>
     </row>
     <row r="248">
@@ -8847,7 +8847,7 @@
         <v>40</v>
       </c>
       <c r="C248" t="n">
-        <v>7.000000000000001</v>
+        <v>7</v>
       </c>
       <c r="D248" t="inlineStr">
         <is>
@@ -8870,7 +8870,7 @@
         </is>
       </c>
       <c r="H248" t="n">
-        <v>72.84841418266296</v>
+        <v>73.7703595161438</v>
       </c>
     </row>
     <row r="249">
@@ -8881,7 +8881,7 @@
         <v>40</v>
       </c>
       <c r="C249" t="n">
-        <v>7.000000000000001</v>
+        <v>7</v>
       </c>
       <c r="D249" t="inlineStr">
         <is>
@@ -8904,7 +8904,7 @@
         </is>
       </c>
       <c r="H249" t="n">
-        <v>74.46511888504028</v>
+        <v>73.59562635421753</v>
       </c>
     </row>
     <row r="250">
@@ -8929,16 +8929,16 @@
       </c>
       <c r="F250" t="inlineStr">
         <is>
-          <t>[[5.0711823, 5.257538, 1.6350428, 1.7153407, 1.6105385, 1.6714023, 1.6146559, 1.777985, 1.7624278, 1.8127462, 1.7132571, 1.7888546, 1.5989786, 1.7481829, 1.7286377, 1.7724464, 1.7314026, 1.7402925, 1.6480916, 1.6647336, 1.6202643, 1.7022164, 1.7261746, 1.8462679, 1.7624159, 1.8103712, 1.7969205, 1.983173, 2.0249257, 2.187679, 2.1571558, 2.1527221, 2.10214, 2.1153686, 2.0078576, 2.0262847, 1.797962, 1.7706282, 1.7457697, 1.8836281, 1.7422074, 1.8169397, 1.7731324, 1.8400117, 1.7236675, 1.848644, 1.7657839, 1.811791, 1.7541556, 1.9226177, 1.8675884, 1.8892856, 1.8176866, 1.8433914, 1.8076562, 1.7607079, 1.6754463, 1.7923611, 1.7369156, 1.7052656], [7.1056341033536325, 8.096553361188105, 2.1765337041851893, 2.2665287714507323, 2.127010964692213, 2.1774227723399044, 2.173287131553665, 2.3920950763969864, 2.3385867402647147, 2.3901395616524206, 2.306399055771067, 2.4300874338000855, 2.1962202374303965, 2.3138212604976656, 2.3834773902660937, 2.465695580075431, 2.355721784320481, 2.3571683151554748, 2.270902078503736, 2.289362969060971, 2.209579320198149, 2.2402506580775388, 2.3056381075479506, 2.4537846352634296, 2.348540839220457, 2.3887839614633797, 2.467114450002598, 2.6860701727374647, 2.776244126905801, 2.9742791336298775, 3.0751480190968805, 3.092412794482569, 2.9932598055139925, 2.890836965676477, 2.7926066984250797, 2.8340420864967175, 2.486423056109446, 2.3975276650273574, 2.3999852458182453, 2.5621149657732682, 2.3511903791559807, 2.431856714168635, 2.4320862143506394, 2.5534299969449124, 2.338866473936478, 2.5193240058297577, 2.4716373411339387, 2.4504008140455507, 2.3028622398435, 2.5245726308697036, 2.515481790766722, 2.5320361764984085, 2.4509095313730658, 2.4795120917562157, 2.436435467005353, 2.3037293592284858, 2.1726511933598114, 2.331971645392227, 2.300099710708042, 2.2588927116972566], [1.889838, 2.1675515, 0.44874674, 0.43468234, 0.45973435, 0.44484258, 0.42806613, 0.4240508, 0.6344984, 0.6411301, 0.5627603, 0.7016713, 0.64141583, 0.6357723, 0.54744124, 0.51770276, 0.47614333, 0.38609228, 0.40110365, 0.45511428, 0.42886177, 0.40769437, 0.42698857, 0.49978706, 0.40550262, 0.36961728, 0.41983697, 0.3834013, 0.45625, 0.37575388, 0.45396212, 0.44579953, 0.52348113, 0.5161277, 0.5214641, 0.54752547, 0.59720194, 0.5481963, 0.5549542, 0.5735562, 0.5091901, 0.40655228, 0.52131486, 0.52352536, 0.5499557, 0.49592578, 0.61361265, 0.56148165, 0.5236529, 0.45364463, 0.58451957, 0.57333785, 0.5249618, 0.5155327, 0.4731566, 0.42844486, 0.43135917, 0.5186543, 0.55715173, 0.62270147]]</t>
+          <t>[[5.0711823, 5.257538, 1.6350428, 1.7153335, 1.6212447, 1.6926938, 1.6280189, 1.7753787, 1.766985, 1.8106343, 1.7173764, 1.7623873, 1.6262614, 1.7758652, 1.8116299, 1.8178447, 1.7222711, 1.7006543, 1.6216753, 1.6291634, 1.5749449, 1.622627, 1.7082068, 1.8309406, 1.7264344, 1.7789749, 1.7739154, 1.9247245, 1.9157372, 2.0489566, 2.0917008, 2.1197681, 2.090901, 2.1204433, 2.0297148, 2.0595226, 1.8336811, 1.7548027, 1.7604629, 1.8285557, 1.7001005, 1.7389598, 1.7280705, 1.7814808, 1.7111431, 1.8975022, 1.8114929, 1.8397379, 1.7818018, 1.9517698, 1.839024, 1.8794295, 1.7985061, 1.8395392, 1.8181252, 1.7791053, 1.706187, 1.8450099, 1.7201064, 1.7300622], [7.1056341033536325, 8.096553361188105, 2.1765337041851893, 2.26651898866042, 2.141387914880405, 2.2036249121154667, 2.173951069250493, 2.374832649358113, 2.3444830193241257, 2.3890244854534135, 2.339639849049528, 2.3677284957042937, 2.1861011937374384, 2.3329485394312233, 2.4504029545959534, 2.4914089409809765, 2.347908095372646, 2.3028097488194312, 2.2580471246902216, 2.2663898097917707, 2.140438433682457, 2.1453985742915047, 2.283213358416438, 2.466884535970878, 2.327276395224531, 2.3516952122344295, 2.378752203903741, 2.5697880821579293, 2.593585273383642, 2.76411319080232, 3.01664929955754, 3.0532471365887504, 3.058546199891798, 2.94236482398874, 2.796714309253233, 2.8246113568904248, 2.5471042459674553, 2.421449291592316, 2.4412918918529196, 2.490767214746131, 2.318853979529834, 2.3491168818002928, 2.441035323384774, 2.4930092344759522, 2.332278853519392, 2.580054653387275, 2.490776499660005, 2.4723113242771775, 2.4029686091893225, 2.6223346257319533, 2.4814789404574027, 2.497639686259884, 2.4379736611286797, 2.496702881038127, 2.4716237399831593, 2.36450385633716, 2.259848234600393, 2.420597059195487, 2.3289425841641633, 2.309923128112294], [1.889838, 2.1675515, 0.44874674, 0.43468067, 0.4586353, 0.4394503, 0.43877843, 0.44712293, 0.62494963, 0.6481767, 0.58672947, 0.65044016, 0.61880314, 0.629418, 0.551749, 0.51496005, 0.47432846, 0.3805432, 0.41703334, 0.43553534, 0.41782337, 0.38798606, 0.4061664, 0.5086878, 0.41283563, 0.38603625, 0.43304685, 0.38677457, 0.4427792, 0.37195694, 0.43782672, 0.41876528, 0.5179844, 0.5188261, 0.5304114, 0.51921004, 0.5516003, 0.5452156, 0.58474094, 0.5718126, 0.5295062, 0.40617126, 0.5462475, 0.5656348, 0.57288796, 0.47392985, 0.56873304, 0.5219941, 0.5213147, 0.42096853, 0.52017134, 0.56878775, 0.517513, 0.49248487, 0.4777843, 0.4523293, 0.46807978, 0.53439134, 0.553356, 0.6370956]]</t>
         </is>
       </c>
       <c r="G250" t="inlineStr">
         <is>
-          <t>[[7.852181773480187, 1.9352298026375228, 1.417640526191716, 1.5035786923328678, 1.5022915602335292, 1.5360023375580165, 1.4668564694190902, 1.6157588951277235, 1.6461339418037553, 1.6761579911096587, 1.5804332898289173, 1.5986648540028805, 1.504786013417552, 1.598324111605191, 1.5827775307231544, 1.6020335144851574, 1.6248614003572468, 1.6065803811536314, 1.5155723153484615, 1.5372282089044615, 1.519079475134721, 1.5631269653772222, 1.5740840332986235, 1.65578788909531, 1.6219953157607028, 1.644759297605534, 1.6489858760139298, 1.791357473365767, 1.8741153723270219, 1.9317655195831958, 1.8939761949003082, 1.901933689048044, 1.9651049803565466, 1.884997925355712, 1.8313993304528384, 1.7485852630835814, 1.6757178279399416, 1.6024700083452283, 1.630622901687939, 1.6826584774745323, 1.6083200983287413, 1.6775574496938308, 1.6383391068286046, 1.6514981542236122, 1.6028427049563565, 1.7305892281558524, 1.6294254916609185, 1.5948172553997568, 1.6200164669813717, 1.7338219330400437, 1.6894763876591807, 1.7056715018351831, 1.68812741021341, 1.6822899583498139, 1.6384070111271545, 1.5676211615641975, 1.5758750396978571, 1.6439156723505675, 1.5659499720118026, 1.5370802979651192], [13.622421583331487, 2.5132168338801346, 1.8821199248585803, 1.9812058543906672, 1.9704989813236145, 2.0148491658032808, 1.9696975344280399, 2.1504328216724446, 2.174785086149167, 2.1934676991058417, 2.103095479235952, 2.174014629991199, 2.0375180260202743, 2.1301539053583185, 2.181711899578526, 2.1792159628105017, 2.1771101673205173, 2.1490443426182932, 2.0582326306769887, 2.082767501515118, 2.0300397465921973, 2.0378577828414097, 2.0751874737617357, 2.178697688501122, 2.1413226640232415, 2.149043944674306, 2.2053225904156415, 2.375133859814305, 2.51985921930832, 2.5664202973061916, 2.7163305810413934, 2.6715360459876614, 2.8029671321890977, 2.5910581931409773, 2.477431648222568, 2.3542640930237346, 2.2697889222853633, 2.1579405626455097, 2.2385064798854013, 2.250408784774562, 2.1310399176788524, 2.223441466482075, 2.2157305850070945, 2.232635523994813, 2.166999060131113, 2.335707853325445, 2.2455891338453213, 2.1022154428275495, 2.1136727739392915, 2.2977635395905156, 2.2721882658406676, 2.2519691955216206, 2.254748711385006, 2.238273924852197, 2.20313708316018, 2.0346630215931585, 2.0400874187883105, 2.146474891933671, 2.055714528239114, 2.022798002819198], [3.2986565280607776, 0.5532409568720651, 0.36842704246542085, 0.38019852871174653, 0.42824634603858985, 0.404839828784617, 0.3788996379118815, 0.40151854476936416, 0.5889084125644788, 0.5751715642120004, 0.5230226419848654, 0.6071989682079401, 0.571136103365539, 0.5728210109066024, 0.47752328218654705, 0.4737604537060751, 0.4414182394382312, 0.35677621337286625, 0.35737656851596505, 0.4239177089739417, 0.39875620025574665, 0.3805297844247386, 0.3868530063119254, 0.43960815053445695, 0.35561722590906003, 0.33044647884430833, 0.3830625772884198, 0.36532063958233874, 0.4172198428899069, 0.3415145847726157, 0.3851879908186369, 0.39628646822836056, 0.4742374876049246, 0.4762446309272002, 0.4649702851387849, 0.48268901446177054, 0.5404966304500732, 0.4989257454107988, 0.5174034925177312, 0.503585291822788, 0.4612899796823845, 0.37169003565169845, 0.473230851354545, 0.45251525200333037, 0.5225657715003623, 0.46757104242443676, 0.5594654939230007, 0.46757134077117424, 0.480126056494968, 0.41156947693555895, 0.5195037987571537, 0.4934155173862555, 0.4832865221040373, 0.4421671097068965, 0.421006810146257, 0.37393332263745543, 0.40480705763709873, 0.4904408576328692, 0.49282473452886055, 0.5421501854304553]]</t>
+          <t>[[7.852181773480187, 1.9352298026375228, 1.417640526191716, 1.5049014864237291, 1.5235631356763826, 1.5472233945331377, 1.489518426173045, 1.598726729739174, 1.6520876697039706, 1.654493400911899, 1.5523788737502835, 1.61302871887954, 1.5409709356624128, 1.638878810469714, 1.622904562749123, 1.606813455827038, 1.589737200212242, 1.5475954566575958, 1.4730441652421684, 1.4924781703909924, 1.4500407563098106, 1.4995828526432922, 1.577394528372999, 1.605918269775705, 1.5716193080012035, 1.6235128572911894, 1.5974364471839606, 1.7125631741810412, 1.7336622984938845, 1.8719520530273435, 1.8630084155672488, 1.9059327525115362, 1.9288045520699073, 1.8918360718970186, 1.8375616837370043, 1.7834010092469768, 1.69357159805124, 1.5959690295679791, 1.589732451082843, 1.615205450078833, 1.586702221413117, 1.607397989671906, 1.5893542013832973, 1.612967481894963, 1.626450665065035, 1.7417112313000171, 1.648063336331858, 1.6275792269294762, 1.648320280120074, 1.732337271657687, 1.6542498304212454, 1.6943943497175997, 1.6852641777452841, 1.6925305663891042, 1.6617703899339773, 1.603904486805774, 1.5881625349497603, 1.6284597546779678, 1.5814617520255223, 1.5616106989601328], [13.622421583331487, 2.5132168338801346, 1.8821199248585803, 1.9840329503692415, 2.0008723652345686, 2.014533535278135, 1.990243768899547, 2.1304705255280845, 2.1820051596753034, 2.1864983174527786, 2.0710514487587854, 2.1479052592188648, 2.0493570779125543, 2.1470954619603466, 2.1783550517731003, 2.194599735341598, 2.13447961811622, 2.089394079053235, 2.0211780618113533, 2.0326192263813767, 1.9499451905772949, 1.9726945767868997, 2.085990440223101, 2.1422651604179945, 2.0806526731664086, 2.1179481327271295, 2.1086562694549387, 2.255108239129573, 2.3115087639092193, 2.516402424802361, 2.6676706391087723, 2.7340487075891993, 2.7697338740296993, 2.576269247131404, 2.481898065065224, 2.413128457829823, 2.3098500552990116, 2.1693329825417567, 2.187743525018699, 2.185293065996739, 2.129286382883691, 2.1589086611448023, 2.17374609929255, 2.1753156264047, 2.190404519980787, 2.3286644153792166, 2.2310137907947514, 2.1734620570559913, 2.217792110473322, 2.330148510939426, 2.2319284189892237, 2.251949638712224, 2.2721598095894753, 2.2732752694722227, 2.2456847305637258, 2.1190634491792073, 2.0923581667311946, 2.1366360822551007, 2.107447235238313, 2.0590840703222426], [3.2986565280607776, 0.5532409568720651, 0.36842704246542085, 0.3691024281426962, 0.43778821553816893, 0.39877908703064074, 0.40576454984806826, 0.39131653856964516, 0.5882140681276771, 0.5846588813853574, 0.5174354279770489, 0.5814893778971783, 0.5681538023444527, 0.5828240042909428, 0.4798853573221037, 0.4642148460047754, 0.44368527237159155, 0.34866042029424826, 0.3624467629687529, 0.396914011227137, 0.37305713849441274, 0.3631292589826306, 0.37651736219986237, 0.42398753485255813, 0.3726164271678302, 0.3481044874243789, 0.39331260395288303, 0.3429362836408002, 0.39781362297331413, 0.35399649983159825, 0.39481219083476826, 0.3950476549822943, 0.46986967370916477, 0.48062438495579235, 0.4964162147951247, 0.45163223036060235, 0.5108554228425674, 0.5200228229569355, 0.5289651441366641, 0.5116360691012315, 0.4973604140173472, 0.3768786297279698, 0.5037842916847689, 0.4700948479335683, 0.5374059729987797, 0.4164016922780867, 0.5111162407453604, 0.4517978696319228, 0.4644130846697635, 0.3701570159661255, 0.46551651047611375, 0.5061502101724019, 0.47074878469327225, 0.42248527184050344, 0.44652323091941565, 0.39827797584627783, 0.42602348812630253, 0.4767540448090527, 0.4969512852168404, 0.5594332558618286]]</t>
         </is>
       </c>
       <c r="H250" t="n">
-        <v>84.82544469833374</v>
+        <v>86.1865131855011</v>
       </c>
     </row>
     <row r="251">
@@ -8972,7 +8972,7 @@
         </is>
       </c>
       <c r="H251" t="n">
-        <v>84.91398143768311</v>
+        <v>86.37507128715515</v>
       </c>
     </row>
     <row r="252">
@@ -9006,7 +9006,7 @@
         </is>
       </c>
       <c r="H252" t="n">
-        <v>325.9576108455658</v>
+        <v>324.1605761051178</v>
       </c>
     </row>
     <row r="253">
@@ -9040,7 +9040,7 @@
         </is>
       </c>
       <c r="H253" t="n">
-        <v>326.1430006027222</v>
+        <v>328.3154129981995</v>
       </c>
     </row>
     <row r="254">
@@ -9074,7 +9074,7 @@
         </is>
       </c>
       <c r="H254" t="n">
-        <v>325.0467426776886</v>
+        <v>323.7486312389374</v>
       </c>
     </row>
     <row r="255">
@@ -9108,7 +9108,7 @@
         </is>
       </c>
       <c r="H255" t="n">
-        <v>68.98445630073547</v>
+        <v>71.04674673080444</v>
       </c>
     </row>
     <row r="256">
@@ -9142,7 +9142,7 @@
         </is>
       </c>
       <c r="H256" t="n">
-        <v>68.88860464096069</v>
+        <v>70.42492318153381</v>
       </c>
     </row>
     <row r="257">
@@ -9176,7 +9176,7 @@
         </is>
       </c>
       <c r="H257" t="n">
-        <v>68.74140620231628</v>
+        <v>70.35260820388794</v>
       </c>
     </row>
     <row r="258">
@@ -9187,7 +9187,7 @@
         <v>60</v>
       </c>
       <c r="C258" t="n">
-        <v>7.000000000000001</v>
+        <v>7</v>
       </c>
       <c r="D258" t="inlineStr">
         <is>
@@ -9210,7 +9210,7 @@
         </is>
       </c>
       <c r="H258" t="n">
-        <v>73.11871290206909</v>
+        <v>74.43398475646973</v>
       </c>
     </row>
     <row r="259">
@@ -9221,7 +9221,7 @@
         <v>60</v>
       </c>
       <c r="C259" t="n">
-        <v>7.000000000000001</v>
+        <v>7</v>
       </c>
       <c r="D259" t="inlineStr">
         <is>
@@ -9244,7 +9244,7 @@
         </is>
       </c>
       <c r="H259" t="n">
-        <v>73.54196643829346</v>
+        <v>74.78356528282166</v>
       </c>
     </row>
     <row r="260">
@@ -9278,7 +9278,7 @@
         </is>
       </c>
       <c r="H260" t="n">
-        <v>85.82506155967712</v>
+        <v>86.85686659812927</v>
       </c>
     </row>
     <row r="261">
@@ -9312,7 +9312,7 @@
         </is>
       </c>
       <c r="H261" t="n">
-        <v>85.40713286399841</v>
+        <v>86.5170567035675</v>
       </c>
     </row>
     <row r="262">
@@ -9346,7 +9346,7 @@
         </is>
       </c>
       <c r="H262" t="n">
-        <v>85.64900350570679</v>
+        <v>86.49705743789673</v>
       </c>
     </row>
     <row r="263">
@@ -9380,7 +9380,7 @@
         </is>
       </c>
       <c r="H263" t="n">
-        <v>328.0758800506592</v>
+        <v>323.0020730495453</v>
       </c>
     </row>
     <row r="264">
@@ -9405,16 +9405,16 @@
       </c>
       <c r="F264" t="inlineStr">
         <is>
-          <t>[[4.5522795, 64.257744, 7.9876137, 9.033665, 9.762339, 33.378197, 4.9001646, 14.970038, 3.0607493, 2.5668273, 2.1872354, 2.2825372, 2.3146079, 2.5237281, 2.6997907, 2.6202242, 2.5602732, 2.4993186, 2.457431, 2.5474763, 2.3448696, 2.4366207, 2.4262424, 2.4720821, 2.5583375, 2.667469, 2.7936604, 2.786063, 2.7422116, 2.765388, 2.8308642, 2.7644327, 2.693016, 2.685273, 2.6254194, 2.774374, 2.616341, 2.6080816, 2.6875587, 2.626991, 2.5225413, 2.6376972, 2.5934782, 2.550796, 2.4868546, 2.574853, 2.5650012, 2.530522, 2.523704, 2.5566566, 2.613419, 2.5714226, 2.6252189, 2.6952598, 2.5926828, 2.5233724, 2.5014508, 2.5264773, 2.5704677, 2.6707845], [6.1225347423385506, 90.50334506939508, 10.7976713425117, 12.209354153984636, 13.487846838139198, 45.27049507802378, 6.420644080632117, 19.896134565646083, 4.047204906316326, 3.3360592822106487, 2.8643906592103976, 2.964499231156642, 3.0197188502929295, 3.298709883075533, 3.496270917953309, 3.4253398476055246, 3.3216906032538787, 3.2946015967171673, 3.212594674344396, 3.353524725162376, 3.0128013555081035, 3.1743551245163117, 3.1385138708673814, 3.180293594818435, 3.33596337194483, 3.528003787179242, 3.6510230629411162, 3.678050071711516, 3.5471707527438108, 3.6328173565575734, 3.653023102761142, 3.6060795788354483, 3.4516711734709764, 3.4168381221519293, 3.377273359057107, 3.610783025721414, 3.4036828963059937, 3.3772415911621843, 3.4388423726173456, 3.389868023309182, 3.2000482436358175, 3.421280482654296, 3.3449821697495463, 3.343085107028673, 3.2616519395758594, 3.3283318826910713, 3.273985750814014, 3.2595886218982892, 3.227922573186781, 3.286591750317029, 3.3520133331051865, 3.352566939787242, 3.4203404160114483, 3.5778548625937363, 3.444217706894817, 3.363491499262752, 3.298670130865344, 3.2920244883556977, 3.3308486897147422, 3.4420366348542415], [88875400000000.0, 2109405500000000.0, 275224120000000.0, 202598040000000.0, 166324390000000.0, 681750600000000.0, 12743.651, 52731.305, 68174586000000.0, 7665.624, 56890680000000.0, 50341670000000.0, 75249765000000.0, 72340690000000.0, 45651916000000.0, 75944014000000.0, 5407.294, 45813405000000.0, 52789393000000.0, 66158586000000.0, 50800050000000.0, 65147687000000.0, 57908084000000.0, 7190.4185, 7695.474, 78042170000000.0, 44251287000000.0, 44277270000000.0, 64435452000000.0, 50804543000000.0, 64384097000000.0, 63036660000000.0, 67535320000000.0, 70293423000000.0, 64469837000000.0, 53462264000000.0, 44288910000000.0, 56089358000000.0, 59646870000000.0, 63229810000000.0, 6211.4995, 64608547000000.0, 41412037000000.0, 7462.68, 51851513000000.0, 54011705000000.0, 44279210000000.0, 46315000000000.0, 55110575000000.0, 53800967000000.0, 5395.9785, 42109800000000.0, 53340350000000.0, 42359727000000.0, 65486876000000.0, 51468570000000.0, 52511755000000.0, 57877900000000.0, 5556.601, 83739060000000.0]]</t>
+          <t>[[4.5522795, 64.257744, 7.9876137, 9.033762, 4.4660516, 5.4576654, 3.8478317, 2.5846837, 2.4817, 2.7050009, 2.5653498, 2.5433931, 2.4827826, 2.6465647, 2.7386763, 2.6644073, 2.6549404, 2.5656252, 2.4985862, 2.566081, 2.4378977, 2.530608, 2.5628695, 2.6296248, 2.6489942, 2.693469, 2.7721834, 2.7663898, 2.6955276, 2.8492575, 2.8783, 2.7491863, 2.6905353, 2.6844056, 2.6411612, 2.797553, 2.6754818, 2.7136168, 2.7217827, 2.6084356, 2.524596, 2.6405387, 2.5608616, 2.5265393, 2.447541, 2.539, 2.5328598, 2.5322046, 2.5141487, 2.576913, 2.614561, 2.5269597, 2.5498884, 2.639457, 2.57203, 2.5652275, 2.544333, 2.598359, 2.5511184, 2.6319156], [6.1225347423385506, 90.50334506939508, 10.7976713425117, 12.209469131563804, 6.3692592129024375, 7.187228255732525, 5.224547860327115, 3.4797180256663, 3.294126838683279, 3.582384131634875, 3.388548606367458, 3.3332328463348824, 3.2725335013217127, 3.43657130787737, 3.5510355876148068, 3.4709076915040384, 3.466796875, 3.380801124886336, 3.269112800610097, 3.350691248618245, 3.1078785117816525, 3.2845075150460596, 3.3555717763305193, 3.4111439955621154, 3.423486617487673, 3.525080329574924, 3.585615289045605, 3.621861249948622, 3.479316906150236, 3.7124263306574963, 3.6773166024166564, 3.5685570071759196, 3.442098974335441, 3.4080455841991744, 3.391344829039165, 3.655012524501148, 3.4697907407254154, 3.519063260107396, 3.5100842025090526, 3.3812053289653283, 3.222209663658954, 3.4149495593879657, 3.3354940722742645, 3.3147989608540223, 3.230475687483104, 3.3066054385679564, 3.256541637752468, 3.272580710655043, 3.259915850670779, 3.325209078991327, 3.3812051879395337, 3.3132337801104588, 3.350138185981787, 3.5026141349716813, 3.429552218956053, 3.4472942578042476, 3.371581147322929, 3.3710841314680278, 3.3032138144860417, 3.424403680276425], [88875400000000.0, 2109405500000000.0, 275224120000000.0, 202608570000000.0, 128708990000000.0, 104647280000000.0, 11542.957, 7271.364, 46090650000000.0, 7745.067, 67044557000000.0, 54164793000000.0, 72131130000000.0, 75808200000000.0, 44418350000000.0, 75358780000000.0, 6521.0996, 48061267000000.0, 54186994000000.0, 65273840000000.0, 44173974000000.0, 62560060000000.0, 56515247000000.0, 7792.557, 7403.3228, 84859820000000.0, 39369272000000.0, 41987680000000.0, 64026327000000.0, 53827294000000.0, 64587953000000.0, 62360044000000.0, 67385460000000.0, 71983580000000.0, 69277118000000.0, 56090820000000.0, 52272360000000.0, 65875830000000.0, 64749807000000.0, 66587432000000.0, 6310.8413, 60308830000000.0, 44510220000000.0, 8479.681, 46440575000000.0, 54009320000000.0, 49953913000000.0, 43422490000000.0, 52928413000000.0, 58474830000000.0, 5667.398, 42959924000000.0, 52192590000000.0, 41386053000000.0, 61068517000000.0, 49845176000000.0, 47024804000000.0, 53758000000000.0, 5170.1797, 81774420000000.0]]</t>
         </is>
       </c>
       <c r="G264" t="inlineStr">
         <is>
-          <t>[[119.84557584504654, 15.810280106181366, 18.688564795859136, 20.245438468756173, 66.72010379670213, 8.71134869215292, 29.271159958329935, 4.224427470445198, 2.517653473351658, 1.9097710762771662, 1.9173977483216664, 1.9645812423779156, 2.0489497101433973, 2.1828787459272125, 2.3233313084832568, 2.246426372937777, 2.2759656431769733, 2.1405435365751906, 2.1673705289058525, 2.1472622249124953, 2.084587610959764, 2.017466053030177, 2.1382746638868997, 2.163102886358006, 2.300483410925212, 2.344512336882643, 2.464287297951212, 2.403113828300346, 2.416860368909895, 2.3372295973546984, 2.4789868690553716, 2.3759427247002436, 2.427643067221499, 2.297367624646238, 2.3139614419344943, 2.3695388949403697, 2.290639655007992, 2.247466209494453, 2.373430857137381, 2.2537779717205857, 2.262720727665517, 2.2463956326855987, 2.2752352602577384, 2.2247827204139545, 2.229026665157076, 2.239113382617435, 2.2644392206858575, 2.197534412448411, 2.2572433820723456, 2.1831675334648852, 2.3075882679488404, 2.2272562714299693, 2.3474274400493687, 2.3149574012199716, 2.2652207606284738, 2.1575345794921494, 2.234883801566998, 2.2149219735311614, 2.289353422557562, 2.2514337646451903], [214.6125956970957, 24.710835437393598, 26.281443655216037, 30.522302117715583, 98.25948956775034, 12.782087494097839, 41.367026437791615, 5.872997085781279, 3.3152885182817102, 2.4449144535430274, 2.4955518685450375, 2.5196128330648637, 2.6464924398801593, 2.8149615759558837, 3.0029366191388367, 2.898478173009672, 2.9254411462635286, 2.7594416708438514, 2.7978714292669054, 2.741133328391663, 2.663649656833395, 2.599239345637795, 2.769708035445526, 2.772089972258924, 2.985121743465725, 3.09247354374385, 3.179646251664471, 3.1175398626785418, 3.099482182386344, 3.051508801383103, 3.1892395287392437, 3.038571534013904, 3.0800652322501985, 2.914404605299294, 2.9480635882654633, 3.0621037470221593, 2.948679837171837, 2.8661444619375787, 3.011081588655086, 2.857858631205734, 2.864444829133631, 2.868294743297282, 2.9246640362209773, 2.8627696009338264, 2.8851031629930253, 2.8513192917921164, 2.8839890171808245, 2.7922365450216238, 2.8735834602578985, 2.7854629811611735, 2.9506024518484772, 2.877886259780809, 3.049720084004316, 3.000347225147738, 2.949642263460884, 2.8356496892363507, 2.8944773657816607, 2.8444981943400145, 2.945756022157374, 2.878519507118136], [3984708511401641.0, 516854599392085.3, 596469632255832.5, 410561475556007.3, 1353666950626852.8, 131710363446451.53, 73495.38606009627, 12829.562947132054, 47044860875275.65, 5999.99061941738, 51645871111212.68, 47317516214904.7, 69220176696014.414, 59411361495326.85, 39255796441814.695, 62640013691158.21, 5220.491608538408, 41785627061761.5, 47802110794465.375, 58239043072000.05, 43536256075970.97, 55000983006254.45, 46900325854388.17, 6302.523619952386, 6528.576713898171, 65782044884436.65, 45215953976680.805, 36378687314811.66, 61907326819171.92, 48029638088744.234, 55493128869781.5, 52692667350643.1, 64848291301771.92, 59250566651141.93, 55954509200916.18, 48460461942385.836, 38417466941751.47, 53035616649323.09, 56260028875498.09, 55104799745634.58, 6095.5335679775635, 55317185803296.66, 37069425041751.37, 5973.627901081647, 47124671274444.7, 47337067320968.07, 43121818031481.61, 43678137425344.38, 50127836763450.336, 43715032173261.23, 5667.182281662518, 41822375725142.0, 47245378071658.84, 37418703276414.4, 58154451621711.0, 47321068381186.98, 49573514637411.336, 54696940773660.93, 4977.563398894617, 68936516532093.41]]</t>
+          <t>[[119.84557584504654, 15.810280106181366, 18.688564795859136, 8.493691646841096, 7.859836709935671, 5.001178783280081, 2.3506252308881375, 2.191269760148362, 2.2263396639991515, 2.276275023204792, 2.246828141120922, 2.2067116510161138, 2.1941081976406354, 2.2913296805107737, 2.3857857281656702, 2.295798371611342, 2.3340094674082663, 2.1858255321830646, 2.191787331192374, 2.1812327428678766, 2.191794531538055, 2.1837427376566114, 2.295094529563424, 2.2562539603210934, 2.326587791349847, 2.326694493368625, 2.4153727608399964, 2.357660642372418, 2.3835704179210486, 2.408237744820594, 2.4880496489245796, 2.3844756768853346, 2.412271405088812, 2.3242105677500735, 2.312529993520757, 2.3890280134255812, 2.385961907567785, 2.294178425312184, 2.329900884029847, 2.287833622683359, 2.287546499489861, 2.2619293261764026, 2.2567085677909726, 2.1723804581455397, 2.218152452138385, 2.1960142456171545, 2.2391474659077817, 2.1723473624107865, 2.280074373342681, 2.2105516311037507, 2.2916896180087507, 2.2213012135356167, 2.2906468603642316, 2.2673750100098293, 2.2963950719626194, 2.2337603384924543, 2.265613398414018, 2.2301896296841934, 2.290097393452951, 2.2452980666883025], [214.6125956970957, 24.710835437393598, 26.281443655216037, 15.597839094943685, 10.447160203413564, 6.950527959228462, 3.0575900949584063, 2.8607049642906657, 2.9062311307058093, 2.9884533861395135, 2.9255161764616235, 2.8679860809612814, 2.8323311220683376, 2.943024551967737, 3.0710015996265816, 2.9697438644661913, 3.0095927062586556, 2.827094366466792, 2.8345510616905734, 2.788808153070428, 2.7894896074186915, 2.8235067183263514, 2.9718376976988536, 2.898206490715666, 2.991685795427938, 3.0138432622036593, 3.08236352664285, 3.0512140009893214, 3.067595597757343, 3.0897283169492717, 3.171120702930853, 3.0914496762799195, 3.0730666232818304, 2.9312449261713, 2.9463221596031346, 3.1008147797763144, 3.0670911974941735, 2.9237151204578593, 2.9745092144734384, 2.918812286325266, 2.92087414460876, 2.8705340536457515, 2.8970404907354816, 2.8178375594180114, 2.912237880170494, 2.8202465058239716, 2.8847722265979474, 2.7781915977342813, 2.917125387513117, 2.834124066122341, 2.9387591462653195, 2.892349929407836, 2.986594587996952, 2.963416405998168, 3.0011066057868696, 2.9548013023786726, 2.949436051217485, 2.86113295503759, 2.949566751299898, 2.9103857642629327], [3984708511401641.0, 516854599392085.3, 596469632255832.5, 166875215545441.16, 173110633561454.72, 73617751546892.81, 5882.46348792531, 7136.516936747322, 41174366298810.11, 7501.370215404498, 58220025560874.57, 45655282854954.56, 65098459762814.49, 63499054503125.41, 39864233361772.375, 61483912161844.8, 6379.429095167868, 41663532536283.01, 51364946871283.9, 57209407525590.98, 44700121634120.92, 56379590344312.74, 49045598217825.945, 6663.229020553068, 6321.474293918045, 77019013187753.17, 37040358091818.94, 33954075298205.81, 60632458682158.055, 50143328880744.98, 55564747523057.24, 51968072532395.305, 62200331117544.234, 59922189063134.65, 55892032506920.234, 51326713746435.9, 43056575176618.664, 59497873194390.17, 57967756060839.8, 52385411843886.86, 6063.185817691721, 54741683448171.266, 41653433810219.266, 7435.489493380461, 48671012841326.77, 52903383742035.41, 45197160607611.14, 40373013850465.39, 48242371254557.21, 51348803861598.02, 5003.292113064277, 37646890074246.36, 47765925928892.1, 35746873932059.72, 52684676770605.67, 44538021821052.27, 42821487185386.24, 49539502985245.58, 4633.533492159052, 69751490173552.5]]</t>
         </is>
       </c>
       <c r="H264" t="n">
-        <v>327.2197415828705</v>
+        <v>324.2798628807068</v>
       </c>
     </row>
     <row r="265">
@@ -9448,7 +9448,7 @@
         </is>
       </c>
       <c r="H265" t="n">
-        <v>69.90077209472656</v>
+        <v>70.77788376808167</v>
       </c>
     </row>
     <row r="266">
@@ -9482,7 +9482,7 @@
         </is>
       </c>
       <c r="H266" t="n">
-        <v>69.81060671806335</v>
+        <v>70.77429938316345</v>
       </c>
     </row>
     <row r="267">
@@ -9516,7 +9516,7 @@
         </is>
       </c>
       <c r="H267" t="n">
-        <v>70.01840257644653</v>
+        <v>70.81188178062439</v>
       </c>
     </row>
     <row r="268">
@@ -9527,7 +9527,7 @@
         <v>80</v>
       </c>
       <c r="C268" t="n">
-        <v>7.000000000000001</v>
+        <v>7</v>
       </c>
       <c r="D268" t="inlineStr">
         <is>
@@ -9550,7 +9550,7 @@
         </is>
       </c>
       <c r="H268" t="n">
-        <v>74.27619576454163</v>
+        <v>74.99134206771851</v>
       </c>
     </row>
     <row r="269">
@@ -9561,7 +9561,7 @@
         <v>80</v>
       </c>
       <c r="C269" t="n">
-        <v>7.000000000000001</v>
+        <v>7</v>
       </c>
       <c r="D269" t="inlineStr">
         <is>
@@ -9584,7 +9584,7 @@
         </is>
       </c>
       <c r="H269" t="n">
-        <v>74.13075971603394</v>
+        <v>74.91050791740417</v>
       </c>
     </row>
     <row r="270">
@@ -9595,7 +9595,7 @@
         <v>80</v>
       </c>
       <c r="C270" t="n">
-        <v>7.000000000000001</v>
+        <v>7</v>
       </c>
       <c r="D270" t="inlineStr">
         <is>
@@ -9618,7 +9618,7 @@
         </is>
       </c>
       <c r="H270" t="n">
-        <v>73.91971397399902</v>
+        <v>74.73431205749512</v>
       </c>
     </row>
     <row r="271">
@@ -9652,7 +9652,7 @@
         </is>
       </c>
       <c r="H271" t="n">
-        <v>86.16939544677734</v>
+        <v>87.16275024414062</v>
       </c>
     </row>
     <row r="272">
@@ -9686,7 +9686,7 @@
         </is>
       </c>
       <c r="H272" t="n">
-        <v>86.58708643913269</v>
+        <v>87.2024188041687</v>
       </c>
     </row>
     <row r="273">
@@ -9720,7 +9720,7 @@
         </is>
       </c>
       <c r="H273" t="n">
-        <v>86.31280279159546</v>
+        <v>87.31514525413513</v>
       </c>
     </row>
     <row r="274">
@@ -9745,16 +9745,16 @@
       </c>
       <c r="F274" t="inlineStr">
         <is>
-          <t>[[5.0775547, 4.735642, 1.5464158, 1.4658083, 1.4398425, 1.5052809, 1.4543039, 1.6368668, 1.5760062, 1.5869349, 1.4898415, 1.5914936, 1.4395621, 1.5468807, 1.5168164, 1.535066, 1.4760871, 1.4447712, 1.4173831, 1.4477216, 1.3899528, 1.4779696, 1.5280119, 1.5836529, 1.5164026, 1.5540504, 1.5706767, 1.7359446, 1.7005606, 1.7649467, 1.7848988, 1.8240122, 1.7199402, 1.6881529, 1.6666327, 1.7413337, 1.5712025, 1.5241003, 1.5363718, 1.6382263, 1.4797858, 1.5698498, 1.4940414, 1.540779, 1.4778961, 1.6258498, 1.5609081, 1.554314, 1.530354, 1.6943252, 1.6534548, 1.6620667, 1.5589293, 1.6061513, 1.5916924, 1.5593711, 1.4933684, 1.6162885, 1.4958597, 1.5102885], [7.11506710018169, 6.852796732654634, 2.0978095710741904, 1.9048407927139628, 1.8781066588967685, 1.949150130109482, 1.939244069859372, 2.1888606608077272, 2.089174651942331, 2.1005985360718773, 2.003326629631687, 2.144816395297591, 1.9365753305381639, 2.0284646524231995, 2.0478024310838507, 2.0707827627760356, 1.9854774716630677, 1.9459252062829304, 1.924913377175268, 1.9606871426103425, 1.8559396888988489, 1.932918237925496, 2.0233825911800585, 2.127662337281077, 2.045977213578853, 2.0783623581332784, 2.1493745736945047, 2.3343434077605685, 2.2828708273076606, 2.35699089807267, 2.497061050988642, 2.5341479819488213, 2.407923921238716, 2.292682168393289, 2.253988228138441, 2.3875255563376756, 2.1519013935102502, 2.0468599741143976, 2.0896351933026174, 2.1677795877497448, 1.95213701818274, 2.0565804584103398, 2.024701640436952, 2.1089931566282023, 2.0024834949132297, 2.200708673950857, 2.158883076571231, 2.072845636681203, 2.04788183245392, 2.283114885986048, 2.240618645354428, 2.2326525471376497, 2.0891463497570304, 2.1398164656181993, 2.1483235276942754, 2.05153550582756, 1.945633275804525, 2.114785609099616, 1.991647026199267, 1.9912389554030547], [1.8978608, 1.502003, 0.4191299, 0.3193812, 0.39583936, 0.39515865, 0.3543989, 0.3962462, 0.52291363, 0.5645484, 0.49047968, 0.5657597, 0.5168333, 0.50724834, 0.4614, 0.41457614, 0.37489757, 0.29444715, 0.31642172, 0.37180907, 0.36606944, 0.347634, 0.3687949, 0.41952172, 0.33986297, 0.3358189, 0.41440728, 0.3633031, 0.42138708, 0.3347265, 0.40707755, 0.43066597, 0.46781528, 0.45122507, 0.45813337, 0.48213407, 0.5477787, 0.45403373, 0.5047866, 0.45057875, 0.4160964, 0.31129155, 0.44600573, 0.44064263, 0.50233805, 0.42841464, 0.4992694, 0.44521222, 0.42923903, 0.35602054, 0.5024888, 0.52999663, 0.46145356, 0.45099008, 0.46460155, 0.39871457, 0.39855677, 0.47613958, 0.46556634, 0.5192168]]</t>
+          <t>[[5.0775547, 4.735642, 1.5464158, 1.4658985, 1.4326645, 1.4853686, 1.4299052, 1.5780861, 1.5196892, 1.5860902, 1.475937, 1.5852998, 1.4339463, 1.5466921, 1.5158331, 1.5235857, 1.4642614, 1.4272634, 1.4064485, 1.435182, 1.3533155, 1.435173, 1.5091815, 1.5967917, 1.5119509, 1.5723678, 1.5771265, 1.7097154, 1.6627859, 1.7470672, 1.7726057, 1.8565624, 1.7333152, 1.7004431, 1.6876451, 1.7260419, 1.5628263, 1.5342498, 1.5118974, 1.6133951, 1.4375, 1.5475247, 1.5048462, 1.55849, 1.4525034, 1.6173358, 1.5237721, 1.5671021, 1.540657, 1.6958134, 1.6553084, 1.6604663, 1.5449692, 1.5952022, 1.5507343, 1.5253904, 1.4655825, 1.6019533, 1.4859673, 1.4669821], [7.11506710018169, 6.852796732654634, 2.0978095710741904, 1.9049625739478688, 1.8695237615095008, 1.927812476155823, 1.913737179883278, 2.115646758876232, 2.031491896090914, 2.0987833358725427, 2.0072040749248132, 2.1313921212608333, 1.928947399468366, 2.0132974596595945, 2.0370831583883495, 2.0489727656507934, 1.9399862641900256, 1.9085905370946785, 1.9197981242504032, 1.9509601038965019, 1.8033852771157626, 1.8900365623086246, 1.989969073012141, 2.122517538189179, 2.0066759031765455, 2.0748479718506423, 2.1521588642446963, 2.299973661852423, 2.2021174731054756, 2.33970659519503, 2.516841996845444, 2.6573798076906088, 2.439156776184875, 2.334234529121823, 2.290835478351357, 2.400141505202374, 2.1406176490379027, 2.054241407580939, 2.0703604062853556, 2.1515509223487976, 1.8908626942927964, 2.017128553644688, 2.049713961486718, 2.1255892890189396, 1.9776602851541394, 2.1838638602642924, 2.1167231539700646, 2.102503115802502, 2.0741247238428437, 2.2910140639980296, 2.25229411260693, 2.2343390401867587, 2.0768799458070886, 2.1122801942855833, 2.092936571307433, 1.9957939863474266, 1.906518198126041, 2.0875137602758023, 1.9758725978961966, 1.9485281598153787], [1.8978608, 1.502003, 0.4191299, 0.31939697, 0.39503866, 0.38526428, 0.36002788, 0.38987455, 0.5219229, 0.57096124, 0.47949928, 0.5671472, 0.52242357, 0.52315694, 0.4714304, 0.41130793, 0.38828793, 0.301527, 0.31444454, 0.36062026, 0.34075993, 0.3251458, 0.36270848, 0.42516083, 0.3605872, 0.34594092, 0.41723025, 0.356134, 0.41833454, 0.32694173, 0.39713663, 0.42612892, 0.463483, 0.44256824, 0.4596224, 0.45001796, 0.5103738, 0.4642988, 0.48810172, 0.48081398, 0.4073109, 0.32283825, 0.4805323, 0.4403206, 0.478487, 0.4164802, 0.48932016, 0.46286377, 0.4379972, 0.37795472, 0.4966162, 0.52564347, 0.43966916, 0.43219358, 0.41880235, 0.35939366, 0.38707203, 0.49395335, 0.4721073, 0.5012211]]</t>
         </is>
       </c>
       <c r="G274" t="inlineStr">
         <is>
-          <t>[[10.72892992574343, 2.233470830531607, 1.0806321528123837, 1.2178705740433247, 1.3128293016625283, 1.3124714148381493, 1.2644807547243055, 1.417037018410418, 1.4143046963655137, 1.3873607587056118, 1.2857513775054663, 1.3587136506448614, 1.2866557872494144, 1.3096141522858753, 1.2713161805764073, 1.3207103370435533, 1.3315677190118, 1.2646064801169195, 1.217197859053145, 1.2614256553373502, 1.2604677546038037, 1.290390517651498, 1.2722574365758241, 1.3065466148148075, 1.3264082702036448, 1.3258506221532822, 1.3184827524010296, 1.456783294644836, 1.4939426222046266, 1.5041172014603066, 1.4904476636024104, 1.4736758780823902, 1.5264100836190526, 1.4171409013393372, 1.4214163692128996, 1.4623253030081307, 1.3890253116471563, 1.3184861163767942, 1.3250501911960086, 1.3806283283567147, 1.3206254920897444, 1.3257092108978679, 1.2761562845968948, 1.318947277562585, 1.325352816183026, 1.4040706572512454, 1.3414024027509204, 1.3013343148020577, 1.3769403881773956, 1.4478037956452277, 1.402738665515969, 1.392446409747427, 1.4094747858188934, 1.3985360694375644, 1.3619192356536027, 1.3094953135650016, 1.363826166602896, 1.3708254066303798, 1.2812553987286146, 1.322054308179285], [18.11934265972583, 2.9524229714291432, 1.4252569049769725, 1.5769170386772016, 1.7050782847927202, 1.7061219715094265, 1.6724404624814693, 1.8519565291907936, 1.8567512065238625, 1.8024948572312387, 1.703529117006659, 1.8104358063847412, 1.7091067243309637, 1.7157875411321695, 1.6862524559998933, 1.7513441094220283, 1.7741400006199353, 1.6885221555616818, 1.6200978904108925, 1.6881488837070404, 1.6582075627909516, 1.6745583578937615, 1.6682789968358223, 1.7435217601328339, 1.751863141673439, 1.7552196933693178, 1.7745898277950642, 1.9235895032561725, 1.9562203640805518, 1.9746177842339645, 2.0433306113398513, 2.0290669996783155, 2.098604983212086, 1.9049707131356943, 1.87873335787414, 1.9704614647369258, 1.8536996620483441, 1.7623552405970113, 1.7595306535599433, 1.7847370460021796, 1.7235193295491271, 1.721141615354013, 1.6918714734432627, 1.7761453818752462, 1.7792773023551516, 1.8859315644238426, 1.8003451465007378, 1.7177430618179592, 1.8354053167148279, 1.9381487244938083, 1.8682431443517942, 1.8371791139217932, 1.8605460607345863, 1.8468074029539125, 1.8161453721044096, 1.708830473882624, 1.7600613349359877, 1.7887959221982381, 1.6782214791110965, 1.7231413160848226], [3.4154331818759185, 0.6173745337336952, 0.2786447861894967, 0.2742831026840727, 0.35617066338987835, 0.3469163627776085, 0.30151763655438474, 0.34095273078808197, 0.46979358962671003, 0.45335222616561316, 0.4140191616959314, 0.4676888904923821, 0.446609585880201, 0.4191459874714017, 0.37715315761641993, 0.3414158210711265, 0.31989544419099114, 0.2532814747030526, 0.28279935711062637, 0.3389457535484864, 0.32656242526639834, 0.30779888936446986, 0.2868047474644955, 0.32597724485804347, 0.3007578902727602, 0.29305847130430845, 0.3340837566130772, 0.31695740419276247, 0.36565819516951836, 0.30317423794068865, 0.34330286255434767, 0.36408387271774273, 0.41730353795104896, 0.37633384733517217, 0.3938021152734924, 0.4055512374363482, 0.4659516370692726, 0.402466932014951, 0.41805582918814926, 0.3669885808777117, 0.3726085524498376, 0.26007410480542464, 0.36500399050209986, 0.39686626238253464, 0.43152315997718543, 0.36835277857746684, 0.4146884023121094, 0.3492898143952761, 0.3776977855690062, 0.3128426552378056, 0.4100308698159468, 0.4629401701807064, 0.41918078296058964, 0.3967213001931347, 0.3759534963378892, 0.30645722732674635, 0.3508747468798046, 0.414546588735708, 0.400555717505583, 0.4391385840275625]]</t>
+          <t>[[10.72892992574343, 2.233470830531607, 1.0806321528123837, 1.206037515951591, 1.282367593750087, 1.2879850258381602, 1.1939383047681817, 1.3409261283500074, 1.3838689394050647, 1.3643966007889843, 1.2626540560382262, 1.3270696275023737, 1.2966421075559378, 1.3119350278348467, 1.2662417324767565, 1.274234576940016, 1.3150669980233658, 1.2387533853910766, 1.2240721627256317, 1.2199293010342198, 1.2376847312387584, 1.2378569034451579, 1.2721597097747002, 1.3108522348437484, 1.3542794525706556, 1.359653298264898, 1.3218743033449674, 1.3924439176776506, 1.4583127168570842, 1.4516417891672013, 1.5032528189607834, 1.5038987356375282, 1.5431467597023032, 1.4245864325046127, 1.3929420628944242, 1.4460690283805209, 1.388101088676097, 1.3112855364861022, 1.296049135619417, 1.315174715289112, 1.2855894834904924, 1.3187262995291948, 1.289372339640685, 1.291149827619152, 1.3092802310117442, 1.3739046140892444, 1.3200273332645445, 1.3065017977038562, 1.3890098551489123, 1.4393975262696121, 1.414633287887534, 1.387259600769419, 1.373396670787771, 1.3628022596276066, 1.3351477969553498, 1.2949540501758696, 1.3355161336867132, 1.357985630987107, 1.2611227559856135, 1.2398217038867556], [18.11934265972583, 2.9524229714291432, 1.4252569049769725, 1.5625052775536048, 1.6646706185512834, 1.6802016256008316, 1.5905488504233956, 1.7668423358495102, 1.8250988974200375, 1.779393597267023, 1.6819488776900844, 1.7790292403666523, 1.721205436783664, 1.7039253220596688, 1.6700280749588747, 1.6994938233486319, 1.7294740351886675, 1.6595093471128894, 1.6343455895294954, 1.6423635127707128, 1.6305828847929653, 1.6206243327079246, 1.6400157698411046, 1.7309824365803823, 1.764450762073066, 1.7947923170553237, 1.7656875085426078, 1.840357256804316, 1.9060478768098204, 1.9230618722582056, 2.125510352752408, 2.0815545139250924, 2.1438022467209836, 1.922664082976434, 1.8570833196004926, 1.9538749301031992, 1.8487333037326483, 1.7533709882187125, 1.7561240209872762, 1.7249033398533187, 1.6734009956502662, 1.710192878698997, 1.7132958368862192, 1.7378505564493654, 1.7522134455694895, 1.8543879131484355, 1.7960946713218005, 1.734039142883523, 1.8596532074736447, 1.9501932828512456, 1.8942262100738323, 1.8372501998817206, 1.8089187561039686, 1.7913973229914446, 1.7842033487164022, 1.6743936809363802, 1.7290867800162695, 1.7702407768918769, 1.6656113021653198, 1.6377124970303283], [3.4154331818759185, 0.6173745337336952, 0.2786447861894967, 0.26856504380460805, 0.35240213101222906, 0.3477531294907926, 0.3042984060456344, 0.31478269894773375, 0.46190787717994747, 0.4578135780520993, 0.3853628127956247, 0.4758233518217964, 0.4586673593357906, 0.4471632956651956, 0.38161472605730795, 0.33400595621681894, 0.3413082549906367, 0.2593099075183452, 0.2697790289134058, 0.3011794413213915, 0.3052408989587239, 0.283016689339218, 0.2991833588563208, 0.34538480201247196, 0.3141963197117188, 0.2992293495712261, 0.347409781175819, 0.2959869791746309, 0.3632922121695596, 0.2841166906003477, 0.3285744458642791, 0.34848943995173987, 0.41011001764943683, 0.36738510376496575, 0.3676254781883365, 0.35485592151012657, 0.42996750943535716, 0.39900203741443313, 0.41624236317420626, 0.37148210820491695, 0.37751940542848306, 0.27842648952823285, 0.40871662105620743, 0.359674143137866, 0.4266283843326274, 0.35678738140269933, 0.4133303921535231, 0.3725921602653244, 0.3814962490094087, 0.3367564626353427, 0.39974309012561393, 0.42816168019835776, 0.3939943407183224, 0.37057454070199863, 0.3579549784914582, 0.29777893014800105, 0.34826851554900917, 0.40418683823564827, 0.39350115057254176, 0.3986283114535907]]</t>
         </is>
       </c>
       <c r="H274" t="n">
-        <v>326.2058348655701</v>
+        <v>324.3645911216736</v>
       </c>
     </row>
     <row r="275">
@@ -9788,7 +9788,7 @@
         </is>
       </c>
       <c r="H275" t="n">
-        <v>326.122150182724</v>
+        <v>323.1751186847687</v>
       </c>
     </row>
     <row r="276">
@@ -9822,7 +9822,7 @@
         </is>
       </c>
       <c r="H276" t="n">
-        <v>327.1627490520477</v>
+        <v>323.6571695804596</v>
       </c>
     </row>
     <row r="277">
@@ -9856,7 +9856,7 @@
         </is>
       </c>
       <c r="H277" t="n">
-        <v>69.30022549629211</v>
+        <v>70.52100205421448</v>
       </c>
     </row>
     <row r="278">
@@ -9890,7 +9890,7 @@
         </is>
       </c>
       <c r="H278" t="n">
-        <v>69.40014624595642</v>
+        <v>70.61803603172302</v>
       </c>
     </row>
     <row r="279">
@@ -9924,7 +9924,7 @@
         </is>
       </c>
       <c r="H279" t="n">
-        <v>69.27498888969421</v>
+        <v>70.50144362449646</v>
       </c>
     </row>
     <row r="280">
@@ -9935,7 +9935,7 @@
         <v>100</v>
       </c>
       <c r="C280" t="n">
-        <v>7.000000000000001</v>
+        <v>7</v>
       </c>
       <c r="D280" t="inlineStr">
         <is>
@@ -9958,7 +9958,7 @@
         </is>
       </c>
       <c r="H280" t="n">
-        <v>73.67093062400818</v>
+        <v>74.76143527030945</v>
       </c>
     </row>
     <row r="281">
@@ -9969,7 +9969,7 @@
         <v>100</v>
       </c>
       <c r="C281" t="n">
-        <v>7.000000000000001</v>
+        <v>7</v>
       </c>
       <c r="D281" t="inlineStr">
         <is>
@@ -9992,7 +9992,7 @@
         </is>
       </c>
       <c r="H281" t="n">
-        <v>73.80939555168152</v>
+        <v>75.45349884033203</v>
       </c>
     </row>
     <row r="282">
@@ -10003,7 +10003,7 @@
         <v>100</v>
       </c>
       <c r="C282" t="n">
-        <v>7.000000000000001</v>
+        <v>7</v>
       </c>
       <c r="D282" t="inlineStr">
         <is>
@@ -10026,7 +10026,7 @@
         </is>
       </c>
       <c r="H282" t="n">
-        <v>73.72736191749573</v>
+        <v>75.21530938148499</v>
       </c>
     </row>
     <row r="283">
@@ -10060,7 +10060,7 @@
         </is>
       </c>
       <c r="H283" t="n">
-        <v>85.84535360336304</v>
+        <v>87.02538418769836</v>
       </c>
     </row>
     <row r="284">
@@ -10094,7 +10094,7 @@
         </is>
       </c>
       <c r="H284" t="n">
-        <v>86.31917357444763</v>
+        <v>87.27173924446106</v>
       </c>
     </row>
     <row r="285">
@@ -10128,7 +10128,7 @@
         </is>
       </c>
       <c r="H285" t="n">
-        <v>86.43506717681885</v>
+        <v>87.51914429664612</v>
       </c>
     </row>
     <row r="286">
@@ -10153,16 +10153,16 @@
       </c>
       <c r="F286" t="inlineStr">
         <is>
-          <t>[[5.07496, 23.785656, 3.1200614, 1.5325747, 1.3946631, 1.4424964, 1.3832153, 1.5580338, 1.5115191, 1.5517043, 1.4515467, 1.5569295, 1.4391974, 1.5586469, 1.4970226, 1.4919174, 1.4250815, 1.3823295, 1.3419662, 1.3734093, 1.3516738, 1.4477297, 1.4994748, 1.5792829, 1.4917657, 1.5369813, 1.5312176, 1.6503035, 1.6565793, 1.7486496, 1.7330046, 1.7963504, 1.750895, 1.7327056, 1.6703856, 1.6957855, 1.5706663, 1.5194094, 1.5178999, 1.5974982, 1.4807901, 1.5365582, 1.5090652, 1.5574632, 1.4726417, 1.647423, 1.5319331, 1.5301378, 1.5081962, 1.6714302, 1.6032499, 1.6157001, 1.526834, 1.5809733, 1.5707525, 1.5348673, 1.48728, 1.6203514, 1.5097749, 1.5029514], [7.1122123673510185, 32.944318554190794, 4.397077604287862, 2.0115406142687706, 1.8235034397888794, 1.877610296979218, 1.8516293928078418, 2.1048339566233802, 2.024210896213597, 2.071609608955733, 1.9680519077348282, 2.123814532650603, 1.9670227587788802, 2.0457210636863854, 2.0089718332627915, 2.0275134418009046, 1.891961563191718, 1.8425054714168225, 1.8237049759764448, 1.8553616462714757, 1.811515409138207, 1.8948847175498449, 1.9658187358336325, 2.0753374262000555, 1.9646556604959677, 2.028602165434482, 2.119798015113216, 2.2302526045254774, 2.255436581050901, 2.356861215337169, 2.475987990496572, 2.518304570570496, 2.441094023003679, 2.3348154288295335, 2.3020253469031187, 2.3436661768864697, 2.149977697212402, 2.048145511397604, 2.0706017634005955, 2.143797034812519, 1.9513198445128364, 2.0238963899215423, 2.052463270409338, 2.133831074386188, 1.9786326306946815, 2.2256091837654437, 2.1070694367962135, 2.0571617632708596, 2.020277228641259, 2.266662254983685, 2.1796663891716817, 2.170388241154123, 2.062708063901619, 2.1318472330280804, 2.1616182811952283, 2.003571539991282, 1.9242127629449084, 2.0882223238696285, 1.9865536482024035, 1.972368940826998], [1.8963157, 7.487386, 0.9038972, 0.37569192, 0.37580326, 0.36987635, 0.35918167, 0.38790506, 0.5161256, 0.559044, 0.48647973, 0.5720197, 0.5398197, 0.52763814, 0.45971787, 0.40202028, 0.37423745, 0.2971931, 0.2982335, 0.3463932, 0.34823558, 0.3384803, 0.3699734, 0.4219218, 0.34313208, 0.3293351, 0.397039, 0.3469157, 0.41221863, 0.32260522, 0.4028741, 0.40288693, 0.44579, 0.4265985, 0.42068955, 0.45005655, 0.50867873, 0.43860087, 0.4791831, 0.45615578, 0.41662607, 0.32328203, 0.45880628, 0.46505862, 0.49908596, 0.44023022, 0.48282892, 0.39565518, 0.41436777, 0.3458621, 0.46636122, 0.49394652, 0.44874525, 0.44183043, 0.42223433, 0.36793664, 0.3925954, 0.48632255, 0.46466586, 0.5146271]]</t>
+          <t>[[5.07496, 23.785656, 3.1200614, 1.5327272, 1.3960662, 1.4434142, 1.3950254, 1.5792416, 1.5209914, 1.5334991, 1.4669282, 1.5384936, 1.3908681, 1.4899681, 1.4579061, 1.4997605, 1.4193197, 1.3952239, 1.3742459, 1.4058717, 1.3540661, 1.4577698, 1.5235898, 1.5840675, 1.4722937, 1.5429237, 1.5572499, 1.7119126, 1.6699452, 1.7566637, 1.7865016, 1.8093305, 1.7315634, 1.709789, 1.6887107, 1.747851, 1.5376377, 1.5174272, 1.5242752, 1.6090187, 1.4731954, 1.5463436, 1.4604082, 1.5385861, 1.4436581, 1.5915766, 1.5162561, 1.5606127, 1.5119894, 1.6303418, 1.6137815, 1.6275265, 1.5160064, 1.55926, 1.5649005, 1.5530924, 1.4602228, 1.5929354, 1.4917539, 1.4863883], [7.1122123673510185, 32.944318554190794, 4.397077604287862, 2.0116386323548814, 1.8203379747957578, 1.8710337969705753, 1.855211934838145, 2.1272489203682214, 2.041589099682137, 2.053348351440169, 1.9997148906622058, 2.097018636909005, 1.874041312223411, 1.9427525478646264, 1.9720128587028853, 2.0187535808519663, 1.8905456147985193, 1.8732325170524093, 1.8841644118828536, 1.9150738593815635, 1.8113695763079043, 1.9173944238795113, 2.010361178197335, 2.1094980839740725, 1.9474528843440893, 2.0483265163638245, 2.1438259500556662, 2.2859644838045536, 2.2595476393213736, 2.368576699713982, 2.5515663609472568, 2.5349465211422646, 2.419087534771119, 2.3200254937119524, 2.3123442107640364, 2.383151771280989, 2.0975442923960466, 2.043344962671406, 2.080830125583452, 2.16990759129806, 1.9425620739026503, 2.0140938080928237, 1.9959135030149313, 2.1095735809665332, 1.9379826836614487, 2.1563068327117354, 2.0751678536786278, 2.068923080902517, 2.0250604078913623, 2.21129527078524, 2.2062589391251715, 2.2235297714034834, 2.0696358204649936, 2.1129327229279857, 2.144353362385369, 2.0665345467615546, 1.909545114184548, 2.081369262577438, 1.9864299676793922, 1.964758444540154], [1.8963157, 7.487386, 0.9038972, 0.37567428, 0.38513383, 0.3745054, 0.359223, 0.3768468, 0.53136146, 0.5737165, 0.48996356, 0.5760853, 0.48850933, 0.47596335, 0.42914686, 0.38872328, 0.36192453, 0.3014931, 0.31343538, 0.35463083, 0.3390176, 0.3321734, 0.37169093, 0.4162415, 0.34592453, 0.3328513, 0.39691502, 0.36009485, 0.41967717, 0.32203668, 0.38633803, 0.40917668, 0.46440887, 0.4424889, 0.44867602, 0.45100242, 0.48869437, 0.44919196, 0.4772586, 0.47079426, 0.41295066, 0.31446245, 0.455327, 0.43618956, 0.48623142, 0.4055539, 0.47212258, 0.40521863, 0.42133218, 0.35204768, 0.48074833, 0.5051396, 0.43867034, 0.44784793, 0.45621327, 0.3946109, 0.3986815, 0.4966751, 0.48179054, 0.54592603]]</t>
         </is>
       </c>
       <c r="G286" t="inlineStr">
         <is>
-          <t>[[49.50637976546157, 7.4289623814331325, 1.248043804864204, 1.2159188500469538, 1.2373162843303345, 1.2106899481619895, 1.1696032466029174, 1.3274555600793148, 1.356396328294928, 1.3072737033966746, 1.2397825108836409, 1.3392768064803016, 1.293114897110236, 1.302833305909272, 1.2333266766747988, 1.25270979984487, 1.2872394651159722, 1.1947520919894878, 1.1396190734302376, 1.1882173570804, 1.2277466319497108, 1.2535985917051728, 1.2377234610450587, 1.2953588686617445, 1.2937500109284203, 1.274459261067056, 1.2623290743775428, 1.3734876307912596, 1.435621149247447, 1.4298073716785453, 1.439579535053079, 1.4928905134446908, 1.5492534556757869, 1.4498856939001632, 1.3847072890852248, 1.4157541741416486, 1.3916541514333653, 1.304768920179899, 1.2669446605226236, 1.3498523527466209, 1.3190814720859725, 1.2920475590849214, 1.2552329790822496, 1.3189540935448134, 1.33118973228329, 1.366649811798346, 1.2810723404758477, 1.2897305155499668, 1.355577003092549, 1.4274952781804733, 1.3455364074461564, 1.348103060972504, 1.3595163273005055, 1.3826059474329324, 1.3235742773524737, 1.2996746289630874, 1.3662066572287097, 1.37849851432476, 1.2898308557645763, 1.2505938321365753], [85.00698957986732, 12.915019011590548, 1.6604892552618813, 1.5844233991297834, 1.6123135032901617, 1.5826093917499588, 1.5512811735964334, 1.761715978938661, 1.8060497542568803, 1.7209188673831757, 1.6587293004785086, 1.8215115599867284, 1.723624909889908, 1.7091086970287273, 1.6339478489630737, 1.6621351510909566, 1.685713415034998, 1.580116734640723, 1.5124849492875971, 1.5907924254520756, 1.6304173648421978, 1.6244738280288267, 1.5964485327059956, 1.7004647858624469, 1.7017412045844396, 1.6855710601560132, 1.6900225222652676, 1.8332538267353535, 1.889458325482511, 1.8913756719082246, 1.992314080978316, 2.0555050950520135, 2.137894752651945, 1.964090284652161, 1.8256205749446959, 1.906727149897419, 1.8661359846970182, 1.751007821700455, 1.705588995942487, 1.7742402352111775, 1.720777023514818, 1.6846449440810651, 1.6584030028722958, 1.7647153017017305, 1.7780418624684606, 1.8352514943007558, 1.7446794454613868, 1.7098793381744908, 1.8176589432793404, 1.9343937715488433, 1.8047583773747764, 1.7853928987483896, 1.818410481084833, 1.8500787032902792, 1.7808953908545202, 1.6902985307128602, 1.7506775199352036, 1.7668590851110442, 1.679694823256606, 1.6392231455546544], [17.06276004506576, 1.8307345357024254, 0.31288489059210256, 0.318641815118027, 0.3382742800557853, 0.31257908049156874, 0.31066223884636357, 0.3276750264372029, 0.45913550066748904, 0.44087052558007506, 0.40859402645412995, 0.48633607429410336, 0.4736395729746161, 0.42390337083531565, 0.3637465430541844, 0.33860173170644503, 0.3249825854735718, 0.24544884674810336, 0.24332694543341943, 0.30475434698733944, 0.3102494365447539, 0.3056161488541514, 0.31187944235678194, 0.33972980086568505, 0.30181947153924976, 0.27617677223884224, 0.33290450350846523, 0.2872577406213298, 0.35186835654397536, 0.2711236673253459, 0.3460475834607795, 0.33300385434626445, 0.37703612692453264, 0.3770196403899757, 0.3556419100808752, 0.3583097032586817, 0.44139066562011153, 0.3752079290892664, 0.39267926112484264, 0.37321360088646593, 0.3720286401402657, 0.27366984841747993, 0.37052552508945197, 0.3935571574788128, 0.45093792172287894, 0.36637872776797115, 0.38356590672756313, 0.3232870611932729, 0.36259530963335374, 0.2934966787554459, 0.3735527577610176, 0.412778858862162, 0.3913846030355513, 0.3762633226382161, 0.3336311502176585, 0.30791477004382095, 0.3432921275896397, 0.41683541142733305, 0.383913073908817, 0.40481051637023163]]</t>
+          <t>[[49.50637976546157, 7.4289623814331325, 1.248043804864204, 1.197523781038182, 1.2465538168623986, 1.2357473097096299, 1.2128146236671955, 1.3316952824469488, 1.3527786402298814, 1.2850678724300826, 1.2481249647284054, 1.2752278165809696, 1.2215265904022239, 1.243435063380761, 1.2217308857155451, 1.2182312788268508, 1.255927851442089, 1.2040575938797347, 1.158477254742777, 1.187481475524071, 1.2121512644214323, 1.256986365932194, 1.2641109050818726, 1.292152964094189, 1.3072343337925276, 1.300669816499781, 1.2916217660452718, 1.3658514496214555, 1.4510287891729976, 1.4605555066705977, 1.4427802547812052, 1.4636360724424826, 1.5210174446063065, 1.4371425896465564, 1.4036942278857543, 1.393501854116929, 1.3664640711078195, 1.316110292169903, 1.2862180741153917, 1.3456053565209096, 1.2847917611864554, 1.2768115131143924, 1.240993743164059, 1.2679497799896438, 1.2854240181917695, 1.3600365141029003, 1.3012631394386514, 1.275461158647278, 1.3348002612340353, 1.405344764700365, 1.3676504932608837, 1.3461152433073975, 1.342401358477888, 1.3291375890172685, 1.3285788742351257, 1.2870460887380806, 1.329069035366059, 1.3857955539721145, 1.253967401808501, 1.247849199930363], [85.00698957986732, 12.915019011590548, 1.6604892552618813, 1.5523210867879804, 1.6164405515241898, 1.5922519057196962, 1.5989849457296073, 1.7730567458540527, 1.8032639526251824, 1.7044933017767445, 1.6700957222873172, 1.7134052905677764, 1.6262671191398002, 1.636505422727259, 1.6162565844209869, 1.624671398941718, 1.6589560900414473, 1.6146224826630822, 1.5520087438396635, 1.5799846685923902, 1.6072436535563877, 1.6422137775758303, 1.6291890990705307, 1.6988869534769149, 1.7155871543612768, 1.7110160835907453, 1.7081687282353812, 1.8084557278919398, 1.8904135516254166, 1.9446370538645044, 2.0025602411951624, 2.0094621665013563, 2.110145015268176, 1.9530063675308778, 1.8475696275512892, 1.8421156320046381, 1.8173311457043515, 1.7603361188176663, 1.7389647238662842, 1.7699983363054133, 1.6709615336514378, 1.6520737399495293, 1.637376985402744, 1.6843431655897916, 1.71048028094278, 1.8062522573843276, 1.7509767539907044, 1.6859707035764335, 1.780173663231618, 1.8981389956394434, 1.8533788329928762, 1.799773264598153, 1.7951111877337542, 1.785382345515148, 1.7850105959019023, 1.6918657536854367, 1.7217699536245767, 1.8021899679762705, 1.6456598723680025, 1.6529338548041843], [17.06276004506576, 1.8307345357024254, 0.31288489059210256, 0.31941665448607703, 0.34441670123989077, 0.32425285295697526, 0.30078250147696955, 0.31751909793577876, 0.4637030054035813, 0.4588712553322274, 0.39822408500145573, 0.44831707428658935, 0.4189921797507992, 0.3868447291003113, 0.3482967059631374, 0.3105952789368031, 0.31420422147649857, 0.2504841974073969, 0.2547943488319293, 0.29845515384551763, 0.3022202054906355, 0.3035315044661245, 0.29910393700539606, 0.33774527165668494, 0.2993269705517732, 0.282261322374904, 0.33941796394868534, 0.292724327453607, 0.35566542178971267, 0.27904991129887224, 0.31563785151290524, 0.31228744313405893, 0.39137143152769616, 0.37293685457807785, 0.3724480358842834, 0.34753452063681445, 0.43732222728579717, 0.385850291636273, 0.3894038476216608, 0.37805340997319153, 0.35943570306694006, 0.26847381385070346, 0.367332289153626, 0.3660027813605205, 0.4308246410062715, 0.34621725115605634, 0.3769282144308968, 0.329574122023466, 0.3564769266670795, 0.2925330365009974, 0.3789739997802766, 0.4032284985387006, 0.38789269752405314, 0.4017305552846504, 0.37023622645006066, 0.31096114147999826, 0.3496043994618475, 0.43554638782652727, 0.39552545785085325, 0.43225409253992475]]</t>
         </is>
       </c>
       <c r="H286" t="n">
-        <v>326.74573969841</v>
+        <v>324.6511497497559</v>
       </c>
     </row>
     <row r="287">
@@ -10196,7 +10196,7 @@
         </is>
       </c>
       <c r="H287" t="n">
-        <v>327.5904669761658</v>
+        <v>325.9997005462646</v>
       </c>
     </row>
     <row r="288">
@@ -10230,7 +10230,7 @@
         </is>
       </c>
       <c r="H288" t="n">
-        <v>327.6160182952881</v>
+        <v>328.2580227851868</v>
       </c>
     </row>
   </sheetData>

</xml_diff>